<commit_message>
Rw Usage Updates S.1.0.1.7 _12:45PM
Boat Enabled -
InCapacity - [17,8,Cnt] ,
NodeW - [-3] ,
BirdW - [7][CityW-MundiaSahi] ,
FuelW_Day - ['22][CityW-CM Nagar] ,
OnHost - [8+1]
VillageW=[0],
CityW=[2] ,
[X-MarketShieldMatrix-X] = [5,2,2,3] = [Lx -2 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.1.0.xlsx
+++ b/Usage_S_1.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58632E67-4136-4923-BEFB-75EC93D36848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56311D26-0A2E-4663-B60F-89522BBB69FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="294">
   <si>
     <t>UnSettled</t>
   </si>
@@ -2591,6 +2591,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2633,42 +2666,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2678,13 +2675,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2698,14 +2695,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2997,7 +2997,7 @@
   <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,15 +3131,15 @@
       </c>
       <c r="AB2" s="15">
         <f>SUM(AB3:AB25)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC2" s="36">
         <f>SUM(AC3:AC25)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD2" s="36">
         <f>SUM(AD3:AD25)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>92</v>
@@ -3306,10 +3306,10 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>4100</v>
+        <v>4120</v>
       </c>
       <c r="C6">
-        <v>4511</v>
+        <v>4513</v>
       </c>
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="E7" s="165"/>
       <c r="F7" s="242"/>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>11100</v>
+        <v>11120</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="165"/>
@@ -3655,17 +3655,30 @@
       <c r="Z11" s="169" t="s">
         <v>233</v>
       </c>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="24"/>
+      <c r="AB11" s="15">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="24">
+        <v>1</v>
+      </c>
+      <c r="AD11">
+        <v>2</v>
+      </c>
       <c r="AE11" s="290"/>
-      <c r="AF11" s="25"/>
-      <c r="AG11" s="25"/>
+      <c r="AF11" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG11" s="25" t="s">
+        <v>20</v>
+      </c>
       <c r="AH11" s="24" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="165"/>
+      <c r="E12" s="165">
+        <v>15</v>
+      </c>
       <c r="F12" s="205"/>
       <c r="G12" s="164"/>
       <c r="H12" s="28" t="s">
@@ -3675,6 +3688,9 @@
         <v>17</v>
       </c>
       <c r="J12" s="213"/>
+      <c r="K12" s="169" t="s">
+        <v>222</v>
+      </c>
       <c r="L12" s="224" t="s">
         <v>123</v>
       </c>
@@ -3691,11 +3707,11 @@
         <v>181</v>
       </c>
       <c r="Q12" s="154">
-        <v>0.83333333333333337</v>
+        <v>0.53125</v>
       </c>
       <c r="R12" s="24"/>
       <c r="S12" s="154">
-        <v>0.83333333333333337</v>
+        <v>0.53125</v>
       </c>
       <c r="U12" s="245">
         <v>45294</v>
@@ -3721,9 +3737,11 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>11100</v>
-      </c>
-      <c r="E13" s="36"/>
+        <v>11120</v>
+      </c>
+      <c r="E13" s="36">
+        <v>5</v>
+      </c>
       <c r="F13" s="206"/>
       <c r="G13" s="246"/>
       <c r="H13" s="9" t="s">
@@ -3754,11 +3772,11 @@
         <v>90</v>
       </c>
       <c r="Q13" s="154">
-        <v>0.98263888888888884</v>
+        <v>0.53125</v>
       </c>
       <c r="R13"/>
       <c r="S13" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.53125</v>
       </c>
       <c r="T13" s="262">
         <v>1</v>
@@ -3923,7 +3941,7 @@
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="263"/>
@@ -4304,8 +4322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
   <dimension ref="A1:T63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4329,18 +4347,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="309" t="s">
+      <c r="E1" s="295" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="311"/>
+      <c r="F1" s="297"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="309" t="s">
+      <c r="H1" s="295" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="310"/>
-      <c r="J1" s="311"/>
+      <c r="I1" s="296"/>
+      <c r="J1" s="297"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4358,7 +4376,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="312">
+      <c r="B2" s="298">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4385,26 +4403,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="315">
+      <c r="K2" s="301">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="307">
+      <c r="L2" s="318">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="297">
+      <c r="M2" s="308">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
         <f>SUM(E2:J63)</f>
-        <v>11060</v>
+        <v>11080</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="313"/>
+      <c r="B3" s="299"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4419,13 +4437,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="316"/>
+      <c r="K3" s="302"/>
       <c r="L3" s="277"/>
-      <c r="M3" s="298"/>
+      <c r="M3" s="309"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="314"/>
+      <c r="B4" s="300"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4440,9 +4458,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="316"/>
+      <c r="K4" s="302"/>
       <c r="L4" s="277"/>
-      <c r="M4" s="298"/>
+      <c r="M4" s="309"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4524,7 +4542,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="299">
+      <c r="B7" s="310">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4541,22 +4559,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="301">
+      <c r="K7" s="312">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="303">
+      <c r="L7" s="314">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="305">
+      <c r="M7" s="316">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="300"/>
+      <c r="B8" s="311"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4577,9 +4595,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="302"/>
-      <c r="L8" s="304"/>
-      <c r="M8" s="306"/>
+      <c r="K8" s="313"/>
+      <c r="L8" s="315"/>
+      <c r="M8" s="317"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -4659,7 +4677,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="299">
+      <c r="B11" s="310">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -4686,7 +4704,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="300"/>
+      <c r="B12" s="311"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -4743,7 +4761,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="299">
+      <c r="B14" s="310">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -4766,7 +4784,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="300"/>
+      <c r="B15" s="311"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -4790,7 +4808,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="312">
+      <c r="B16" s="298">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -4821,7 +4839,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="313"/>
+      <c r="B17" s="299"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -4839,7 +4857,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="312">
+      <c r="B18" s="298">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4868,7 +4886,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="314"/>
+      <c r="B19" s="300"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4928,7 +4946,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="317">
+      <c r="B21" s="303">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4956,7 +4974,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="318"/>
+      <c r="B22" s="304"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -5096,7 +5114,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="308"/>
+      <c r="B27" s="294"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5427,7 +5445,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="308"/>
+      <c r="B40" s="294"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5482,7 +5500,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="308"/>
+      <c r="B42" s="294"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5602,7 +5620,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="308"/>
+      <c r="B47" s="294"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5643,7 +5661,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="308"/>
+      <c r="B49" s="294"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -5669,7 +5687,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="308"/>
+      <c r="B50" s="294"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -5781,7 +5799,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="308"/>
+      <c r="B54" s="294"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -5862,7 +5880,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="294">
+      <c r="B57" s="305">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -5882,7 +5900,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="295"/>
+      <c r="B58" s="306"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -5911,7 +5929,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="296"/>
+      <c r="B59" s="307"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -5963,7 +5981,7 @@
       <c r="M60" s="18"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="308"/>
+      <c r="B61" s="294"/>
       <c r="C61" s="142"/>
       <c r="D61" s="18">
         <v>240</v>
@@ -6018,7 +6036,9 @@
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
       <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
+      <c r="H63" s="18">
+        <v>20</v>
+      </c>
       <c r="I63" s="18">
         <v>30</v>
       </c>
@@ -6031,6 +6051,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="B60:B62"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:B4"/>
@@ -6047,22 +6083,6 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10498,7 +10518,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="323">
+      <c r="AX32" s="330">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -10536,7 +10556,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="323">
+      <c r="BN32" s="330">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -10685,7 +10705,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="324"/>
+      <c r="AX33" s="331"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10721,7 +10741,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="324"/>
+      <c r="BN33" s="331"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10872,7 +10892,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="325"/>
+      <c r="AX34" s="332"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10910,7 +10930,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="325"/>
+      <c r="BN34" s="332"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -12383,7 +12403,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="323">
+      <c r="C44" s="330">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12421,10 +12441,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="332">
+      <c r="S44" s="323">
         <v>25</v>
       </c>
-      <c r="T44" s="323">
+      <c r="T44" s="330">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12433,7 +12453,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="326" t="s">
+      <c r="W44" s="325" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12462,10 +12482,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="332">
+      <c r="AJ44" s="323">
         <v>50</v>
       </c>
-      <c r="AK44" s="323">
+      <c r="AK44" s="330">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12475,7 +12495,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="326" t="s">
+      <c r="AO44" s="325" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -12505,7 +12525,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="332">
+      <c r="BD44" s="323">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -12516,7 +12536,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="326" t="s">
+      <c r="BI44" s="325" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -12545,7 +12565,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="332">
+      <c r="BW44" s="323">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -12556,7 +12576,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="326" t="s">
+      <c r="CB44" s="325" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -12588,7 +12608,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="324"/>
+      <c r="C45" s="331"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -12622,15 +12642,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="333"/>
-      <c r="T45" s="325"/>
+      <c r="S45" s="324"/>
+      <c r="T45" s="332"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="327"/>
+      <c r="W45" s="326"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12657,8 +12677,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="333"/>
-      <c r="AK45" s="325"/>
+      <c r="AJ45" s="324"/>
+      <c r="AK45" s="332"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -12666,7 +12686,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="327"/>
+      <c r="AO45" s="326"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12694,7 +12714,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="333"/>
+      <c r="BD45" s="324"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -12705,7 +12725,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="327"/>
+      <c r="BI45" s="326"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12732,7 +12752,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="333"/>
+      <c r="BW45" s="324"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -12741,7 +12761,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="327"/>
+      <c r="CB45" s="326"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12771,7 +12791,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="325"/>
+      <c r="C46" s="332"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13376,11 +13396,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="328"/>
+      <c r="AQ49" s="327"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="320"/>
-      <c r="AV49" s="321"/>
+      <c r="AU49" s="319"/>
+      <c r="AV49" s="320"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -13392,11 +13412,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="328"/>
+      <c r="BK49" s="327"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="320"/>
-      <c r="BP49" s="321"/>
+      <c r="BO49" s="319"/>
+      <c r="BP49" s="320"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -13407,11 +13427,11 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="328"/>
+      <c r="CD49" s="327"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="320"/>
-      <c r="CI49" s="321"/>
+      <c r="CH49" s="319"/>
+      <c r="CI49" s="320"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
@@ -13431,11 +13451,11 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="328"/>
+      <c r="AQ50" s="327"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="320"/>
-      <c r="AV50" s="321"/>
+      <c r="AU50" s="319"/>
+      <c r="AV50" s="320"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
@@ -13452,11 +13472,11 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="328"/>
+      <c r="BK50" s="327"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="320"/>
-      <c r="BP50" s="321"/>
+      <c r="BO50" s="319"/>
+      <c r="BP50" s="320"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
@@ -13472,11 +13492,11 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="328"/>
+      <c r="CD50" s="327"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="320"/>
-      <c r="CI50" s="321"/>
+      <c r="CH50" s="319"/>
+      <c r="CI50" s="320"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
@@ -13536,14 +13556,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="329"/>
+      <c r="AQ51" s="328"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="330"/>
-      <c r="AV51" s="331"/>
+      <c r="AU51" s="329"/>
+      <c r="AV51" s="322"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -13555,14 +13575,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="329"/>
+      <c r="BK51" s="328"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="330"/>
-      <c r="BP51" s="331"/>
+      <c r="BO51" s="329"/>
+      <c r="BP51" s="322"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -13573,14 +13593,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="329"/>
+      <c r="CD51" s="328"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="330"/>
-      <c r="CI51" s="331"/>
+      <c r="CH51" s="329"/>
+      <c r="CI51" s="322"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -16960,8 +16980,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="320"/>
-      <c r="O66" s="321"/>
+      <c r="N66" s="319"/>
+      <c r="O66" s="320"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -17104,8 +17124,8 @@
       <c r="J67" s="276"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="320"/>
-      <c r="O67" s="321"/>
+      <c r="N67" s="319"/>
+      <c r="O67" s="320"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
@@ -17124,8 +17144,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="320"/>
-      <c r="AI67" s="321"/>
+      <c r="AH67" s="319"/>
+      <c r="AI67" s="320"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -17196,7 +17216,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="322"/>
+      <c r="J68" s="321"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -17214,8 +17234,8 @@
       <c r="AC68" s="119"/>
       <c r="AD68" s="276"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="320"/>
-      <c r="AI68" s="321"/>
+      <c r="AH68" s="319"/>
+      <c r="AI68" s="320"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
@@ -17234,8 +17254,8 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="320"/>
-      <c r="BB68" s="321"/>
+      <c r="BA68" s="319"/>
+      <c r="BB68" s="320"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
@@ -17254,8 +17274,8 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="320"/>
-      <c r="BW68" s="321"/>
+      <c r="BV68" s="319"/>
+      <c r="BW68" s="320"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
       <c r="BZ68" s="46"/>
@@ -17274,8 +17294,8 @@
       <c r="CJ68" s="119"/>
       <c r="CK68" s="117"/>
       <c r="CN68" s="2"/>
-      <c r="CO68" s="320"/>
-      <c r="CP68" s="321"/>
+      <c r="CO68" s="319"/>
+      <c r="CP68" s="320"/>
       <c r="CQ68" s="1"/>
       <c r="CR68" s="1"/>
       <c r="CS68" s="46"/>
@@ -17321,7 +17341,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="322"/>
+      <c r="AD69" s="321"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -17339,8 +17359,8 @@
       <c r="AV69" s="119"/>
       <c r="AW69" s="276"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="320"/>
-      <c r="BB69" s="321"/>
+      <c r="BA69" s="319"/>
+      <c r="BB69" s="320"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
@@ -17353,8 +17373,8 @@
       <c r="BQ69" s="119"/>
       <c r="BR69" s="276"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="320"/>
-      <c r="BW69" s="321"/>
+      <c r="BV69" s="319"/>
+      <c r="BW69" s="320"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
       <c r="BZ69" s="46"/>
@@ -17367,8 +17387,8 @@
       <c r="CJ69" s="119"/>
       <c r="CK69" s="276"/>
       <c r="CN69" s="2"/>
-      <c r="CO69" s="320"/>
-      <c r="CP69" s="321"/>
+      <c r="CO69" s="319"/>
+      <c r="CP69" s="320"/>
       <c r="CQ69" s="1"/>
       <c r="CR69" s="1"/>
       <c r="CS69" s="46"/>
@@ -17429,7 +17449,7 @@
       <c r="CH70" s="137"/>
       <c r="CI70" s="203"/>
       <c r="CJ70" s="201"/>
-      <c r="CK70" s="322"/>
+      <c r="CK70" s="321"/>
       <c r="CL70" s="50"/>
       <c r="CM70" s="50"/>
       <c r="CN70" s="79"/>
@@ -17537,10 +17557,10 @@
       <c r="DD72" s="137"/>
       <c r="DE72" s="137"/>
       <c r="DF72" s="5"/>
-      <c r="DG72" s="319" t="s">
+      <c r="DG72" s="333" t="s">
         <v>291</v>
       </c>
-      <c r="DH72" s="319"/>
+      <c r="DH72" s="333"/>
       <c r="DI72" s="270"/>
       <c r="DJ72" s="271"/>
       <c r="DK72" s="272" t="s">
@@ -17569,40 +17589,34 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="DG72:DH72"/>
+    <mergeCell ref="CW53:CY53"/>
+    <mergeCell ref="CW68:CX68"/>
+    <mergeCell ref="DJ68:DJ69"/>
+    <mergeCell ref="DE69:DE70"/>
+    <mergeCell ref="DG70:DH70"/>
+    <mergeCell ref="DI70:DJ70"/>
+    <mergeCell ref="CC53:CE53"/>
+    <mergeCell ref="CC68:CD68"/>
+    <mergeCell ref="CO68:CO69"/>
+    <mergeCell ref="CP68:CP69"/>
+    <mergeCell ref="CK69:CK70"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -17618,34 +17632,40 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="CC53:CE53"/>
-    <mergeCell ref="CC68:CD68"/>
-    <mergeCell ref="CO68:CO69"/>
-    <mergeCell ref="CP68:CP69"/>
-    <mergeCell ref="CK69:CK70"/>
-    <mergeCell ref="DG72:DH72"/>
-    <mergeCell ref="CW53:CY53"/>
-    <mergeCell ref="CW68:CX68"/>
-    <mergeCell ref="DJ68:DJ69"/>
-    <mergeCell ref="DE69:DE70"/>
-    <mergeCell ref="DG70:DH70"/>
-    <mergeCell ref="DI70:DJ70"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.8 _8:20PM
Boat Enabled -
InCapacity - [17,8,5,3,,Cnt] ,
NodeW - [-3] ,
BirdW - [7][CityW-MundiaSahi] ,
FuelW_Day - ['22][CityW-CM Nagar] ,
OnHost - [8+1]
VillageW=[0],
CityW=[1] ,
[X-MarketShieldMatrix-X] = [6,3,6,7] = [Lx -3 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.1.0.xlsx
+++ b/Usage_S_1.1.0.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B3F287-31E2-43F3-A21D-D0306921A2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917C7590-B55A-4092-80E0-AC1FBA40F5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
-    <sheet name="Hd" sheetId="4" r:id="rId2"/>
-    <sheet name="Purchase" sheetId="3" r:id="rId3"/>
-    <sheet name="Hist" sheetId="2" r:id="rId4"/>
+    <sheet name="MSM" sheetId="5" r:id="rId2"/>
+    <sheet name="Hd" sheetId="4" r:id="rId3"/>
+    <sheet name="Purchase" sheetId="3" r:id="rId4"/>
+    <sheet name="Hist" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="317">
   <si>
     <t>UnSettled</t>
   </si>
@@ -922,13 +923,79 @@
   </si>
   <si>
     <t>Spouse WL F RPF</t>
+  </si>
+  <si>
+    <t>X-NC Market-X</t>
+  </si>
+  <si>
+    <t>X-Cow(2)-X</t>
+  </si>
+  <si>
+    <t>X-BorderW-X</t>
+  </si>
+  <si>
+    <t>RailWay Union</t>
+  </si>
+  <si>
+    <t>bike</t>
+  </si>
+  <si>
+    <t>X-MambaF(1)-X</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Marwadi WL</t>
+  </si>
+  <si>
+    <t>X-MWL(5)  - X</t>
+  </si>
+  <si>
+    <t>ScootyT</t>
+  </si>
+  <si>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>1IS+1BR+ToLet1+1ckl+1INCpp+1BJDpp</t>
+  </si>
+  <si>
+    <t>X-RCCWL(2)  - X</t>
+  </si>
+  <si>
+    <t>X-MarketW(6)-X</t>
+  </si>
+  <si>
+    <t>Sahoo</t>
+  </si>
+  <si>
+    <t>00_X_25LB</t>
+  </si>
+  <si>
+    <t>Spouse WL F IT Teacher</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>(1PF+1PF]_RCC</t>
+  </si>
+  <si>
+    <t>x-92BR-x</t>
+  </si>
+  <si>
+    <t>Hub</t>
+  </si>
+  <si>
+    <t>1ckl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1126,8 +1193,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1242,8 +1330,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF385E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="49">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1861,11 +1955,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="335">
+  <cellXfs count="352">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2492,7 +2610,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2531,6 +2648,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2579,6 +2710,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2588,10 +2728,49 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2602,39 +2781,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2710,7 +2856,24 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2719,9 +2882,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF385E3"/>
       <color rgb="FF99FF99"/>
       <color rgb="FFD515BA"/>
-      <color rgb="FFF385E3"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2998,10 +3161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI26"/>
+  <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3014,11 +3177,11 @@
     <col min="7" max="7" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="117" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="117" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" style="192" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="117" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="117" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" style="152" customWidth="1"/>
@@ -3036,11 +3199,11 @@
     <col min="29" max="29" width="5.28515625" style="1" customWidth="1"/>
     <col min="30" max="30" width="5.28515625" customWidth="1"/>
     <col min="31" max="31" width="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z1" s="287" t="s">
+      <c r="Z1" s="292" t="s">
         <v>247</v>
       </c>
       <c r="AA1" s="36" t="s">
@@ -3055,12 +3218,12 @@
       <c r="AD1" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="AF1" s="273" t="s">
+      <c r="AF1" s="278" t="s">
         <v>241</v>
       </c>
-      <c r="AG1" s="274"/>
-      <c r="AH1" s="274"/>
-      <c r="AI1" s="275"/>
+      <c r="AG1" s="279"/>
+      <c r="AH1" s="279"/>
+      <c r="AI1" s="280"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -3069,15 +3232,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="280">
+      <c r="C2" s="285">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="284" t="s">
+      <c r="E2" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="285"/>
-      <c r="G2" s="286"/>
+      <c r="F2" s="290"/>
+      <c r="G2" s="291"/>
       <c r="H2" s="26" t="s">
         <v>43</v>
       </c>
@@ -3128,22 +3291,22 @@
       <c r="Y2" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="Z2" s="288"/>
+      <c r="Z2" s="293"/>
       <c r="AA2" s="36">
         <f>SUM(AA3:AA19)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB2" s="15">
         <f>SUM(AB3:AB25)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC2" s="36">
         <f>SUM(AC3:AC25)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AD2" s="36">
         <f>SUM(AD3:AD25)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>92</v>
@@ -3157,13 +3320,13 @@
       <c r="AI2" s="8"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="278" t="s">
+      <c r="A3" s="283" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="281"/>
+      <c r="C3" s="286"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
@@ -3178,10 +3341,10 @@
       </c>
       <c r="AB3" s="253"/>
       <c r="AC3" s="109"/>
-      <c r="AE3" s="289"/>
+      <c r="AE3" s="297"/>
     </row>
     <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="279"/>
+      <c r="A4" s="284"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -3191,7 +3354,9 @@
       <c r="E4" s="244">
         <v>5</v>
       </c>
-      <c r="F4" s="205"/>
+      <c r="F4" s="205">
+        <v>10</v>
+      </c>
       <c r="G4" s="247"/>
       <c r="H4" s="9" t="s">
         <v>199</v>
@@ -3221,13 +3386,13 @@
         <v>30</v>
       </c>
       <c r="Q4" s="154">
-        <v>0.4826388888888889</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>130</v>
       </c>
       <c r="S4" s="154">
-        <v>0.83333333333333337</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="U4" s="245">
         <v>45295</v>
@@ -3240,7 +3405,7 @@
       </c>
       <c r="AB4" s="20"/>
       <c r="AC4" s="24"/>
-      <c r="AE4" s="290"/>
+      <c r="AE4" s="298"/>
       <c r="AF4" s="25"/>
       <c r="AG4" s="25"/>
       <c r="AH4" s="24" t="s">
@@ -3255,7 +3420,9 @@
       <c r="E5" s="218">
         <v>30</v>
       </c>
-      <c r="F5" s="206"/>
+      <c r="F5" s="206">
+        <v>5</v>
+      </c>
       <c r="G5" s="127"/>
       <c r="H5" s="9" t="s">
         <v>1</v>
@@ -3266,9 +3433,7 @@
       <c r="J5" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K5" s="169" t="s">
-        <v>289</v>
-      </c>
+      <c r="K5" s="169"/>
       <c r="L5" s="167" t="s">
         <v>142</v>
       </c>
@@ -3285,10 +3450,10 @@
         <v>86</v>
       </c>
       <c r="Q5" s="154">
-        <v>0.4826388888888889</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="S5" s="154">
-        <v>0.83333333333333337</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="U5" s="245">
         <v>45295</v>
@@ -3301,7 +3466,7 @@
       </c>
       <c r="AB5" s="20"/>
       <c r="AC5" s="24"/>
-      <c r="AE5" s="290"/>
+      <c r="AE5" s="298"/>
       <c r="AF5" s="25"/>
       <c r="AG5" s="25"/>
       <c r="AH5" s="24" t="s">
@@ -3310,10 +3475,10 @@
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>4213</v>
+        <v>4368</v>
       </c>
       <c r="C6">
-        <v>4513</v>
+        <v>4552</v>
       </c>
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
@@ -3362,11 +3527,11 @@
         <v>221</v>
       </c>
       <c r="AA6" s="238">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB6" s="15"/>
       <c r="AC6" s="24"/>
-      <c r="AE6" s="290"/>
+      <c r="AE6" s="298"/>
       <c r="AF6" s="25"/>
       <c r="AH6" s="24"/>
     </row>
@@ -3377,9 +3542,6 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>207</v>
-      </c>
       <c r="E7" s="165"/>
       <c r="F7" s="242">
         <v>10</v>
@@ -3430,7 +3592,7 @@
       <c r="AA7" s="26"/>
       <c r="AB7" s="15"/>
       <c r="AC7" s="24"/>
-      <c r="AE7" s="290"/>
+      <c r="AE7" s="298"/>
       <c r="AF7" s="25"/>
       <c r="AG7" s="25"/>
       <c r="AH7" s="24" t="s">
@@ -3439,7 +3601,9 @@
     </row>
     <row r="8" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="219"/>
-      <c r="F8" s="242"/>
+      <c r="F8" s="242">
+        <v>25</v>
+      </c>
       <c r="G8" s="190"/>
       <c r="H8" s="9" t="s">
         <v>72</v>
@@ -3448,7 +3612,9 @@
         <v>17</v>
       </c>
       <c r="J8" s="213"/>
-      <c r="K8" s="194"/>
+      <c r="K8" s="275" t="s">
+        <v>300</v>
+      </c>
       <c r="L8" s="83" t="s">
         <v>214</v>
       </c>
@@ -3465,10 +3631,13 @@
         <v>65</v>
       </c>
       <c r="Q8" s="154">
-        <v>0.98263888888888884</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="S8" s="154">
-        <v>0.98263888888888884</v>
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="T8" s="274">
+        <v>1</v>
       </c>
       <c r="U8" s="245">
         <v>45295</v>
@@ -3482,7 +3651,7 @@
       <c r="AA8" s="25"/>
       <c r="AB8" s="15"/>
       <c r="AC8" s="24"/>
-      <c r="AE8" s="290"/>
+      <c r="AE8" s="298"/>
       <c r="AF8" s="25"/>
       <c r="AG8" s="25"/>
       <c r="AH8" s="24" t="s">
@@ -3495,7 +3664,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>11213</v>
+        <v>11368</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="165">
@@ -3546,10 +3715,22 @@
       </c>
       <c r="AA9" s="25"/>
       <c r="AB9" s="15"/>
-      <c r="AC9" s="24"/>
-      <c r="AE9" s="290"/>
-      <c r="AF9" s="25"/>
-      <c r="AH9" s="24"/>
+      <c r="AC9" s="24">
+        <v>1</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="298"/>
+      <c r="AF9" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG9" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="AH9" s="24" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="220">
@@ -3558,7 +3739,9 @@
       <c r="F10" s="206">
         <v>8</v>
       </c>
-      <c r="G10" s="177"/>
+      <c r="G10" s="177">
+        <v>10</v>
+      </c>
       <c r="H10" s="9" t="s">
         <v>81</v>
       </c>
@@ -3587,13 +3770,13 @@
         <v>66</v>
       </c>
       <c r="Q10" s="154">
-        <v>0.4826388888888889</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>126</v>
       </c>
       <c r="S10" s="154">
-        <v>0.4826388888888889</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="U10" s="245">
         <v>45295</v>
@@ -3609,7 +3792,7 @@
         <v>1</v>
       </c>
       <c r="AC10" s="24"/>
-      <c r="AE10" s="290"/>
+      <c r="AE10" s="298"/>
       <c r="AF10" s="25"/>
       <c r="AG10" s="25"/>
       <c r="AH10" s="24">
@@ -3622,13 +3805,15 @@
       </c>
       <c r="B11" s="8">
         <f>B9-B13</f>
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="E11" s="221"/>
       <c r="F11" s="242">
         <v>5</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="37">
+        <v>5</v>
+      </c>
       <c r="H11" s="9" t="s">
         <v>102</v>
       </c>
@@ -3680,7 +3865,7 @@
       <c r="AD11">
         <v>2</v>
       </c>
-      <c r="AE11" s="290"/>
+      <c r="AE11" s="298"/>
       <c r="AF11" s="25" t="s">
         <v>181</v>
       </c>
@@ -3698,7 +3883,9 @@
       <c r="F12" s="205">
         <v>55</v>
       </c>
-      <c r="G12" s="164"/>
+      <c r="G12" s="164">
+        <v>100</v>
+      </c>
       <c r="H12" s="28" t="s">
         <v>128</v>
       </c>
@@ -3725,11 +3912,11 @@
         <v>181</v>
       </c>
       <c r="Q12" s="154">
-        <v>0.53125</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="R12" s="24"/>
       <c r="S12" s="154">
-        <v>0.53125</v>
+        <v>0.83680555555555547</v>
       </c>
       <c r="U12" s="245">
         <v>45294</v>
@@ -3741,12 +3928,18 @@
         <v>234</v>
       </c>
       <c r="AB12" s="15"/>
-      <c r="AC12" s="36"/>
-      <c r="AE12" s="290"/>
-      <c r="AF12" s="25"/>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="24">
+      <c r="AC12" s="272">
         <v>1</v>
+      </c>
+      <c r="AE12" s="298"/>
+      <c r="AF12" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH12" s="24" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3755,7 +3948,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>11120</v>
+        <v>11368</v>
       </c>
       <c r="E13" s="36">
         <v>5</v>
@@ -3771,7 +3964,7 @@
         <v>17</v>
       </c>
       <c r="J13" s="228" t="s">
-        <v>186</v>
+        <v>311</v>
       </c>
       <c r="K13" s="194" t="s">
         <v>242</v>
@@ -3798,7 +3991,7 @@
       <c r="S13" s="154">
         <v>0.53125</v>
       </c>
-      <c r="T13" s="262">
+      <c r="T13" s="261">
         <v>1</v>
       </c>
       <c r="U13" s="245">
@@ -3812,7 +4005,7 @@
       </c>
       <c r="AB13" s="15"/>
       <c r="AC13" s="24"/>
-      <c r="AE13" s="290"/>
+      <c r="AE13" s="298"/>
       <c r="AF13" s="25"/>
       <c r="AG13" s="25"/>
       <c r="AH13" s="24"/>
@@ -3871,7 +4064,7 @@
       <c r="AC14" s="241">
         <v>1</v>
       </c>
-      <c r="AE14" s="290"/>
+      <c r="AE14" s="298"/>
       <c r="AF14" s="25"/>
       <c r="AG14" s="25"/>
       <c r="AH14" s="24" t="s">
@@ -3921,11 +4114,22 @@
       <c r="Z15" s="169" t="s">
         <v>238</v>
       </c>
-      <c r="AB15" s="20"/>
-      <c r="AC15" s="24"/>
-      <c r="AE15" s="290"/>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="25"/>
+      <c r="AB15" s="15">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="36">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="298"/>
+      <c r="AF15" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG15" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="AH15" s="24" t="s">
         <v>246</v>
       </c>
@@ -3947,41 +4151,43 @@
         <v>239</v>
       </c>
       <c r="AC16" s="24"/>
-      <c r="AE16" s="290"/>
+      <c r="AE16" s="298"/>
       <c r="AF16" s="25"/>
       <c r="AH16" s="24"/>
     </row>
     <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="282" t="s">
+      <c r="E17" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="283"/>
+      <c r="F17" s="288"/>
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>156</v>
+        <v>311</v>
       </c>
       <c r="I17" s="26"/>
-      <c r="J17" s="263"/>
+      <c r="J17" s="262"/>
       <c r="K17" s="169" t="s">
         <v>273</v>
       </c>
       <c r="L17" s="254"/>
-      <c r="N17" s="265" t="s">
+      <c r="N17" s="277" t="s">
         <v>276</v>
       </c>
-      <c r="O17" s="18"/>
-      <c r="P17" s="266"/>
-      <c r="Q17" s="159" t="s">
+      <c r="O17" s="82"/>
+      <c r="P17" s="349" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q17" s="273" t="s">
         <v>271</v>
       </c>
-      <c r="R17" s="277"/>
-      <c r="S17" s="267" t="s">
+      <c r="R17" s="282"/>
+      <c r="S17" s="266" t="s">
         <v>284</v>
       </c>
-      <c r="V17" s="260"/>
+      <c r="V17" s="259"/>
       <c r="Y17" s="25" t="s">
         <v>244</v>
       </c>
@@ -3991,10 +4197,16 @@
       <c r="AA17" s="50"/>
       <c r="AB17" s="15"/>
       <c r="AC17" s="115"/>
-      <c r="AD17" s="50"/>
-      <c r="AE17" s="290"/>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
+      <c r="AD17" s="50">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="298"/>
+      <c r="AF17" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="AG17" s="25" t="s">
+        <v>15</v>
+      </c>
       <c r="AH17" s="24" t="s">
         <v>246</v>
       </c>
@@ -4012,19 +4224,21 @@
       <c r="F18" s="24"/>
       <c r="G18" s="20"/>
       <c r="I18" s="226"/>
-      <c r="J18" s="263"/>
+      <c r="J18" s="262"/>
       <c r="K18" s="194" t="s">
         <v>269</v>
       </c>
-      <c r="L18" s="169"/>
-      <c r="M18" s="276"/>
-      <c r="N18" s="159" t="s">
-        <v>280</v>
-      </c>
-      <c r="O18" s="18"/>
-      <c r="P18" s="266"/>
-      <c r="Q18" s="159"/>
-      <c r="R18" s="277"/>
+      <c r="L18" s="345"/>
+      <c r="M18" s="347" t="s">
+        <v>315</v>
+      </c>
+      <c r="N18" s="350" t="s">
+        <v>306</v>
+      </c>
+      <c r="O18" s="350"/>
+      <c r="P18" s="351"/>
+      <c r="Q18" s="161"/>
+      <c r="R18" s="282"/>
       <c r="S18" s="17"/>
       <c r="X18" s="25" t="s">
         <v>286</v>
@@ -4036,7 +4250,7 @@
         <v>254</v>
       </c>
       <c r="AC18" s="24"/>
-      <c r="AE18" s="290"/>
+      <c r="AE18" s="298"/>
       <c r="AF18" s="25"/>
       <c r="AG18" s="25"/>
       <c r="AH18" s="24" t="s">
@@ -4044,23 +4258,24 @@
       </c>
     </row>
     <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="1"/>
       <c r="I19" s="226"/>
       <c r="K19" s="169" t="s">
         <v>288</v>
       </c>
       <c r="L19" s="119"/>
-      <c r="M19" s="276"/>
-      <c r="N19" s="159" t="s">
-        <v>275</v>
-      </c>
-      <c r="O19" s="292" t="s">
+      <c r="M19" s="348"/>
+      <c r="N19" s="346" t="s">
+        <v>313</v>
+      </c>
+      <c r="O19" s="294" t="s">
         <v>290</v>
       </c>
-      <c r="P19" s="292"/>
-      <c r="Q19" s="293" t="s">
+      <c r="P19" s="294"/>
+      <c r="Q19" s="295" t="s">
         <v>277</v>
       </c>
-      <c r="R19" s="293"/>
+      <c r="R19" s="295"/>
       <c r="S19" s="17"/>
       <c r="Y19" s="25" t="s">
         <v>244</v>
@@ -4072,7 +4287,7 @@
       <c r="AB19" s="79"/>
       <c r="AC19" s="115"/>
       <c r="AD19" s="50"/>
-      <c r="AE19" s="290"/>
+      <c r="AE19" s="298"/>
       <c r="AF19" s="25"/>
       <c r="AG19" s="25"/>
       <c r="AH19" s="24" t="s">
@@ -4080,23 +4295,26 @@
       </c>
     </row>
     <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="264"/>
-      <c r="B20" s="264"/>
+      <c r="A20" s="263"/>
+      <c r="B20" s="263"/>
       <c r="I20" s="227"/>
       <c r="K20" s="169" t="s">
         <v>272</v>
       </c>
       <c r="L20" s="119"/>
-      <c r="N20" s="159" t="s">
-        <v>274</v>
+      <c r="M20" s="231" t="s">
+        <v>315</v>
+      </c>
+      <c r="N20" s="344" t="s">
+        <v>310</v>
       </c>
       <c r="O20" s="18"/>
-      <c r="P20" s="266"/>
+      <c r="P20" s="265"/>
       <c r="Q20" s="159" t="s">
         <v>279</v>
       </c>
       <c r="R20" s="17"/>
-      <c r="S20" s="267" t="s">
+      <c r="S20" s="266" t="s">
         <v>285</v>
       </c>
       <c r="Y20" s="25" t="s">
@@ -4106,10 +4324,10 @@
         <v>260</v>
       </c>
       <c r="AA20" s="255"/>
-      <c r="AB20" s="259"/>
-      <c r="AC20" s="258"/>
-      <c r="AD20" s="257"/>
-      <c r="AE20" s="290"/>
+      <c r="AB20" s="258"/>
+      <c r="AC20" s="257"/>
+      <c r="AD20" s="256"/>
+      <c r="AE20" s="298"/>
       <c r="AF20" s="25"/>
       <c r="AG20" s="25"/>
       <c r="AH20" s="24" t="s">
@@ -4118,16 +4336,18 @@
     </row>
     <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K21" s="169" t="s">
-        <v>222</v>
-      </c>
-      <c r="N21" s="18"/>
-      <c r="O21" s="292" t="s">
+        <v>303</v>
+      </c>
+      <c r="N21" s="273" t="s">
+        <v>314</v>
+      </c>
+      <c r="O21" s="296" t="s">
         <v>291</v>
       </c>
-      <c r="P21" s="292"/>
-      <c r="Q21" s="268"/>
+      <c r="P21" s="296"/>
+      <c r="Q21" s="267"/>
       <c r="R21" s="17"/>
-      <c r="S21" s="267" t="s">
+      <c r="S21" s="266" t="s">
         <v>285</v>
       </c>
       <c r="X21" s="25" t="s">
@@ -4144,10 +4364,10 @@
       <c r="AC21" s="109">
         <v>1</v>
       </c>
-      <c r="AD21" s="44">
+      <c r="AD21" s="43">
         <v>1</v>
       </c>
-      <c r="AE21" s="290"/>
+      <c r="AE21" s="298"/>
       <c r="AF21" s="25" t="s">
         <v>65</v>
       </c>
@@ -4159,8 +4379,14 @@
       </c>
     </row>
     <row r="22" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="169" t="s">
+        <v>303</v>
+      </c>
       <c r="S22" s="24" t="s">
         <v>278</v>
+      </c>
+      <c r="X22" s="25" t="s">
+        <v>296</v>
       </c>
       <c r="Y22" s="25" t="s">
         <v>244</v>
@@ -4171,15 +4397,21 @@
       <c r="AA22" s="48"/>
       <c r="AB22" s="15"/>
       <c r="AC22" s="24"/>
-      <c r="AD22" s="49"/>
-      <c r="AE22" s="290"/>
-      <c r="AF22" s="25"/>
-      <c r="AG22" s="25"/>
+      <c r="AE22" s="298"/>
+      <c r="AF22" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="AG22" s="25" t="s">
+        <v>299</v>
+      </c>
       <c r="AH22" s="24" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="169" t="s">
+        <v>307</v>
+      </c>
       <c r="Y23" s="25" t="s">
         <v>244</v>
       </c>
@@ -4189,8 +4421,8 @@
       <c r="AA23" s="63"/>
       <c r="AB23" s="116"/>
       <c r="AC23" s="115"/>
-      <c r="AD23" s="51"/>
-      <c r="AE23" s="290"/>
+      <c r="AD23" s="50"/>
+      <c r="AE23" s="298"/>
       <c r="AF23" s="25"/>
       <c r="AG23" s="25"/>
       <c r="AH23" s="24" t="s">
@@ -4198,6 +4430,15 @@
       </c>
     </row>
     <row r="24" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q24" s="300" t="s">
+        <v>302</v>
+      </c>
+      <c r="R24" s="266">
+        <v>3</v>
+      </c>
+      <c r="S24" s="276" t="s">
+        <v>305</v>
+      </c>
       <c r="Y24" s="25" t="s">
         <v>244</v>
       </c>
@@ -4205,10 +4446,10 @@
         <v>264</v>
       </c>
       <c r="AA24" s="255"/>
-      <c r="AB24" s="259"/>
-      <c r="AC24" s="258"/>
+      <c r="AB24" s="258"/>
+      <c r="AC24" s="257"/>
       <c r="AD24" s="256"/>
-      <c r="AE24" s="290"/>
+      <c r="AE24" s="298"/>
       <c r="AF24" s="25"/>
       <c r="AG24" s="25"/>
       <c r="AH24" s="24" t="s">
@@ -4216,6 +4457,22 @@
       </c>
     </row>
     <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="25">
+        <v>2</v>
+      </c>
+      <c r="J25" s="231" t="s">
+        <v>309</v>
+      </c>
+      <c r="L25" s="231" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q25" s="301"/>
+      <c r="R25" s="266">
+        <v>1</v>
+      </c>
+      <c r="S25" s="276" t="s">
+        <v>304</v>
+      </c>
       <c r="X25" s="25" t="s">
         <v>271</v>
       </c>
@@ -4226,10 +4483,10 @@
         <v>265</v>
       </c>
       <c r="AA25" s="255"/>
-      <c r="AB25" s="259"/>
-      <c r="AC25" s="258"/>
+      <c r="AB25" s="258"/>
+      <c r="AC25" s="257"/>
       <c r="AD25" s="256"/>
-      <c r="AE25" s="291"/>
+      <c r="AE25" s="298"/>
       <c r="AF25" s="25"/>
       <c r="AG25" s="25"/>
       <c r="AH25" s="24" t="s">
@@ -4237,15 +4494,70 @@
       </c>
     </row>
     <row r="26" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="169" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q26" s="302"/>
+      <c r="R26" s="266">
+        <v>1</v>
+      </c>
+      <c r="S26" s="276" t="s">
+        <v>279</v>
+      </c>
       <c r="Y26" s="25" t="s">
         <v>244</v>
       </c>
       <c r="Z26" s="169" t="s">
         <v>260</v>
       </c>
+      <c r="AE26" s="298"/>
+    </row>
+    <row r="27" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I27" s="25">
+        <v>1</v>
+      </c>
+      <c r="J27" s="231" t="s">
+        <v>309</v>
+      </c>
+      <c r="L27" s="233"/>
+      <c r="X27" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y27" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z27" s="169" t="s">
+        <v>295</v>
+      </c>
+      <c r="AE27" s="298"/>
+    </row>
+    <row r="28" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z28" s="169" t="s">
+        <v>297</v>
+      </c>
+      <c r="AB28" s="15">
+        <v>2</v>
+      </c>
+      <c r="AD28">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="299"/>
+      <c r="AF28" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG28" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="AH28" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="AE3:AE28"/>
+    <mergeCell ref="Q24:Q26"/>
+    <mergeCell ref="N18:P18"/>
     <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="R17:R18"/>
@@ -4254,10 +4566,8 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AE3:AE25"/>
     <mergeCell ref="O19:P19"/>
     <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="O21:P21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4265,6 +4575,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA042A2-96BD-44DA-910A-B3A3BB4C8DBC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233D1215-9A26-4445-A7E9-A9CB7916DD22}">
   <dimension ref="B2:B14"/>
   <sheetViews>
@@ -4338,12 +4662,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N58" sqref="N58"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4367,18 +4691,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="309" t="s">
+      <c r="E1" s="319" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="311"/>
+      <c r="F1" s="321"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="309" t="s">
+      <c r="H1" s="319" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="310"/>
-      <c r="J1" s="311"/>
+      <c r="I1" s="320"/>
+      <c r="J1" s="321"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4396,7 +4720,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="312">
+      <c r="B2" s="322">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4423,26 +4747,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="315">
+      <c r="K2" s="325">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="307">
+      <c r="L2" s="314">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="297">
+      <c r="M2" s="306">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J63)</f>
-        <v>11080</v>
+        <f>SUM(E2:J65)</f>
+        <v>11328</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="313"/>
+      <c r="B3" s="323"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4457,13 +4781,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="316"/>
-      <c r="L3" s="277"/>
-      <c r="M3" s="298"/>
+      <c r="K3" s="326"/>
+      <c r="L3" s="282"/>
+      <c r="M3" s="307"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="314"/>
+      <c r="B4" s="324"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4478,9 +4802,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="316"/>
-      <c r="L4" s="277"/>
-      <c r="M4" s="298"/>
+      <c r="K4" s="326"/>
+      <c r="L4" s="282"/>
+      <c r="M4" s="307"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4562,7 +4886,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="299">
+      <c r="B7" s="303">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4579,22 +4903,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="301">
+      <c r="K7" s="308">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="303">
+      <c r="L7" s="310">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="305">
+      <c r="M7" s="312">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="300"/>
+      <c r="B8" s="305"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4615,9 +4939,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="302"/>
-      <c r="L8" s="304"/>
-      <c r="M8" s="306"/>
+      <c r="K8" s="309"/>
+      <c r="L8" s="311"/>
+      <c r="M8" s="313"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -4697,7 +5021,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="299">
+      <c r="B11" s="303">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -4724,7 +5048,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="300"/>
+      <c r="B12" s="305"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -4781,7 +5105,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="299">
+      <c r="B14" s="303">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -4804,7 +5128,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="300"/>
+      <c r="B15" s="305"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -4828,7 +5152,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="312">
+      <c r="B16" s="322">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -4859,7 +5183,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="313"/>
+      <c r="B17" s="323"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -4877,7 +5201,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="312">
+      <c r="B18" s="322">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4906,7 +5230,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="314"/>
+      <c r="B19" s="324"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4966,7 +5290,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="317">
+      <c r="B21" s="327">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4994,7 +5318,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="318"/>
+      <c r="B22" s="328"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -5046,7 +5370,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="280">
+      <c r="B24" s="285">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -5075,7 +5399,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="281"/>
+      <c r="B25" s="286"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -5103,7 +5427,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="280">
+      <c r="B26" s="285">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -5134,7 +5458,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="308"/>
+      <c r="B27" s="318"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5165,7 +5489,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="280">
+      <c r="B28" s="285">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -5187,7 +5511,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="281"/>
+      <c r="B29" s="286"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -5213,7 +5537,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="280">
+      <c r="B30" s="285">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -5236,7 +5560,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="281"/>
+      <c r="B31" s="286"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -5263,7 +5587,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="280">
+      <c r="B32" s="285">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -5285,7 +5609,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="281"/>
+      <c r="B33" s="286"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -5338,7 +5662,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="280">
+      <c r="B35" s="285">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -5365,7 +5689,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="281"/>
+      <c r="B36" s="286"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -5387,7 +5711,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="280">
+      <c r="B37" s="285">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -5420,7 +5744,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="281"/>
+      <c r="B38" s="286"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -5438,7 +5762,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="280">
+      <c r="B39" s="285">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -5465,7 +5789,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="308"/>
+      <c r="B40" s="318"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5493,7 +5817,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="280">
+      <c r="B41" s="285">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -5520,7 +5844,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="308"/>
+      <c r="B42" s="318"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5538,7 +5862,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="281"/>
+      <c r="B43" s="286"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -5567,7 +5891,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="280">
+      <c r="B44" s="285">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -5593,7 +5917,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="281"/>
+      <c r="B45" s="286"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -5618,7 +5942,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="280">
+      <c r="B46" s="285">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -5640,7 +5964,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="308"/>
+      <c r="B47" s="318"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5661,7 +5985,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="280">
+      <c r="B48" s="285">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -5681,7 +6005,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="308"/>
+      <c r="B49" s="318"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -5707,7 +6031,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="308"/>
+      <c r="B50" s="318"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -5734,7 +6058,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="280">
+      <c r="B51" s="285">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -5756,7 +6080,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="281"/>
+      <c r="B52" s="286"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -5789,7 +6113,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="280">
+      <c r="B53" s="285">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -5819,7 +6143,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="308"/>
+      <c r="B54" s="318"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -5846,7 +6170,7 @@
       <c r="A55" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="280">
+      <c r="B55" s="285">
         <v>31</v>
       </c>
       <c r="C55" s="96"/>
@@ -5874,7 +6198,7 @@
       <c r="M55" s="82"/>
     </row>
     <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="281"/>
+      <c r="B56" s="286"/>
       <c r="C56" s="96"/>
       <c r="D56" s="82"/>
       <c r="E56" s="82">
@@ -5900,7 +6224,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="294">
+      <c r="B57" s="315">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -5920,7 +6244,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="295"/>
+      <c r="B58" s="316"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -5949,7 +6273,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="296"/>
+      <c r="B59" s="317"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -5975,7 +6299,7 @@
       <c r="M59" s="18"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="280">
+      <c r="B60" s="285">
         <v>2</v>
       </c>
       <c r="C60" s="142"/>
@@ -6001,7 +6325,7 @@
       <c r="M60" s="18"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="308"/>
+      <c r="B61" s="318"/>
       <c r="C61" s="142"/>
       <c r="D61" s="18">
         <v>240</v>
@@ -6027,7 +6351,7 @@
       <c r="M61" s="18"/>
     </row>
     <row r="62" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="281"/>
+      <c r="B62" s="286"/>
       <c r="C62" s="142"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
@@ -6048,7 +6372,7 @@
       <c r="A63" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="280">
+      <c r="B63" s="303">
         <v>3</v>
       </c>
       <c r="C63" s="142"/>
@@ -6069,32 +6393,50 @@
       <c r="L63" s="18"/>
       <c r="M63" s="18"/>
     </row>
-    <row r="64" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="281"/>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B64" s="304"/>
       <c r="C64" s="142"/>
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
-      <c r="G64" s="334">
+      <c r="G64" s="18">
         <v>55</v>
       </c>
       <c r="H64" s="18"/>
-      <c r="I64" s="334">
+      <c r="I64" s="18">
         <v>18</v>
       </c>
-      <c r="J64" s="334">
+      <c r="J64" s="18">
         <v>20</v>
       </c>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
       <c r="M64" s="18"/>
     </row>
+    <row r="65" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="305"/>
+      <c r="C65" s="142"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18">
+        <v>100</v>
+      </c>
+      <c r="G65" s="18">
+        <v>25</v>
+      </c>
+      <c r="H65" s="18">
+        <v>10</v>
+      </c>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18">
+        <v>20</v>
+      </c>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B41:B43"/>
@@ -6105,13 +6447,14 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B63:B65"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B11:B12"/>
@@ -6120,16 +6463,19 @@
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B51:B52"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EF39B9-450C-4C51-9807-7AFD5CC29C14}">
   <dimension ref="A1:DN73"/>
   <sheetViews>
@@ -9330,10 +9676,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="282" t="s">
+      <c r="AG24" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="283"/>
+      <c r="AH24" s="288"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -9353,10 +9699,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="282" t="s">
+      <c r="AZ24" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="283"/>
+      <c r="BA24" s="288"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -9376,10 +9722,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="282" t="s">
+      <c r="BR24" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="283"/>
+      <c r="BS24" s="288"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -9402,10 +9748,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="284" t="s">
+      <c r="B26" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="286"/>
+      <c r="C26" s="291"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9442,10 +9788,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="284" t="s">
+      <c r="R26" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="286"/>
+      <c r="S26" s="291"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9482,10 +9828,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="284" t="s">
+      <c r="AG26" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="286"/>
+      <c r="AH26" s="291"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9522,10 +9868,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="284" t="s">
+      <c r="AW26" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="286"/>
+      <c r="AX26" s="291"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9562,10 +9908,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="284" t="s">
+      <c r="BM26" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="286"/>
+      <c r="BN26" s="291"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -10559,7 +10905,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="323">
+      <c r="AX32" s="333">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -10597,7 +10943,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="323">
+      <c r="BN32" s="333">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -10746,7 +11092,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="324"/>
+      <c r="AX33" s="334"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10782,7 +11128,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="324"/>
+      <c r="BN33" s="334"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -10933,7 +11279,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="325"/>
+      <c r="AX34" s="335"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10971,7 +11317,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="325"/>
+      <c r="BN34" s="335"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11202,10 +11548,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="282" t="s">
+      <c r="B36" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="283"/>
+      <c r="C36" s="288"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -11223,10 +11569,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="282" t="s">
+      <c r="R36" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="283"/>
+      <c r="S36" s="288"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -11244,10 +11590,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="282" t="s">
+      <c r="AG36" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="283"/>
+      <c r="AH36" s="288"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -11265,10 +11611,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="282" t="s">
+      <c r="AW36" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="283"/>
+      <c r="AX36" s="288"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -11286,10 +11632,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="282" t="s">
+      <c r="BM36" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="283"/>
+      <c r="BN36" s="288"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -11309,10 +11655,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="284" t="s">
+      <c r="B38" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="286"/>
+      <c r="C38" s="291"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11352,10 +11698,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="284" t="s">
+      <c r="S38" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="286"/>
+      <c r="T38" s="291"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11395,11 +11741,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="284" t="s">
+      <c r="AJ38" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="285"/>
-      <c r="AL38" s="286"/>
+      <c r="AK38" s="290"/>
+      <c r="AL38" s="291"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11444,11 +11790,11 @@
         <f ca="1">TODAY()</f>
         <v>45294</v>
       </c>
-      <c r="BD38" s="284" t="s">
+      <c r="BD38" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="285"/>
-      <c r="BF38" s="286"/>
+      <c r="BE38" s="290"/>
+      <c r="BF38" s="291"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11488,11 +11834,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="284" t="s">
+      <c r="BW38" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="285"/>
-      <c r="BY38" s="286"/>
+      <c r="BX38" s="290"/>
+      <c r="BY38" s="291"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -12444,7 +12790,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="323">
+      <c r="C44" s="333">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12482,10 +12828,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="332">
+      <c r="S44" s="342">
         <v>25</v>
       </c>
-      <c r="T44" s="323">
+      <c r="T44" s="333">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12494,7 +12840,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="326" t="s">
+      <c r="W44" s="336" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12523,10 +12869,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="332">
+      <c r="AJ44" s="342">
         <v>50</v>
       </c>
-      <c r="AK44" s="323">
+      <c r="AK44" s="333">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12536,7 +12882,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="326" t="s">
+      <c r="AO44" s="336" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -12566,7 +12912,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="332">
+      <c r="BD44" s="342">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -12577,7 +12923,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="326" t="s">
+      <c r="BI44" s="336" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -12606,7 +12952,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="332">
+      <c r="BW44" s="342">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -12617,7 +12963,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="326" t="s">
+      <c r="CB44" s="336" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -12649,7 +12995,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="324"/>
+      <c r="C45" s="334"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -12683,15 +13029,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="333"/>
-      <c r="T45" s="325"/>
+      <c r="S45" s="343"/>
+      <c r="T45" s="335"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="327"/>
+      <c r="W45" s="337"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12718,8 +13064,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="333"/>
-      <c r="AK45" s="325"/>
+      <c r="AJ45" s="343"/>
+      <c r="AK45" s="335"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -12727,7 +13073,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="327"/>
+      <c r="AO45" s="337"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12755,7 +13101,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="333"/>
+      <c r="BD45" s="343"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -12766,7 +13112,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="327"/>
+      <c r="BI45" s="337"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12793,7 +13139,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="333"/>
+      <c r="BW45" s="343"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -12802,7 +13148,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="327"/>
+      <c r="CB45" s="337"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -12832,7 +13178,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="325"/>
+      <c r="C46" s="335"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13259,10 +13605,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="282" t="s">
+      <c r="B48" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="283"/>
+      <c r="C48" s="288"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -13281,10 +13627,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="282" t="s">
+      <c r="S48" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="283"/>
+      <c r="T48" s="288"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -13437,11 +13783,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="328"/>
+      <c r="AQ49" s="338"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="320"/>
-      <c r="AV49" s="321"/>
+      <c r="AU49" s="330"/>
+      <c r="AV49" s="331"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -13453,11 +13799,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="328"/>
+      <c r="BK49" s="338"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="320"/>
-      <c r="BP49" s="321"/>
+      <c r="BO49" s="330"/>
+      <c r="BP49" s="331"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -13468,20 +13814,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="328"/>
+      <c r="CD49" s="338"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="320"/>
-      <c r="CI49" s="321"/>
+      <c r="CH49" s="330"/>
+      <c r="CI49" s="331"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="282" t="s">
+      <c r="AJ50" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="283"/>
+      <c r="AK50" s="288"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -13492,19 +13838,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="328"/>
+      <c r="AQ50" s="338"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="320"/>
-      <c r="AV50" s="321"/>
+      <c r="AU50" s="330"/>
+      <c r="AV50" s="331"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="282" t="s">
+      <c r="BD50" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="283"/>
+      <c r="BE50" s="288"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -13513,18 +13859,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="328"/>
+      <c r="BK50" s="338"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="320"/>
-      <c r="BP50" s="321"/>
+      <c r="BO50" s="330"/>
+      <c r="BP50" s="331"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="282" t="s">
+      <c r="BW50" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="283"/>
+      <c r="BX50" s="288"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -13533,21 +13879,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="328"/>
+      <c r="CD50" s="338"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="320"/>
-      <c r="CI50" s="321"/>
+      <c r="CH50" s="330"/>
+      <c r="CI50" s="331"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="284" t="s">
+      <c r="B51" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="285"/>
-      <c r="D51" s="286"/>
+      <c r="C51" s="290"/>
+      <c r="D51" s="291"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -13597,14 +13943,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="329"/>
+      <c r="AQ51" s="339"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="330"/>
-      <c r="AV51" s="331"/>
+      <c r="AU51" s="340"/>
+      <c r="AV51" s="341"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -13616,14 +13962,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="329"/>
+      <c r="BK51" s="339"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="330"/>
-      <c r="BP51" s="331"/>
+      <c r="BO51" s="340"/>
+      <c r="BP51" s="341"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -13634,14 +13980,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="329"/>
+      <c r="CD51" s="339"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="330"/>
-      <c r="CI51" s="331"/>
+      <c r="CH51" s="340"/>
+      <c r="CI51" s="341"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -13662,11 +14008,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="284" t="s">
+      <c r="V52" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="285"/>
-      <c r="X52" s="286"/>
+      <c r="W52" s="290"/>
+      <c r="X52" s="291"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -13768,11 +14114,11 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="46"/>
-      <c r="AO53" s="284" t="s">
+      <c r="AO53" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="AP53" s="285"/>
-      <c r="AQ53" s="286"/>
+      <c r="AP53" s="290"/>
+      <c r="AQ53" s="291"/>
       <c r="AR53" s="26" t="s">
         <v>43</v>
       </c>
@@ -13819,11 +14165,11 @@
         <f ca="1">TODAY()</f>
         <v>45294</v>
       </c>
-      <c r="BJ53" s="284" t="s">
+      <c r="BJ53" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="BK53" s="285"/>
-      <c r="BL53" s="286"/>
+      <c r="BK53" s="290"/>
+      <c r="BL53" s="291"/>
       <c r="BM53" s="26" t="s">
         <v>43</v>
       </c>
@@ -13866,11 +14212,11 @@
       <c r="BZ53" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="CC53" s="284" t="s">
+      <c r="CC53" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="CD53" s="285"/>
-      <c r="CE53" s="286"/>
+      <c r="CD53" s="290"/>
+      <c r="CE53" s="291"/>
       <c r="CF53" s="26" t="s">
         <v>43</v>
       </c>
@@ -13914,11 +14260,11 @@
         <v>108</v>
       </c>
       <c r="CV53" s="42"/>
-      <c r="CW53" s="284" t="s">
+      <c r="CW53" s="289" t="s">
         <v>145</v>
       </c>
-      <c r="CX53" s="285"/>
-      <c r="CY53" s="286"/>
+      <c r="CX53" s="290"/>
+      <c r="CY53" s="291"/>
       <c r="CZ53" s="26" t="s">
         <v>43</v>
       </c>
@@ -16275,7 +16621,7 @@
       <c r="DK62" s="154">
         <v>0.83333333333333337</v>
       </c>
-      <c r="DL62" s="261">
+      <c r="DL62" s="260">
         <v>3</v>
       </c>
       <c r="DM62" s="248">
@@ -16790,7 +17136,7 @@
       <c r="DK64" s="154">
         <v>0.88611111111111107</v>
       </c>
-      <c r="DL64" s="262">
+      <c r="DL64" s="261">
         <v>1</v>
       </c>
       <c r="DM64" s="248">
@@ -17005,10 +17351,10 @@
       </c>
     </row>
     <row r="66" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="282" t="s">
+      <c r="B66" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="283"/>
+      <c r="C66" s="288"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -17021,8 +17367,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="320"/>
-      <c r="O66" s="321"/>
+      <c r="N66" s="330"/>
+      <c r="O66" s="331"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -17162,18 +17508,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="276"/>
+      <c r="J67" s="281"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="320"/>
-      <c r="O67" s="321"/>
+      <c r="N67" s="330"/>
+      <c r="O67" s="331"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="282" t="s">
+      <c r="V67" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="283"/>
+      <c r="W67" s="288"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -17185,8 +17531,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="320"/>
-      <c r="AI67" s="321"/>
+      <c r="AH67" s="330"/>
+      <c r="AI67" s="331"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -17257,7 +17603,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="322"/>
+      <c r="J68" s="332"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -17273,17 +17619,17 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="276"/>
+      <c r="AD68" s="281"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="320"/>
-      <c r="AI68" s="321"/>
+      <c r="AH68" s="330"/>
+      <c r="AI68" s="331"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
-      <c r="AO68" s="282" t="s">
+      <c r="AO68" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="AP68" s="283"/>
+      <c r="AP68" s="288"/>
       <c r="AQ68" s="189"/>
       <c r="AR68" s="9">
         <f>SUM(AO55:AQ66)</f>
@@ -17295,15 +17641,15 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="320"/>
-      <c r="BB68" s="321"/>
+      <c r="BA68" s="330"/>
+      <c r="BB68" s="331"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
-      <c r="BJ68" s="282" t="s">
+      <c r="BJ68" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="BK68" s="283"/>
+      <c r="BK68" s="288"/>
       <c r="BL68" s="189"/>
       <c r="BM68" s="9">
         <f>SUM(BJ55:BL66)</f>
@@ -17315,15 +17661,15 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="320"/>
-      <c r="BW68" s="321"/>
+      <c r="BV68" s="330"/>
+      <c r="BW68" s="331"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
       <c r="BZ68" s="46"/>
-      <c r="CC68" s="282" t="s">
+      <c r="CC68" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="CD68" s="283"/>
+      <c r="CD68" s="288"/>
       <c r="CE68" s="189"/>
       <c r="CF68" s="9">
         <f>SUM(CC55:CE66)</f>
@@ -17335,41 +17681,41 @@
       <c r="CJ68" s="119"/>
       <c r="CK68" s="117"/>
       <c r="CN68" s="2"/>
-      <c r="CO68" s="320"/>
-      <c r="CP68" s="321"/>
+      <c r="CO68" s="330"/>
+      <c r="CP68" s="331"/>
       <c r="CQ68" s="1"/>
       <c r="CR68" s="1"/>
       <c r="CS68" s="46"/>
       <c r="CV68" s="110"/>
-      <c r="CW68" s="282" t="s">
+      <c r="CW68" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="CX68" s="283"/>
+      <c r="CX68" s="288"/>
       <c r="CY68" s="189"/>
       <c r="CZ68" s="9">
         <f>SUM(CW55:CY66)</f>
         <v>525</v>
       </c>
       <c r="DA68" s="26"/>
-      <c r="DB68" s="263"/>
-      <c r="DC68" s="269"/>
+      <c r="DB68" s="262"/>
+      <c r="DC68" s="268"/>
       <c r="DD68" s="254"/>
       <c r="DE68" s="117"/>
-      <c r="DF68" s="265" t="s">
+      <c r="DF68" s="264" t="s">
         <v>276</v>
       </c>
       <c r="DG68" s="18"/>
-      <c r="DH68" s="266"/>
+      <c r="DH68" s="265"/>
       <c r="DI68" s="159" t="s">
         <v>271</v>
       </c>
-      <c r="DJ68" s="277"/>
-      <c r="DK68" s="267" t="s">
+      <c r="DJ68" s="282"/>
+      <c r="DK68" s="266" t="s">
         <v>284</v>
       </c>
       <c r="DL68" s="1"/>
       <c r="DM68" s="46"/>
-      <c r="DN68" s="260"/>
+      <c r="DN68" s="259"/>
     </row>
     <row r="69" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V69" s="236"/>
@@ -17382,7 +17728,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="322"/>
+      <c r="AD69" s="332"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -17398,10 +17744,10 @@
       <c r="AT69" s="119"/>
       <c r="AU69" s="192"/>
       <c r="AV69" s="119"/>
-      <c r="AW69" s="276"/>
+      <c r="AW69" s="281"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="320"/>
-      <c r="BB69" s="321"/>
+      <c r="BA69" s="330"/>
+      <c r="BB69" s="331"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
@@ -17412,10 +17758,10 @@
       <c r="BO69" s="119"/>
       <c r="BP69" s="192"/>
       <c r="BQ69" s="119"/>
-      <c r="BR69" s="276"/>
+      <c r="BR69" s="281"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="320"/>
-      <c r="BW69" s="321"/>
+      <c r="BV69" s="330"/>
+      <c r="BW69" s="331"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
       <c r="BZ69" s="46"/>
@@ -17426,10 +17772,10 @@
       <c r="CH69" s="119"/>
       <c r="CI69" s="192"/>
       <c r="CJ69" s="119"/>
-      <c r="CK69" s="276"/>
+      <c r="CK69" s="281"/>
       <c r="CN69" s="2"/>
-      <c r="CO69" s="320"/>
-      <c r="CP69" s="321"/>
+      <c r="CO69" s="330"/>
+      <c r="CP69" s="331"/>
       <c r="CQ69" s="1"/>
       <c r="CR69" s="1"/>
       <c r="CS69" s="46"/>
@@ -17438,17 +17784,17 @@
       <c r="CX69" s="24"/>
       <c r="CY69" s="20"/>
       <c r="DA69" s="226"/>
-      <c r="DB69" s="263"/>
+      <c r="DB69" s="262"/>
       <c r="DC69" s="169"/>
       <c r="DD69" s="169"/>
-      <c r="DE69" s="276"/>
+      <c r="DE69" s="281"/>
       <c r="DF69" s="159" t="s">
         <v>280</v>
       </c>
       <c r="DG69" s="18"/>
-      <c r="DH69" s="266"/>
+      <c r="DH69" s="265"/>
       <c r="DI69" s="159"/>
-      <c r="DJ69" s="277"/>
+      <c r="DJ69" s="282"/>
       <c r="DK69" s="17"/>
       <c r="DL69" s="1"/>
       <c r="DM69" s="46"/>
@@ -17461,7 +17807,7 @@
       <c r="AT70" s="117"/>
       <c r="AU70" s="192"/>
       <c r="AV70" s="119"/>
-      <c r="AW70" s="276"/>
+      <c r="AW70" s="281"/>
       <c r="AZ70" s="2"/>
       <c r="BA70" s="152"/>
       <c r="BB70" s="1"/>
@@ -17475,7 +17821,7 @@
       <c r="BO70" s="117"/>
       <c r="BP70" s="192"/>
       <c r="BQ70" s="119"/>
-      <c r="BR70" s="276"/>
+      <c r="BR70" s="281"/>
       <c r="BU70" s="2"/>
       <c r="BV70" s="152"/>
       <c r="BW70" s="1"/>
@@ -17490,7 +17836,7 @@
       <c r="CH70" s="137"/>
       <c r="CI70" s="203"/>
       <c r="CJ70" s="201"/>
-      <c r="CK70" s="322"/>
+      <c r="CK70" s="332"/>
       <c r="CL70" s="50"/>
       <c r="CM70" s="50"/>
       <c r="CN70" s="79"/>
@@ -17507,18 +17853,18 @@
       <c r="DB70" s="117"/>
       <c r="DC70" s="194"/>
       <c r="DD70" s="119"/>
-      <c r="DE70" s="276"/>
+      <c r="DE70" s="281"/>
       <c r="DF70" s="159" t="s">
         <v>275</v>
       </c>
-      <c r="DG70" s="292" t="s">
+      <c r="DG70" s="296" t="s">
         <v>290</v>
       </c>
-      <c r="DH70" s="292"/>
-      <c r="DI70" s="293" t="s">
+      <c r="DH70" s="296"/>
+      <c r="DI70" s="295" t="s">
         <v>277</v>
       </c>
-      <c r="DJ70" s="293"/>
+      <c r="DJ70" s="295"/>
       <c r="DK70" s="17"/>
       <c r="DL70" s="1"/>
       <c r="DM70" s="46"/>
@@ -17575,12 +17921,12 @@
         <v>274</v>
       </c>
       <c r="DG71" s="18"/>
-      <c r="DH71" s="266"/>
+      <c r="DH71" s="265"/>
       <c r="DI71" s="159" t="s">
         <v>279</v>
       </c>
       <c r="DJ71" s="17"/>
-      <c r="DK71" s="267" t="s">
+      <c r="DK71" s="266" t="s">
         <v>285</v>
       </c>
       <c r="DL71" s="1"/>
@@ -17598,13 +17944,13 @@
       <c r="DD72" s="137"/>
       <c r="DE72" s="137"/>
       <c r="DF72" s="5"/>
-      <c r="DG72" s="319" t="s">
+      <c r="DG72" s="329" t="s">
         <v>291</v>
       </c>
-      <c r="DH72" s="319"/>
-      <c r="DI72" s="270"/>
-      <c r="DJ72" s="271"/>
-      <c r="DK72" s="272" t="s">
+      <c r="DH72" s="329"/>
+      <c r="DI72" s="269"/>
+      <c r="DJ72" s="270"/>
+      <c r="DK72" s="271" t="s">
         <v>285</v>
       </c>
       <c r="DL72" s="65"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.9 _11:20PM
Boat Enabled -
InCapacity - [17,8,5,3,1,Cnt] ,
NodeW - [-3] ,
BirdW - [7][CityW-MundiaSahi] ,
FuelW_Night - ['22][CityW-CM Nagar] ,
OnHost - [8+1]
VillageW=[0],
CityW=[1] ,
[X-MarketShieldMatrix-X] = [6,3,6,7] = [Lx -3 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.1.0.xlsx
+++ b/Usage_S_1.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917C7590-B55A-4092-80E0-AC1FBA40F5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7AA833-3E81-463C-9BC2-3B088F5294CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -973,9 +973,6 @@
     <t>00_X_25LB</t>
   </si>
   <si>
-    <t>Spouse WL F IT Teacher</t>
-  </si>
-  <si>
     <t>Auto</t>
   </si>
   <si>
@@ -989,6 +986,9 @@
   </si>
   <si>
     <t>1ckl</t>
+  </si>
+  <si>
+    <t>MarketXRecovery</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="352">
+  <cellXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2627,7 +2627,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2662,6 +2661,84 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2671,152 +2748,95 @@
     <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2856,24 +2876,26 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3161,10 +3183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI28"/>
+  <dimension ref="A1:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,176 +3197,178 @@
     <col min="5" max="5" width="7" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="117" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="192" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="117" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" style="117" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" style="152" customWidth="1"/>
-    <col min="18" max="18" width="4.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" style="24" customWidth="1"/>
-    <col min="22" max="22" width="5.140625" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.85546875" customWidth="1"/>
-    <col min="28" max="28" width="3.85546875" style="2" customWidth="1"/>
-    <col min="29" max="29" width="5.28515625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="5.28515625" customWidth="1"/>
-    <col min="31" max="31" width="1" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="117" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" style="192" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="117" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="117" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="152" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" style="24" customWidth="1"/>
+    <col min="23" max="23" width="5.140625" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.85546875" customWidth="1"/>
+    <col min="29" max="29" width="3.85546875" style="2" customWidth="1"/>
+    <col min="30" max="30" width="5.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="5.28515625" customWidth="1"/>
+    <col min="32" max="32" width="1" customWidth="1"/>
+    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z1" s="292" t="s">
+    <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA1" s="308" t="s">
         <v>247</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AB1" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="AC1" s="250" t="s">
+      <c r="AD1" s="250" t="s">
         <v>236</v>
       </c>
-      <c r="AD1" s="249" t="s">
+      <c r="AE1" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="AF1" s="278" t="s">
+      <c r="AG1" s="305" t="s">
         <v>241</v>
       </c>
-      <c r="AG1" s="279"/>
-      <c r="AH1" s="279"/>
-      <c r="AI1" s="280"/>
+      <c r="AH1" s="306"/>
+      <c r="AI1" s="306"/>
+      <c r="AJ1" s="307"/>
     </row>
-    <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="285">
+      <c r="C2" s="287">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="289" t="s">
+      <c r="E2" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="290"/>
-      <c r="G2" s="291"/>
-      <c r="H2" s="26" t="s">
+      <c r="F2" s="292"/>
+      <c r="G2" s="293"/>
+      <c r="H2" s="281"/>
+      <c r="I2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="J2" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="214" t="s">
+      <c r="L2" s="214" t="s">
         <v>195</v>
       </c>
-      <c r="L2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="M2" s="83" t="s">
+      <c r="N2" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="143" t="s">
+      <c r="P2" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="171" t="s">
+      <c r="Q2" s="171" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" s="153" t="s">
+      <c r="R2" s="153" t="s">
         <v>267</v>
       </c>
-      <c r="R2" s="36" t="s">
+      <c r="S2" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="S2" s="156" t="s">
+      <c r="T2" s="156" t="s">
         <v>268</v>
       </c>
-      <c r="T2" s="214" t="s">
+      <c r="U2" s="214" t="s">
         <v>224</v>
       </c>
-      <c r="U2" s="36" t="s">
+      <c r="V2" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="W2" s="98">
+      <c r="X2" s="98">
         <f ca="1">TODAY()</f>
         <v>45294</v>
       </c>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="9" t="s">
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="Z2" s="293"/>
-      <c r="AA2" s="36">
-        <f>SUM(AA3:AA19)</f>
+      <c r="AA2" s="309"/>
+      <c r="AB2" s="36">
+        <f>SUM(AB3:AB19)</f>
         <v>6</v>
       </c>
-      <c r="AB2" s="15">
-        <f>SUM(AB3:AB25)</f>
+      <c r="AC2" s="15">
+        <f>SUM(AC3:AC25)</f>
         <v>3</v>
-      </c>
-      <c r="AC2" s="36">
-        <f>SUM(AC3:AC25)</f>
-        <v>6</v>
       </c>
       <c r="AD2" s="36">
         <f>SUM(AD3:AD25)</f>
+        <v>6</v>
+      </c>
+      <c r="AE2" s="36">
+        <f>SUM(AE3:AE25)</f>
         <v>7</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AG2" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AG2" s="26" t="s">
+      <c r="AH2" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="AH2" s="26" t="s">
+      <c r="AI2" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="283" t="s">
+    <row r="3" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="285" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="286"/>
+      <c r="C3" s="288"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="25" t="s">
+      <c r="Z3" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z3" s="169" t="s">
+      <c r="AA3" s="169" t="s">
         <v>218</v>
       </c>
-      <c r="AA3" s="238">
+      <c r="AB3" s="238">
         <v>1</v>
       </c>
-      <c r="AB3" s="253"/>
-      <c r="AC3" s="109"/>
-      <c r="AE3" s="297"/>
+      <c r="AC3" s="253"/>
+      <c r="AD3" s="109"/>
+      <c r="AF3" s="297"/>
     </row>
-    <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="284"/>
+    <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="286"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -3357,63 +3381,68 @@
       <c r="F4" s="205">
         <v>10</v>
       </c>
-      <c r="G4" s="247"/>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="353">
+        <v>10</v>
+      </c>
+      <c r="H4" s="353"/>
+      <c r="I4" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="I4" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="213" t="s">
+      <c r="J4" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="213" t="s">
         <v>187</v>
       </c>
-      <c r="K4" s="169" t="s">
+      <c r="L4" s="169" t="s">
         <v>281</v>
       </c>
-      <c r="L4" s="83" t="s">
+      <c r="M4" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="M4" s="224" t="s">
+      <c r="N4" s="224" t="s">
         <v>156</v>
       </c>
-      <c r="N4" s="143" t="s">
+      <c r="O4" s="143" t="s">
         <v>193</v>
       </c>
-      <c r="O4" s="169" t="s">
+      <c r="P4" s="169" t="s">
         <v>156</v>
       </c>
-      <c r="P4" s="37" t="s">
+      <c r="Q4" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="154">
+      <c r="R4" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="S4" s="154">
+      <c r="T4" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="U4" s="245">
+      <c r="V4" s="245">
         <v>45295</v>
       </c>
-      <c r="Y4" s="25" t="s">
+      <c r="Z4" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z4" s="169" t="s">
+      <c r="AA4" s="169" t="s">
         <v>220</v>
       </c>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="24"/>
-      <c r="AE4" s="298"/>
-      <c r="AF4" s="25"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="24"/>
+      <c r="AF4" s="298"/>
       <c r="AG4" s="25"/>
-      <c r="AH4" s="24" t="s">
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>275</v>
+      </c>
       <c r="D5" s="156">
         <v>-2</v>
       </c>
@@ -3424,315 +3453,340 @@
         <v>5</v>
       </c>
       <c r="G5" s="127"/>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="127">
+        <v>50</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="213" t="s">
+      <c r="J5" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K5" s="169"/>
-      <c r="L5" s="167" t="s">
+      <c r="L5" s="169" t="s">
+        <v>288</v>
+      </c>
+      <c r="M5" s="167" t="s">
         <v>142</v>
       </c>
-      <c r="M5" s="224" t="s">
+      <c r="N5" s="224" t="s">
         <v>85</v>
       </c>
-      <c r="N5" s="143" t="s">
+      <c r="O5" s="143" t="s">
         <v>119</v>
       </c>
-      <c r="O5" s="237" t="s">
+      <c r="P5" s="237" t="s">
         <v>137</v>
       </c>
-      <c r="P5" s="197" t="s">
+      <c r="Q5" s="197" t="s">
         <v>86</v>
       </c>
-      <c r="Q5" s="154">
+      <c r="R5" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="S5" s="154">
+      <c r="T5" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="U5" s="245">
+      <c r="V5" s="245">
         <v>45295</v>
       </c>
-      <c r="Y5" s="25" t="s">
+      <c r="Z5" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z5" s="215" t="s">
+      <c r="AA5" s="215" t="s">
         <v>219</v>
       </c>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="24"/>
-      <c r="AE5" s="298"/>
-      <c r="AF5" s="25"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="24"/>
+      <c r="AF5" s="298"/>
       <c r="AG5" s="25"/>
-      <c r="AH5" s="24" t="s">
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>4368</v>
       </c>
       <c r="C6">
-        <v>4552</v>
+        <v>4000</v>
       </c>
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
       <c r="G6" s="127"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="127">
+        <v>30</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="I6" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="213" t="s">
+      <c r="J6" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K6" s="169"/>
-      <c r="L6" s="83" t="s">
+      <c r="L6" s="169" t="s">
+        <v>288</v>
+      </c>
+      <c r="M6" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="M6" s="83" t="s">
+      <c r="N6" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="143" t="s">
+      <c r="O6" s="143" t="s">
         <v>120</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="P6" s="176" t="s">
+      <c r="Q6" s="176" t="s">
         <v>69</v>
       </c>
-      <c r="Q6" s="154">
+      <c r="R6" s="154">
         <v>0.98263888888888884</v>
       </c>
-      <c r="S6" s="154">
+      <c r="T6" s="154">
         <v>0.88611111111111107</v>
       </c>
-      <c r="U6" s="245">
+      <c r="V6" s="245">
         <v>45294</v>
       </c>
-      <c r="X6" s="25" t="s">
+      <c r="Y6" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="Y6" s="25" t="s">
+      <c r="Z6" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z6" s="169" t="s">
+      <c r="AA6" s="169" t="s">
         <v>221</v>
       </c>
-      <c r="AA6" s="238">
+      <c r="AB6" s="238">
         <v>4</v>
       </c>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="24"/>
-      <c r="AE6" s="298"/>
-      <c r="AF6" s="25"/>
-      <c r="AH6" s="24"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="24"/>
+      <c r="AF6" s="298"/>
+      <c r="AG6" s="25"/>
+      <c r="AI6" s="24"/>
     </row>
-    <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="29">
         <v>0</v>
+      </c>
+      <c r="C7">
+        <v>52</v>
       </c>
       <c r="E7" s="165"/>
       <c r="F7" s="242">
         <v>10</v>
       </c>
-      <c r="G7" s="177"/>
-      <c r="H7" s="9" t="s">
+      <c r="G7" s="177">
+        <v>50</v>
+      </c>
+      <c r="H7" s="177"/>
+      <c r="I7" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="I7" s="104" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="83" t="s">
+      <c r="J7" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="169" t="s">
+      <c r="L7" s="169" t="s">
         <v>293</v>
       </c>
-      <c r="L7" s="83" t="s">
+      <c r="M7" s="83" t="s">
         <v>139</v>
       </c>
-      <c r="M7" s="83" t="s">
+      <c r="N7" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="N7" s="143" t="s">
+      <c r="O7" s="143" t="s">
         <v>192</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="37" t="s">
+      <c r="Q7" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="Q7" s="154">
+      <c r="R7" s="154">
         <v>0.98263888888888884</v>
       </c>
-      <c r="S7" s="154">
+      <c r="T7" s="154">
         <v>0.73263888888888884</v>
       </c>
-      <c r="U7" s="245">
+      <c r="V7" s="245">
         <v>45294</v>
       </c>
-      <c r="Y7" s="25" t="s">
+      <c r="Z7" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z7" s="169" t="s">
+      <c r="AA7" s="169" t="s">
         <v>217</v>
       </c>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="24"/>
-      <c r="AE7" s="298"/>
-      <c r="AF7" s="25"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="24"/>
+      <c r="AF7" s="298"/>
       <c r="AG7" s="25"/>
-      <c r="AH7" s="24" t="s">
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>195</v>
+      </c>
       <c r="E8" s="219"/>
       <c r="F8" s="242">
         <v>25</v>
       </c>
-      <c r="G8" s="190"/>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="352">
+        <v>10</v>
+      </c>
+      <c r="H8" s="352"/>
+      <c r="I8" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="213"/>
-      <c r="K8" s="275" t="s">
+      <c r="J8" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="213"/>
+      <c r="L8" s="274" t="s">
         <v>300</v>
       </c>
-      <c r="L8" s="83" t="s">
+      <c r="M8" s="83" t="s">
         <v>214</v>
       </c>
-      <c r="M8" s="83" t="s">
+      <c r="N8" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="187" t="s">
+      <c r="O8" s="187" t="s">
         <v>196</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="P8" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="P8" s="188" t="s">
+      <c r="Q8" s="188" t="s">
         <v>65</v>
       </c>
-      <c r="Q8" s="154">
+      <c r="R8" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="S8" s="154">
+      <c r="T8" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="T8" s="274">
+      <c r="U8" s="273">
         <v>1</v>
       </c>
-      <c r="U8" s="245">
+      <c r="V8" s="245">
         <v>45295</v>
       </c>
-      <c r="Y8" s="25" t="s">
+      <c r="Z8" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z8" s="169" t="s">
+      <c r="AA8" s="169" t="s">
         <v>228</v>
       </c>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="24"/>
-      <c r="AE8" s="298"/>
-      <c r="AF8" s="25"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="24"/>
+      <c r="AF8" s="298"/>
       <c r="AG8" s="25"/>
-      <c r="AH8" s="24" t="s">
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>11368</v>
+        <v>11643</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="165">
         <v>14</v>
       </c>
-      <c r="G9" s="177"/>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="352">
+        <v>10</v>
+      </c>
+      <c r="H9" s="352"/>
+      <c r="I9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I9" s="104" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="213" t="s">
+      <c r="J9" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K9" s="169" t="s">
+      <c r="L9" s="169" t="s">
         <v>273</v>
       </c>
-      <c r="L9" s="223" t="s">
+      <c r="M9" s="223" t="s">
         <v>163</v>
       </c>
-      <c r="M9" s="224" t="s">
+      <c r="N9" s="224" t="s">
         <v>170</v>
       </c>
-      <c r="N9" s="143" t="s">
+      <c r="O9" s="143" t="s">
         <v>191</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="P9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="P9" s="37" t="s">
+      <c r="Q9" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="154">
+      <c r="R9" s="154">
         <v>0.73263888888888884</v>
       </c>
-      <c r="S9" s="154">
+      <c r="T9" s="154">
         <v>0.64583333333333337</v>
       </c>
-      <c r="U9" s="245">
+      <c r="V9" s="245">
         <v>45294</v>
       </c>
-      <c r="Y9" s="25" t="s">
+      <c r="Z9" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="Z9" s="169" t="s">
+      <c r="AA9" s="169" t="s">
         <v>229</v>
       </c>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="15"/>
-      <c r="AC9" s="24">
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="24">
         <v>1</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>1</v>
       </c>
-      <c r="AE9" s="298"/>
-      <c r="AF9" s="25" t="s">
+      <c r="AF9" s="298"/>
+      <c r="AG9" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="AG9" s="26" t="s">
+      <c r="AH9" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="AH9" s="24" t="s">
+      <c r="AI9" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="220">
         <v>8</v>
       </c>
@@ -3742,70 +3796,73 @@
       <c r="G10" s="177">
         <v>10</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="177">
+        <v>70</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="213" t="s">
+      <c r="J10" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="213" t="s">
         <v>294</v>
       </c>
-      <c r="K10" s="194" t="s">
+      <c r="L10" s="194" t="s">
         <v>242</v>
       </c>
-      <c r="L10" s="83" t="s">
+      <c r="M10" s="83" t="s">
         <v>143</v>
       </c>
-      <c r="M10" s="225" t="s">
+      <c r="N10" s="225" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="144" t="s">
+      <c r="O10" s="144" t="s">
         <v>122</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="P10" s="37" t="s">
+      <c r="Q10" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="Q10" s="154">
+      <c r="R10" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S10" s="154">
+      <c r="T10" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="U10" s="245">
+      <c r="V10" s="245">
         <v>45295</v>
       </c>
-      <c r="X10" s="216"/>
-      <c r="Y10" s="25" t="s">
+      <c r="Y10" s="216"/>
+      <c r="Z10" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="Z10" s="169" t="s">
+      <c r="AA10" s="169" t="s">
         <v>232</v>
       </c>
-      <c r="AB10" s="15">
+      <c r="AC10" s="15">
         <v>1</v>
       </c>
-      <c r="AC10" s="24"/>
-      <c r="AE10" s="298"/>
-      <c r="AF10" s="25"/>
+      <c r="AD10" s="24"/>
+      <c r="AF10" s="298"/>
       <c r="AG10" s="25"/>
-      <c r="AH10" s="24">
+      <c r="AH10" s="25"/>
+      <c r="AI10" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="8">
         <f>B9-B13</f>
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="E11" s="221"/>
       <c r="F11" s="242">
@@ -3814,69 +3871,70 @@
       <c r="G11" s="37">
         <v>5</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="37"/>
+      <c r="I11" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="213" t="s">
+      <c r="J11" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="213" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="169" t="s">
+      <c r="L11" s="169" t="s">
         <v>282</v>
       </c>
-      <c r="L11" s="83" t="s">
+      <c r="M11" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="M11" s="83" t="s">
+      <c r="N11" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="N11" s="186" t="s">
+      <c r="O11" s="186" t="s">
         <v>110</v>
       </c>
-      <c r="O11" s="41" t="s">
+      <c r="P11" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="P11" s="198" t="s">
+      <c r="Q11" s="198" t="s">
         <v>161</v>
       </c>
-      <c r="Q11" s="154">
+      <c r="R11" s="154">
         <v>0.83333333333333337</v>
       </c>
-      <c r="S11" s="154">
+      <c r="T11" s="154">
         <v>0.83333333333333337</v>
       </c>
-      <c r="U11" s="245">
+      <c r="V11" s="245">
         <v>45294</v>
       </c>
-      <c r="Y11" s="25" t="s">
+      <c r="Z11" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="Z11" s="169" t="s">
+      <c r="AA11" s="169" t="s">
         <v>233</v>
       </c>
-      <c r="AB11" s="15">
+      <c r="AC11" s="15">
         <v>1</v>
       </c>
-      <c r="AC11" s="24">
+      <c r="AD11" s="24">
         <v>1</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>2</v>
       </c>
-      <c r="AE11" s="298"/>
-      <c r="AF11" s="25" t="s">
+      <c r="AF11" s="298"/>
+      <c r="AG11" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="AG11" s="25" t="s">
+      <c r="AH11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="AH11" s="24" t="s">
+      <c r="AI11" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="165">
         <v>15</v>
       </c>
@@ -3886,69 +3944,70 @@
       <c r="G12" s="164">
         <v>100</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="164"/>
+      <c r="I12" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="I12" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="213"/>
-      <c r="K12" s="169" t="s">
+      <c r="J12" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="213"/>
+      <c r="L12" s="169" t="s">
         <v>222</v>
       </c>
-      <c r="L12" s="224" t="s">
+      <c r="M12" s="224" t="s">
         <v>123</v>
       </c>
-      <c r="M12" s="225" t="s">
+      <c r="N12" s="225" t="s">
         <v>62</v>
       </c>
-      <c r="N12" s="143" t="s">
+      <c r="O12" s="143" t="s">
         <v>197</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="188" t="s">
+      <c r="Q12" s="188" t="s">
         <v>181</v>
       </c>
-      <c r="Q12" s="154">
+      <c r="R12" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="R12" s="24"/>
-      <c r="S12" s="154">
+      <c r="S12" s="24"/>
+      <c r="T12" s="154">
         <v>0.83680555555555547</v>
       </c>
-      <c r="U12" s="245">
+      <c r="V12" s="245">
         <v>45294</v>
       </c>
-      <c r="Y12" s="25" t="s">
+      <c r="Z12" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z12" s="169" t="s">
+      <c r="AA12" s="169" t="s">
         <v>234</v>
       </c>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="272">
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="271">
         <v>1</v>
       </c>
-      <c r="AE12" s="298"/>
-      <c r="AF12" s="25" t="s">
+      <c r="AF12" s="298"/>
+      <c r="AG12" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="AG12" s="25" t="s">
+      <c r="AH12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AH12" s="24" t="s">
+      <c r="AI12" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>11368</v>
+        <v>11673</v>
       </c>
       <c r="E13" s="36">
         <v>5</v>
@@ -3956,122 +4015,128 @@
       <c r="F13" s="206">
         <v>1</v>
       </c>
-      <c r="G13" s="246"/>
-      <c r="H13" s="9" t="s">
+      <c r="G13" s="246">
+        <v>35</v>
+      </c>
+      <c r="H13" s="246">
+        <v>10</v>
+      </c>
+      <c r="I13" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="I13" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="228" t="s">
-        <v>311</v>
-      </c>
-      <c r="K13" s="194" t="s">
+      <c r="J13" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="228" t="s">
+        <v>314</v>
+      </c>
+      <c r="L13" s="194" t="s">
         <v>242</v>
       </c>
-      <c r="L13" s="183" t="s">
+      <c r="M13" s="183" t="s">
         <v>155</v>
       </c>
-      <c r="M13" s="183" t="s">
+      <c r="N13" s="183" t="s">
         <v>85</v>
       </c>
-      <c r="N13" s="41" t="s">
+      <c r="O13" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="O13" s="41" t="s">
+      <c r="P13" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="P13" s="229" t="s">
+      <c r="Q13" s="229" t="s">
         <v>90</v>
       </c>
-      <c r="Q13" s="154">
+      <c r="R13" s="154">
         <v>0.53125</v>
       </c>
-      <c r="R13"/>
-      <c r="S13" s="154">
+      <c r="S13"/>
+      <c r="T13" s="154">
         <v>0.53125</v>
       </c>
-      <c r="T13" s="261">
+      <c r="U13" s="261">
         <v>1</v>
       </c>
-      <c r="U13" s="245">
+      <c r="V13" s="245">
         <v>45294</v>
       </c>
-      <c r="Y13" s="25" t="s">
+      <c r="Z13" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z13" s="169" t="s">
+      <c r="AA13" s="169" t="s">
         <v>235</v>
       </c>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="24"/>
-      <c r="AE13" s="298"/>
-      <c r="AF13" s="25"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="24"/>
+      <c r="AF13" s="298"/>
       <c r="AG13" s="25"/>
-      <c r="AH13" s="24"/>
+      <c r="AH13" s="25"/>
+      <c r="AI13" s="24"/>
     </row>
-    <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="165"/>
       <c r="F14" s="205"/>
       <c r="G14" s="127"/>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="127"/>
+      <c r="I14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="213"/>
-      <c r="K14" s="169"/>
-      <c r="L14" s="83" t="s">
+      <c r="J14" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="213"/>
+      <c r="L14" s="169"/>
+      <c r="M14" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="M14" s="224" t="s">
+      <c r="N14" s="224" t="s">
         <v>62</v>
       </c>
-      <c r="N14" s="143" t="s">
+      <c r="O14" s="143" t="s">
         <v>200</v>
       </c>
-      <c r="O14" s="169" t="s">
+      <c r="P14" s="169" t="s">
         <v>47</v>
       </c>
-      <c r="P14" s="37" t="s">
+      <c r="Q14" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="Q14" s="154">
+      <c r="R14" s="154">
         <v>0.73263888888888884</v>
       </c>
-      <c r="R14"/>
-      <c r="S14" s="154">
+      <c r="S14"/>
+      <c r="T14" s="154">
         <v>0.94097222222222221</v>
       </c>
-      <c r="U14" s="245">
+      <c r="V14" s="245">
         <v>45294</v>
       </c>
-      <c r="X14" s="25" t="s">
+      <c r="Y14" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="Y14" s="25" t="s">
+      <c r="Z14" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="Z14" s="169" t="s">
+      <c r="AA14" s="169" t="s">
         <v>237</v>
       </c>
-      <c r="AA14" s="239">
+      <c r="AB14" s="239">
         <v>1</v>
       </c>
-      <c r="AC14" s="241">
+      <c r="AD14" s="241">
         <v>1</v>
       </c>
-      <c r="AE14" s="298"/>
-      <c r="AF14" s="25"/>
+      <c r="AF14" s="298"/>
       <c r="AG14" s="25"/>
-      <c r="AH14" s="24" t="s">
+      <c r="AH14" s="25"/>
+      <c r="AI14" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>2</v>
       </c>
@@ -4083,135 +4148,143 @@
       <c r="E15" s="165"/>
       <c r="F15" s="34"/>
       <c r="G15" s="177"/>
-      <c r="H15" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="I15" s="107" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="231"/>
-      <c r="K15" s="169"/>
-      <c r="L15" s="83" t="s">
-        <v>176</v>
-      </c>
-      <c r="M15" s="233"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="154">
+      <c r="H15" s="177"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="231"/>
+      <c r="L15" s="169"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="233"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="154">
         <v>0.88611111111111107</v>
       </c>
-      <c r="R15"/>
-      <c r="S15" s="154">
+      <c r="S15"/>
+      <c r="T15" s="154">
         <v>0.88611111111111107</v>
       </c>
-      <c r="U15" s="245">
+      <c r="V15" s="245">
         <v>45293</v>
       </c>
-      <c r="Y15" s="25" t="s">
+      <c r="Z15" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="Z15" s="169" t="s">
+      <c r="AA15" s="169" t="s">
         <v>238</v>
       </c>
-      <c r="AB15" s="15">
+      <c r="AC15" s="15">
         <v>1</v>
       </c>
-      <c r="AC15" s="36">
+      <c r="AD15" s="36">
         <v>1</v>
       </c>
-      <c r="AD15">
+      <c r="AE15">
         <v>1</v>
       </c>
-      <c r="AE15" s="298"/>
-      <c r="AF15" s="25" t="s">
+      <c r="AF15" s="298"/>
+      <c r="AG15" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="AG15" s="26" t="s">
+      <c r="AH15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="AH15" s="24" t="s">
+      <c r="AI15" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
-      <c r="I16" s="234"/>
-      <c r="J16" s="119"/>
-      <c r="K16" s="216"/>
-      <c r="L16" s="119"/>
-      <c r="X16" s="216" t="s">
+      <c r="J16" s="234"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="216"/>
+      <c r="M16" s="119"/>
+      <c r="Y16" s="216" t="s">
         <v>287</v>
       </c>
-      <c r="Y16" s="25" t="s">
+      <c r="Z16" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z16" s="169" t="s">
+      <c r="AA16" s="169" t="s">
         <v>239</v>
       </c>
-      <c r="AC16" s="24"/>
-      <c r="AE16" s="298"/>
-      <c r="AF16" s="25"/>
-      <c r="AH16" s="24"/>
+      <c r="AD16" s="24"/>
+      <c r="AF16" s="298"/>
+      <c r="AG16" s="25"/>
+      <c r="AI16" s="24"/>
     </row>
-    <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="287" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="288"/>
-      <c r="G17" s="189"/>
-      <c r="H17" s="9">
+      <c r="E17" s="34">
+        <f>SUM(E4:E15)</f>
+        <v>63</v>
+      </c>
+      <c r="F17" s="34">
+        <f>SUM(F4:F15)</f>
+        <v>133</v>
+      </c>
+      <c r="G17" s="34">
+        <f>SUM(G4:G15)</f>
+        <v>230</v>
+      </c>
+      <c r="H17" s="189">
+        <f>SUM(H4:H15)</f>
+        <v>160</v>
+      </c>
+      <c r="I17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>311</v>
-      </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="262"/>
-      <c r="K17" s="169" t="s">
+        <v>426</v>
+      </c>
+      <c r="J17" s="26"/>
+      <c r="K17" s="262"/>
+      <c r="L17" s="169" t="s">
         <v>273</v>
       </c>
-      <c r="L17" s="254"/>
-      <c r="N17" s="277" t="s">
+      <c r="M17" s="254"/>
+      <c r="O17" s="276" t="s">
         <v>276</v>
       </c>
-      <c r="O17" s="82"/>
-      <c r="P17" s="349" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q17" s="273" t="s">
+      <c r="P17" s="82"/>
+      <c r="Q17" s="280" t="s">
+        <v>315</v>
+      </c>
+      <c r="R17" s="272" t="s">
         <v>271</v>
       </c>
-      <c r="R17" s="282"/>
-      <c r="S17" s="266" t="s">
+      <c r="S17" s="284"/>
+      <c r="T17" s="265" t="s">
         <v>284</v>
       </c>
-      <c r="V17" s="259"/>
-      <c r="Y17" s="25" t="s">
+      <c r="W17" s="259"/>
+      <c r="Z17" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z17" s="169" t="s">
+      <c r="AA17" s="169" t="s">
         <v>240</v>
       </c>
-      <c r="AA17" s="50"/>
-      <c r="AB17" s="15"/>
-      <c r="AC17" s="115"/>
-      <c r="AD17" s="50">
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="115"/>
+      <c r="AE17" s="50">
         <v>2</v>
       </c>
-      <c r="AE17" s="298"/>
-      <c r="AF17" s="25" t="s">
+      <c r="AF17" s="298"/>
+      <c r="AG17" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="AG17" s="25" t="s">
+      <c r="AH17" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AH17" s="24" t="s">
+      <c r="AI17" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -4220,354 +4293,377 @@
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
+      <c r="E18" s="289" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="290"/>
       <c r="G18" s="20"/>
-      <c r="I18" s="226"/>
-      <c r="J18" s="262"/>
-      <c r="K18" s="194" t="s">
+      <c r="H18" s="20"/>
+      <c r="J18" s="226"/>
+      <c r="K18" s="262"/>
+      <c r="L18" s="194" t="s">
         <v>269</v>
       </c>
-      <c r="L18" s="345"/>
-      <c r="M18" s="347" t="s">
-        <v>315</v>
-      </c>
-      <c r="N18" s="350" t="s">
+      <c r="M18" s="278"/>
+      <c r="N18" s="282" t="s">
+        <v>314</v>
+      </c>
+      <c r="O18" s="303" t="s">
         <v>306</v>
       </c>
-      <c r="O18" s="350"/>
-      <c r="P18" s="351"/>
-      <c r="Q18" s="161"/>
-      <c r="R18" s="282"/>
-      <c r="S18" s="17"/>
-      <c r="X18" s="25" t="s">
+      <c r="P18" s="303"/>
+      <c r="Q18" s="304"/>
+      <c r="R18" s="161"/>
+      <c r="S18" s="284"/>
+      <c r="T18" s="17"/>
+      <c r="Y18" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="Y18" s="25" t="s">
+      <c r="Z18" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z18" s="169" t="s">
+      <c r="AA18" s="169" t="s">
         <v>254</v>
       </c>
-      <c r="AC18" s="24"/>
-      <c r="AE18" s="298"/>
-      <c r="AF18" s="25"/>
+      <c r="AD18" s="24"/>
+      <c r="AF18" s="298"/>
       <c r="AG18" s="25"/>
-      <c r="AH18" s="24" t="s">
+      <c r="AH18" s="25"/>
+      <c r="AI18" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H19" s="1"/>
-      <c r="I19" s="226"/>
-      <c r="K19" s="169" t="s">
+    <row r="19" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="354">
+        <v>35</v>
+      </c>
+      <c r="F19" s="59">
+        <v>40</v>
+      </c>
+      <c r="G19" s="355">
+        <v>100</v>
+      </c>
+      <c r="H19" s="357"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="226"/>
+      <c r="L19" s="169" t="s">
         <v>288</v>
       </c>
-      <c r="L19" s="119"/>
-      <c r="M19" s="348"/>
-      <c r="N19" s="346" t="s">
+      <c r="M19" s="119"/>
+      <c r="N19" s="283"/>
+      <c r="O19" s="279" t="s">
+        <v>312</v>
+      </c>
+      <c r="P19" s="294" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q19" s="294"/>
+      <c r="R19" s="295" t="s">
+        <v>277</v>
+      </c>
+      <c r="S19" s="295"/>
+      <c r="T19" s="17"/>
+      <c r="Z19" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA19" s="169" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB19" s="50"/>
+      <c r="AC19" s="79"/>
+      <c r="AD19" s="115"/>
+      <c r="AE19" s="50"/>
+      <c r="AF19" s="298"/>
+      <c r="AG19" s="25"/>
+      <c r="AH19" s="25"/>
+      <c r="AI19" s="24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="359" t="s">
+        <v>316</v>
+      </c>
+      <c r="B20" s="29">
+        <v>30</v>
+      </c>
+      <c r="E20" s="236">
+        <v>30</v>
+      </c>
+      <c r="F20" s="65">
+        <v>70</v>
+      </c>
+      <c r="G20" s="356"/>
+      <c r="H20" s="357"/>
+      <c r="J20" s="227"/>
+      <c r="L20" s="169" t="s">
+        <v>272</v>
+      </c>
+      <c r="M20" s="119"/>
+      <c r="N20" s="231" t="s">
+        <v>314</v>
+      </c>
+      <c r="O20" s="277" t="s">
+        <v>310</v>
+      </c>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="264"/>
+      <c r="R20" s="159" t="s">
+        <v>279</v>
+      </c>
+      <c r="S20" s="17"/>
+      <c r="T20" s="265" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z20" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA20" s="169" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB20" s="255"/>
+      <c r="AC20" s="258"/>
+      <c r="AD20" s="257"/>
+      <c r="AE20" s="256"/>
+      <c r="AF20" s="298"/>
+      <c r="AG20" s="25"/>
+      <c r="AH20" s="25"/>
+      <c r="AI20" s="24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="169"/>
+      <c r="O21" s="272" t="s">
         <v>313</v>
       </c>
-      <c r="O19" s="294" t="s">
-        <v>290</v>
-      </c>
-      <c r="P19" s="294"/>
-      <c r="Q19" s="295" t="s">
-        <v>277</v>
-      </c>
-      <c r="R19" s="295"/>
-      <c r="S19" s="17"/>
-      <c r="Y19" s="25" t="s">
+      <c r="P21" s="296" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q21" s="296"/>
+      <c r="R21" s="266"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="265" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y21" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z21" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z19" s="169" t="s">
-        <v>255</v>
-      </c>
-      <c r="AA19" s="50"/>
-      <c r="AB19" s="79"/>
-      <c r="AC19" s="115"/>
-      <c r="AD19" s="50"/>
-      <c r="AE19" s="298"/>
-      <c r="AF19" s="25"/>
-      <c r="AG19" s="25"/>
-      <c r="AH19" s="24" t="s">
+      <c r="AA21" s="169" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB21" s="42"/>
+      <c r="AC21" s="15"/>
+      <c r="AD21" s="109">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="43">
+        <v>1</v>
+      </c>
+      <c r="AF21" s="298"/>
+      <c r="AG21" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH21" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI21" s="24" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="263"/>
-      <c r="B20" s="263"/>
-      <c r="I20" s="227"/>
-      <c r="K20" s="169" t="s">
-        <v>272</v>
-      </c>
-      <c r="L20" s="119"/>
-      <c r="M20" s="231" t="s">
-        <v>315</v>
-      </c>
-      <c r="N20" s="344" t="s">
-        <v>310</v>
-      </c>
-      <c r="O20" s="18"/>
-      <c r="P20" s="265"/>
-      <c r="Q20" s="159" t="s">
+    <row r="22" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="169" t="s">
+        <v>303</v>
+      </c>
+      <c r="T22" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y22" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="Z22" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA22" s="169" t="s">
+        <v>262</v>
+      </c>
+      <c r="AB22" s="48"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="24"/>
+      <c r="AF22" s="298"/>
+      <c r="AG22" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="AH22" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="AI22" s="24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="169" t="s">
+        <v>307</v>
+      </c>
+      <c r="Z23" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA23" s="169" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB23" s="63"/>
+      <c r="AC23" s="116"/>
+      <c r="AD23" s="115"/>
+      <c r="AE23" s="50"/>
+      <c r="AF23" s="298"/>
+      <c r="AG23" s="25"/>
+      <c r="AH23" s="25"/>
+      <c r="AI23" s="24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R24" s="300" t="s">
+        <v>302</v>
+      </c>
+      <c r="S24" s="265">
+        <v>3</v>
+      </c>
+      <c r="T24" s="275" t="s">
+        <v>305</v>
+      </c>
+      <c r="Z24" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA24" s="169" t="s">
+        <v>264</v>
+      </c>
+      <c r="AB24" s="255"/>
+      <c r="AC24" s="258"/>
+      <c r="AD24" s="257"/>
+      <c r="AE24" s="256"/>
+      <c r="AF24" s="298"/>
+      <c r="AG24" s="25"/>
+      <c r="AH24" s="25"/>
+      <c r="AI24" s="24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="25">
+        <v>2</v>
+      </c>
+      <c r="K25" s="231" t="s">
+        <v>309</v>
+      </c>
+      <c r="M25" s="231" t="s">
+        <v>308</v>
+      </c>
+      <c r="R25" s="301"/>
+      <c r="S25" s="265">
+        <v>1</v>
+      </c>
+      <c r="T25" s="275" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y25" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="Z25" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="AA25" s="169" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB25" s="255"/>
+      <c r="AC25" s="258"/>
+      <c r="AD25" s="257"/>
+      <c r="AE25" s="256"/>
+      <c r="AF25" s="298"/>
+      <c r="AG25" s="25"/>
+      <c r="AH25" s="25"/>
+      <c r="AI25" s="24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L26" s="169" t="s">
+        <v>289</v>
+      </c>
+      <c r="R26" s="302"/>
+      <c r="S26" s="265">
+        <v>1</v>
+      </c>
+      <c r="T26" s="275" t="s">
         <v>279</v>
       </c>
-      <c r="R20" s="17"/>
-      <c r="S20" s="266" t="s">
-        <v>285</v>
-      </c>
-      <c r="Y20" s="25" t="s">
+      <c r="Z26" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z20" s="169" t="s">
+      <c r="AA26" s="169" t="s">
         <v>260</v>
       </c>
-      <c r="AA20" s="255"/>
-      <c r="AB20" s="258"/>
-      <c r="AC20" s="257"/>
-      <c r="AD20" s="256"/>
-      <c r="AE20" s="298"/>
-      <c r="AF20" s="25"/>
-      <c r="AG20" s="25"/>
-      <c r="AH20" s="24" t="s">
-        <v>246</v>
-      </c>
+      <c r="AF26" s="298"/>
     </row>
-    <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K21" s="169" t="s">
-        <v>303</v>
-      </c>
-      <c r="N21" s="273" t="s">
-        <v>314</v>
-      </c>
-      <c r="O21" s="296" t="s">
-        <v>291</v>
-      </c>
-      <c r="P21" s="296"/>
-      <c r="Q21" s="267"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="266" t="s">
-        <v>285</v>
-      </c>
-      <c r="X21" s="25" t="s">
+    <row r="27" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="25">
+        <v>1</v>
+      </c>
+      <c r="K27" s="231" t="s">
+        <v>309</v>
+      </c>
+      <c r="M27" s="233"/>
+      <c r="Y27" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="Y21" s="25" t="s">
+      <c r="Z27" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="Z21" s="169" t="s">
-        <v>261</v>
-      </c>
-      <c r="AA21" s="42"/>
-      <c r="AB21" s="15"/>
-      <c r="AC21" s="109">
+      <c r="AA27" s="169" t="s">
+        <v>295</v>
+      </c>
+      <c r="AF27" s="298"/>
+    </row>
+    <row r="28" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA28" s="169" t="s">
+        <v>297</v>
+      </c>
+      <c r="AC28" s="15">
+        <v>2</v>
+      </c>
+      <c r="AE28">
         <v>1</v>
       </c>
-      <c r="AD21" s="43">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="298"/>
-      <c r="AF21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG21" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH21" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K22" s="169" t="s">
-        <v>303</v>
-      </c>
-      <c r="S22" s="24" t="s">
-        <v>278</v>
-      </c>
-      <c r="X22" s="25" t="s">
-        <v>296</v>
-      </c>
-      <c r="Y22" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="Z22" s="169" t="s">
-        <v>262</v>
-      </c>
-      <c r="AA22" s="48"/>
-      <c r="AB22" s="15"/>
-      <c r="AC22" s="24"/>
-      <c r="AE22" s="298"/>
-      <c r="AF22" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="AG22" s="25" t="s">
-        <v>299</v>
-      </c>
-      <c r="AH22" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K23" s="169" t="s">
-        <v>307</v>
-      </c>
-      <c r="Y23" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="Z23" s="169" t="s">
-        <v>263</v>
-      </c>
-      <c r="AA23" s="63"/>
-      <c r="AB23" s="116"/>
-      <c r="AC23" s="115"/>
-      <c r="AD23" s="50"/>
-      <c r="AE23" s="298"/>
-      <c r="AF23" s="25"/>
-      <c r="AG23" s="25"/>
-      <c r="AH23" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q24" s="300" t="s">
-        <v>302</v>
-      </c>
-      <c r="R24" s="266">
-        <v>3</v>
-      </c>
-      <c r="S24" s="276" t="s">
-        <v>305</v>
-      </c>
-      <c r="Y24" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="Z24" s="169" t="s">
-        <v>264</v>
-      </c>
-      <c r="AA24" s="255"/>
-      <c r="AB24" s="258"/>
-      <c r="AC24" s="257"/>
-      <c r="AD24" s="256"/>
-      <c r="AE24" s="298"/>
-      <c r="AF24" s="25"/>
-      <c r="AG24" s="25"/>
-      <c r="AH24" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I25" s="25">
-        <v>2</v>
-      </c>
-      <c r="J25" s="231" t="s">
-        <v>309</v>
-      </c>
-      <c r="L25" s="231" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q25" s="301"/>
-      <c r="R25" s="266">
-        <v>1</v>
-      </c>
-      <c r="S25" s="276" t="s">
-        <v>304</v>
-      </c>
-      <c r="X25" s="25" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y25" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="Z25" s="169" t="s">
-        <v>265</v>
-      </c>
-      <c r="AA25" s="255"/>
-      <c r="AB25" s="258"/>
-      <c r="AC25" s="257"/>
-      <c r="AD25" s="256"/>
-      <c r="AE25" s="298"/>
-      <c r="AF25" s="25"/>
-      <c r="AG25" s="25"/>
-      <c r="AH25" s="24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K26" s="169" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q26" s="302"/>
-      <c r="R26" s="266">
-        <v>1</v>
-      </c>
-      <c r="S26" s="276" t="s">
-        <v>279</v>
-      </c>
-      <c r="Y26" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="Z26" s="169" t="s">
-        <v>260</v>
-      </c>
-      <c r="AE26" s="298"/>
-    </row>
-    <row r="27" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="25">
-        <v>1</v>
-      </c>
-      <c r="J27" s="231" t="s">
-        <v>309</v>
-      </c>
-      <c r="L27" s="233"/>
-      <c r="X27" s="25" t="s">
-        <v>279</v>
-      </c>
-      <c r="Y27" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="Z27" s="169" t="s">
-        <v>295</v>
-      </c>
-      <c r="AE27" s="298"/>
-    </row>
-    <row r="28" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z28" s="169" t="s">
-        <v>297</v>
-      </c>
-      <c r="AB28" s="15">
-        <v>2</v>
-      </c>
-      <c r="AD28">
-        <v>1</v>
-      </c>
-      <c r="AE28" s="299"/>
-      <c r="AF28" s="25" t="s">
+      <c r="AF28" s="299"/>
+      <c r="AG28" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="AG28" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="AH28" s="1">
+      <c r="AH28" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="AI28" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="AE3:AE28"/>
-    <mergeCell ref="Q24:Q26"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="AF3:AF28"/>
+    <mergeCell ref="R24:R26"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="S17:S18"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:S19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4664,10 +4760,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:T65"/>
+  <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4691,18 +4787,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="319" t="s">
+      <c r="E1" s="326" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="321"/>
+      <c r="F1" s="328"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="319" t="s">
+      <c r="H1" s="326" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="320"/>
-      <c r="J1" s="321"/>
+      <c r="I1" s="327"/>
+      <c r="J1" s="328"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4720,7 +4816,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="322">
+      <c r="B2" s="329">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4747,26 +4843,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="325">
+      <c r="K2" s="332">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="314">
+      <c r="L2" s="321">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="306">
+      <c r="M2" s="313">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J65)</f>
-        <v>11328</v>
+        <f>SUM(E2:J67)</f>
+        <v>11633</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="323"/>
+      <c r="B3" s="330"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4781,13 +4877,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="326"/>
-      <c r="L3" s="282"/>
-      <c r="M3" s="307"/>
+      <c r="K3" s="333"/>
+      <c r="L3" s="284"/>
+      <c r="M3" s="314"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="324"/>
+      <c r="B4" s="331"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4802,9 +4898,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="326"/>
-      <c r="L4" s="282"/>
-      <c r="M4" s="307"/>
+      <c r="K4" s="333"/>
+      <c r="L4" s="284"/>
+      <c r="M4" s="314"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4886,7 +4982,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="303">
+      <c r="B7" s="310">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4903,22 +4999,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="308">
+      <c r="K7" s="315">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="310">
+      <c r="L7" s="317">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="312">
+      <c r="M7" s="319">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="305"/>
+      <c r="B8" s="312"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4939,9 +5035,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="309"/>
-      <c r="L8" s="311"/>
-      <c r="M8" s="313"/>
+      <c r="K8" s="316"/>
+      <c r="L8" s="318"/>
+      <c r="M8" s="320"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -5021,7 +5117,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="303">
+      <c r="B11" s="310">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -5048,7 +5144,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="305"/>
+      <c r="B12" s="312"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -5105,7 +5201,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="303">
+      <c r="B14" s="310">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -5128,7 +5224,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="305"/>
+      <c r="B15" s="312"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -5152,7 +5248,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="322">
+      <c r="B16" s="329">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -5183,7 +5279,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="323"/>
+      <c r="B17" s="330"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -5201,7 +5297,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="322">
+      <c r="B18" s="329">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -5230,7 +5326,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="324"/>
+      <c r="B19" s="331"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -5290,7 +5386,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="327">
+      <c r="B21" s="334">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -5318,7 +5414,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="328"/>
+      <c r="B22" s="335"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -5370,7 +5466,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="285">
+      <c r="B24" s="287">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -5399,7 +5495,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="286"/>
+      <c r="B25" s="288"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -5427,7 +5523,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="285">
+      <c r="B26" s="287">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -5458,7 +5554,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="318"/>
+      <c r="B27" s="325"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5489,7 +5585,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="285">
+      <c r="B28" s="287">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -5511,7 +5607,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="286"/>
+      <c r="B29" s="288"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -5537,7 +5633,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="285">
+      <c r="B30" s="287">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -5560,7 +5656,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="286"/>
+      <c r="B31" s="288"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -5587,7 +5683,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="285">
+      <c r="B32" s="287">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -5609,7 +5705,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="286"/>
+      <c r="B33" s="288"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -5662,7 +5758,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="285">
+      <c r="B35" s="287">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -5689,7 +5785,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="286"/>
+      <c r="B36" s="288"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -5711,7 +5807,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="285">
+      <c r="B37" s="287">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -5744,7 +5840,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="286"/>
+      <c r="B38" s="288"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -5762,7 +5858,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="285">
+      <c r="B39" s="287">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -5789,7 +5885,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="318"/>
+      <c r="B40" s="325"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5817,7 +5913,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="285">
+      <c r="B41" s="287">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -5844,7 +5940,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="318"/>
+      <c r="B42" s="325"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5862,7 +5958,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="286"/>
+      <c r="B43" s="288"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -5891,7 +5987,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="285">
+      <c r="B44" s="287">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -5917,7 +6013,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="286"/>
+      <c r="B45" s="288"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -5942,7 +6038,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="285">
+      <c r="B46" s="287">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -5964,7 +6060,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="318"/>
+      <c r="B47" s="325"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -5985,7 +6081,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="285">
+      <c r="B48" s="287">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -6005,7 +6101,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="318"/>
+      <c r="B49" s="325"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -6031,7 +6127,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="318"/>
+      <c r="B50" s="325"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -6058,7 +6154,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="285">
+      <c r="B51" s="287">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -6080,7 +6176,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="286"/>
+      <c r="B52" s="288"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -6113,7 +6209,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="285">
+      <c r="B53" s="287">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -6143,7 +6239,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="318"/>
+      <c r="B54" s="325"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -6170,7 +6266,7 @@
       <c r="A55" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="285">
+      <c r="B55" s="287">
         <v>31</v>
       </c>
       <c r="C55" s="96"/>
@@ -6198,7 +6294,7 @@
       <c r="M55" s="82"/>
     </row>
     <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="286"/>
+      <c r="B56" s="288"/>
       <c r="C56" s="96"/>
       <c r="D56" s="82"/>
       <c r="E56" s="82">
@@ -6224,7 +6320,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="315">
+      <c r="B57" s="322">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -6244,7 +6340,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="316"/>
+      <c r="B58" s="323"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -6273,7 +6369,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="317"/>
+      <c r="B59" s="324"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -6299,7 +6395,7 @@
       <c r="M59" s="18"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="285">
+      <c r="B60" s="287">
         <v>2</v>
       </c>
       <c r="C60" s="142"/>
@@ -6325,7 +6421,7 @@
       <c r="M60" s="18"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="318"/>
+      <c r="B61" s="325"/>
       <c r="C61" s="142"/>
       <c r="D61" s="18">
         <v>240</v>
@@ -6351,7 +6447,7 @@
       <c r="M61" s="18"/>
     </row>
     <row r="62" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="286"/>
+      <c r="B62" s="288"/>
       <c r="C62" s="142"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
@@ -6372,7 +6468,7 @@
       <c r="A63" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="303">
+      <c r="B63" s="310">
         <v>3</v>
       </c>
       <c r="C63" s="142"/>
@@ -6394,7 +6490,7 @@
       <c r="M63" s="18"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="304"/>
+      <c r="B64" s="311"/>
       <c r="C64" s="142"/>
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
@@ -6413,8 +6509,8 @@
       <c r="L64" s="18"/>
       <c r="M64" s="18"/>
     </row>
-    <row r="65" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="305"/>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B65" s="311"/>
       <c r="C65" s="142"/>
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
@@ -6435,8 +6531,53 @@
       <c r="L65" s="18"/>
       <c r="M65" s="18"/>
     </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B66" s="311"/>
+      <c r="C66" s="142"/>
+      <c r="D66" s="18">
+        <v>500</v>
+      </c>
+      <c r="E66" s="18">
+        <v>35</v>
+      </c>
+      <c r="F66" s="18">
+        <v>50</v>
+      </c>
+      <c r="G66" s="358">
+        <v>70</v>
+      </c>
+      <c r="H66" s="18">
+        <v>30</v>
+      </c>
+      <c r="I66" s="18">
+        <v>30</v>
+      </c>
+      <c r="J66" s="358">
+        <v>60</v>
+      </c>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="18"/>
+    </row>
+    <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="312"/>
+      <c r="C67" s="142"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="358">
+        <v>30</v>
+      </c>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B63:B67"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B41:B43"/>
@@ -6454,7 +6595,6 @@
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B63:B65"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B11:B12"/>
@@ -9676,10 +9816,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="287" t="s">
+      <c r="AG24" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="288"/>
+      <c r="AH24" s="290"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -9699,10 +9839,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="287" t="s">
+      <c r="AZ24" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="288"/>
+      <c r="BA24" s="290"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -9722,10 +9862,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="287" t="s">
+      <c r="BR24" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="288"/>
+      <c r="BS24" s="290"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -9748,10 +9888,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="289" t="s">
+      <c r="B26" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="291"/>
+      <c r="C26" s="293"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9788,10 +9928,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="289" t="s">
+      <c r="R26" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="291"/>
+      <c r="S26" s="293"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9828,10 +9968,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="289" t="s">
+      <c r="AG26" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="291"/>
+      <c r="AH26" s="293"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9868,10 +10008,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="289" t="s">
+      <c r="AW26" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="291"/>
+      <c r="AX26" s="293"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9908,10 +10048,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="289" t="s">
+      <c r="BM26" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="291"/>
+      <c r="BN26" s="293"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -10905,7 +11045,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="333">
+      <c r="AX32" s="341">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -10943,7 +11083,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="333">
+      <c r="BN32" s="341">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -11092,7 +11232,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="334"/>
+      <c r="AX33" s="342"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -11128,7 +11268,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="334"/>
+      <c r="BN33" s="342"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -11279,7 +11419,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="335"/>
+      <c r="AX34" s="343"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11317,7 +11457,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="335"/>
+      <c r="BN34" s="343"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11548,10 +11688,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="287" t="s">
+      <c r="B36" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="288"/>
+      <c r="C36" s="290"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -11569,10 +11709,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="287" t="s">
+      <c r="R36" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="288"/>
+      <c r="S36" s="290"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -11590,10 +11730,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="287" t="s">
+      <c r="AG36" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="288"/>
+      <c r="AH36" s="290"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -11611,10 +11751,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="287" t="s">
+      <c r="AW36" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="288"/>
+      <c r="AX36" s="290"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -11632,10 +11772,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="287" t="s">
+      <c r="BM36" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="288"/>
+      <c r="BN36" s="290"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -11655,10 +11795,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="289" t="s">
+      <c r="B38" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="291"/>
+      <c r="C38" s="293"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11698,10 +11838,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="289" t="s">
+      <c r="S38" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="291"/>
+      <c r="T38" s="293"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11741,11 +11881,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="289" t="s">
+      <c r="AJ38" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="290"/>
-      <c r="AL38" s="291"/>
+      <c r="AK38" s="292"/>
+      <c r="AL38" s="293"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11790,11 +11930,11 @@
         <f ca="1">TODAY()</f>
         <v>45294</v>
       </c>
-      <c r="BD38" s="289" t="s">
+      <c r="BD38" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="290"/>
-      <c r="BF38" s="291"/>
+      <c r="BE38" s="292"/>
+      <c r="BF38" s="293"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11834,11 +11974,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="289" t="s">
+      <c r="BW38" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="290"/>
-      <c r="BY38" s="291"/>
+      <c r="BX38" s="292"/>
+      <c r="BY38" s="293"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -12790,7 +12930,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="333">
+      <c r="C44" s="341">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12828,10 +12968,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="342">
+      <c r="S44" s="350">
         <v>25</v>
       </c>
-      <c r="T44" s="333">
+      <c r="T44" s="341">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12840,7 +12980,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="336" t="s">
+      <c r="W44" s="344" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12869,10 +13009,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="342">
+      <c r="AJ44" s="350">
         <v>50</v>
       </c>
-      <c r="AK44" s="333">
+      <c r="AK44" s="341">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12882,7 +13022,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="336" t="s">
+      <c r="AO44" s="344" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -12912,7 +13052,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="342">
+      <c r="BD44" s="350">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -12923,7 +13063,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="336" t="s">
+      <c r="BI44" s="344" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -12952,7 +13092,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="342">
+      <c r="BW44" s="350">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -12963,7 +13103,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="336" t="s">
+      <c r="CB44" s="344" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -12995,7 +13135,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="334"/>
+      <c r="C45" s="342"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -13029,15 +13169,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="343"/>
-      <c r="T45" s="335"/>
+      <c r="S45" s="351"/>
+      <c r="T45" s="343"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="337"/>
+      <c r="W45" s="345"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13064,8 +13204,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="343"/>
-      <c r="AK45" s="335"/>
+      <c r="AJ45" s="351"/>
+      <c r="AK45" s="343"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -13073,7 +13213,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="337"/>
+      <c r="AO45" s="345"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13101,7 +13241,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="343"/>
+      <c r="BD45" s="351"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -13112,7 +13252,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="337"/>
+      <c r="BI45" s="345"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13139,7 +13279,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="343"/>
+      <c r="BW45" s="351"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -13148,7 +13288,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="337"/>
+      <c r="CB45" s="345"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13178,7 +13318,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="335"/>
+      <c r="C46" s="343"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13605,10 +13745,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="287" t="s">
+      <c r="B48" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="288"/>
+      <c r="C48" s="290"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -13627,10 +13767,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="287" t="s">
+      <c r="S48" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="288"/>
+      <c r="T48" s="290"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -13783,11 +13923,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="338"/>
+      <c r="AQ49" s="346"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="330"/>
-      <c r="AV49" s="331"/>
+      <c r="AU49" s="338"/>
+      <c r="AV49" s="339"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -13799,11 +13939,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="338"/>
+      <c r="BK49" s="346"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="330"/>
-      <c r="BP49" s="331"/>
+      <c r="BO49" s="338"/>
+      <c r="BP49" s="339"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -13814,20 +13954,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="338"/>
+      <c r="CD49" s="346"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="330"/>
-      <c r="CI49" s="331"/>
+      <c r="CH49" s="338"/>
+      <c r="CI49" s="339"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="287" t="s">
+      <c r="AJ50" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="288"/>
+      <c r="AK50" s="290"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -13838,19 +13978,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="338"/>
+      <c r="AQ50" s="346"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="330"/>
-      <c r="AV50" s="331"/>
+      <c r="AU50" s="338"/>
+      <c r="AV50" s="339"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="287" t="s">
+      <c r="BD50" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="288"/>
+      <c r="BE50" s="290"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -13859,18 +13999,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="338"/>
+      <c r="BK50" s="346"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="330"/>
-      <c r="BP50" s="331"/>
+      <c r="BO50" s="338"/>
+      <c r="BP50" s="339"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="287" t="s">
+      <c r="BW50" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="288"/>
+      <c r="BX50" s="290"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -13879,21 +14019,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="338"/>
+      <c r="CD50" s="346"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="330"/>
-      <c r="CI50" s="331"/>
+      <c r="CH50" s="338"/>
+      <c r="CI50" s="339"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="289" t="s">
+      <c r="B51" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="290"/>
-      <c r="D51" s="291"/>
+      <c r="C51" s="292"/>
+      <c r="D51" s="293"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -13943,14 +14083,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="339"/>
+      <c r="AQ51" s="347"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="340"/>
-      <c r="AV51" s="341"/>
+      <c r="AU51" s="348"/>
+      <c r="AV51" s="349"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -13962,14 +14102,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="339"/>
+      <c r="BK51" s="347"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="340"/>
-      <c r="BP51" s="341"/>
+      <c r="BO51" s="348"/>
+      <c r="BP51" s="349"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -13980,14 +14120,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="339"/>
+      <c r="CD51" s="347"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="340"/>
-      <c r="CI51" s="341"/>
+      <c r="CH51" s="348"/>
+      <c r="CI51" s="349"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -14008,11 +14148,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="289" t="s">
+      <c r="V52" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="290"/>
-      <c r="X52" s="291"/>
+      <c r="W52" s="292"/>
+      <c r="X52" s="293"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -14114,11 +14254,11 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="46"/>
-      <c r="AO53" s="289" t="s">
+      <c r="AO53" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="AP53" s="290"/>
-      <c r="AQ53" s="291"/>
+      <c r="AP53" s="292"/>
+      <c r="AQ53" s="293"/>
       <c r="AR53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14165,11 +14305,11 @@
         <f ca="1">TODAY()</f>
         <v>45294</v>
       </c>
-      <c r="BJ53" s="289" t="s">
+      <c r="BJ53" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="BK53" s="290"/>
-      <c r="BL53" s="291"/>
+      <c r="BK53" s="292"/>
+      <c r="BL53" s="293"/>
       <c r="BM53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14212,11 +14352,11 @@
       <c r="BZ53" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="CC53" s="289" t="s">
+      <c r="CC53" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="CD53" s="290"/>
-      <c r="CE53" s="291"/>
+      <c r="CD53" s="292"/>
+      <c r="CE53" s="293"/>
       <c r="CF53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14260,11 +14400,11 @@
         <v>108</v>
       </c>
       <c r="CV53" s="42"/>
-      <c r="CW53" s="289" t="s">
+      <c r="CW53" s="291" t="s">
         <v>145</v>
       </c>
-      <c r="CX53" s="290"/>
-      <c r="CY53" s="291"/>
+      <c r="CX53" s="292"/>
+      <c r="CY53" s="293"/>
       <c r="CZ53" s="26" t="s">
         <v>43</v>
       </c>
@@ -17351,10 +17491,10 @@
       </c>
     </row>
     <row r="66" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="287" t="s">
+      <c r="B66" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="288"/>
+      <c r="C66" s="290"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -17367,8 +17507,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="330"/>
-      <c r="O66" s="331"/>
+      <c r="N66" s="338"/>
+      <c r="O66" s="339"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -17508,18 +17648,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="281"/>
+      <c r="J67" s="337"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="330"/>
-      <c r="O67" s="331"/>
+      <c r="N67" s="338"/>
+      <c r="O67" s="339"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="287" t="s">
+      <c r="V67" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="288"/>
+      <c r="W67" s="290"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -17531,8 +17671,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="330"/>
-      <c r="AI67" s="331"/>
+      <c r="AH67" s="338"/>
+      <c r="AI67" s="339"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -17603,7 +17743,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="332"/>
+      <c r="J68" s="340"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -17619,17 +17759,17 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="281"/>
+      <c r="AD68" s="337"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="330"/>
-      <c r="AI68" s="331"/>
+      <c r="AH68" s="338"/>
+      <c r="AI68" s="339"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
-      <c r="AO68" s="287" t="s">
+      <c r="AO68" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="AP68" s="288"/>
+      <c r="AP68" s="290"/>
       <c r="AQ68" s="189"/>
       <c r="AR68" s="9">
         <f>SUM(AO55:AQ66)</f>
@@ -17641,15 +17781,15 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="330"/>
-      <c r="BB68" s="331"/>
+      <c r="BA68" s="338"/>
+      <c r="BB68" s="339"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
-      <c r="BJ68" s="287" t="s">
+      <c r="BJ68" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="BK68" s="288"/>
+      <c r="BK68" s="290"/>
       <c r="BL68" s="189"/>
       <c r="BM68" s="9">
         <f>SUM(BJ55:BL66)</f>
@@ -17661,15 +17801,15 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="330"/>
-      <c r="BW68" s="331"/>
+      <c r="BV68" s="338"/>
+      <c r="BW68" s="339"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
       <c r="BZ68" s="46"/>
-      <c r="CC68" s="287" t="s">
+      <c r="CC68" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="CD68" s="288"/>
+      <c r="CD68" s="290"/>
       <c r="CE68" s="189"/>
       <c r="CF68" s="9">
         <f>SUM(CC55:CE66)</f>
@@ -17681,16 +17821,16 @@
       <c r="CJ68" s="119"/>
       <c r="CK68" s="117"/>
       <c r="CN68" s="2"/>
-      <c r="CO68" s="330"/>
-      <c r="CP68" s="331"/>
+      <c r="CO68" s="338"/>
+      <c r="CP68" s="339"/>
       <c r="CQ68" s="1"/>
       <c r="CR68" s="1"/>
       <c r="CS68" s="46"/>
       <c r="CV68" s="110"/>
-      <c r="CW68" s="287" t="s">
+      <c r="CW68" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="CX68" s="288"/>
+      <c r="CX68" s="290"/>
       <c r="CY68" s="189"/>
       <c r="CZ68" s="9">
         <f>SUM(CW55:CY66)</f>
@@ -17698,19 +17838,19 @@
       </c>
       <c r="DA68" s="26"/>
       <c r="DB68" s="262"/>
-      <c r="DC68" s="268"/>
+      <c r="DC68" s="267"/>
       <c r="DD68" s="254"/>
       <c r="DE68" s="117"/>
-      <c r="DF68" s="264" t="s">
+      <c r="DF68" s="263" t="s">
         <v>276</v>
       </c>
       <c r="DG68" s="18"/>
-      <c r="DH68" s="265"/>
+      <c r="DH68" s="264"/>
       <c r="DI68" s="159" t="s">
         <v>271</v>
       </c>
-      <c r="DJ68" s="282"/>
-      <c r="DK68" s="266" t="s">
+      <c r="DJ68" s="284"/>
+      <c r="DK68" s="265" t="s">
         <v>284</v>
       </c>
       <c r="DL68" s="1"/>
@@ -17728,7 +17868,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="332"/>
+      <c r="AD69" s="340"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -17744,10 +17884,10 @@
       <c r="AT69" s="119"/>
       <c r="AU69" s="192"/>
       <c r="AV69" s="119"/>
-      <c r="AW69" s="281"/>
+      <c r="AW69" s="337"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="330"/>
-      <c r="BB69" s="331"/>
+      <c r="BA69" s="338"/>
+      <c r="BB69" s="339"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
@@ -17758,10 +17898,10 @@
       <c r="BO69" s="119"/>
       <c r="BP69" s="192"/>
       <c r="BQ69" s="119"/>
-      <c r="BR69" s="281"/>
+      <c r="BR69" s="337"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="330"/>
-      <c r="BW69" s="331"/>
+      <c r="BV69" s="338"/>
+      <c r="BW69" s="339"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
       <c r="BZ69" s="46"/>
@@ -17772,10 +17912,10 @@
       <c r="CH69" s="119"/>
       <c r="CI69" s="192"/>
       <c r="CJ69" s="119"/>
-      <c r="CK69" s="281"/>
+      <c r="CK69" s="337"/>
       <c r="CN69" s="2"/>
-      <c r="CO69" s="330"/>
-      <c r="CP69" s="331"/>
+      <c r="CO69" s="338"/>
+      <c r="CP69" s="339"/>
       <c r="CQ69" s="1"/>
       <c r="CR69" s="1"/>
       <c r="CS69" s="46"/>
@@ -17787,14 +17927,14 @@
       <c r="DB69" s="262"/>
       <c r="DC69" s="169"/>
       <c r="DD69" s="169"/>
-      <c r="DE69" s="281"/>
+      <c r="DE69" s="337"/>
       <c r="DF69" s="159" t="s">
         <v>280</v>
       </c>
       <c r="DG69" s="18"/>
-      <c r="DH69" s="265"/>
+      <c r="DH69" s="264"/>
       <c r="DI69" s="159"/>
-      <c r="DJ69" s="282"/>
+      <c r="DJ69" s="284"/>
       <c r="DK69" s="17"/>
       <c r="DL69" s="1"/>
       <c r="DM69" s="46"/>
@@ -17807,7 +17947,7 @@
       <c r="AT70" s="117"/>
       <c r="AU70" s="192"/>
       <c r="AV70" s="119"/>
-      <c r="AW70" s="281"/>
+      <c r="AW70" s="337"/>
       <c r="AZ70" s="2"/>
       <c r="BA70" s="152"/>
       <c r="BB70" s="1"/>
@@ -17821,7 +17961,7 @@
       <c r="BO70" s="117"/>
       <c r="BP70" s="192"/>
       <c r="BQ70" s="119"/>
-      <c r="BR70" s="281"/>
+      <c r="BR70" s="337"/>
       <c r="BU70" s="2"/>
       <c r="BV70" s="152"/>
       <c r="BW70" s="1"/>
@@ -17836,7 +17976,7 @@
       <c r="CH70" s="137"/>
       <c r="CI70" s="203"/>
       <c r="CJ70" s="201"/>
-      <c r="CK70" s="332"/>
+      <c r="CK70" s="340"/>
       <c r="CL70" s="50"/>
       <c r="CM70" s="50"/>
       <c r="CN70" s="79"/>
@@ -17853,7 +17993,7 @@
       <c r="DB70" s="117"/>
       <c r="DC70" s="194"/>
       <c r="DD70" s="119"/>
-      <c r="DE70" s="281"/>
+      <c r="DE70" s="337"/>
       <c r="DF70" s="159" t="s">
         <v>275</v>
       </c>
@@ -17921,12 +18061,12 @@
         <v>274</v>
       </c>
       <c r="DG71" s="18"/>
-      <c r="DH71" s="265"/>
+      <c r="DH71" s="264"/>
       <c r="DI71" s="159" t="s">
         <v>279</v>
       </c>
       <c r="DJ71" s="17"/>
-      <c r="DK71" s="266" t="s">
+      <c r="DK71" s="265" t="s">
         <v>285</v>
       </c>
       <c r="DL71" s="1"/>
@@ -17944,13 +18084,13 @@
       <c r="DD72" s="137"/>
       <c r="DE72" s="137"/>
       <c r="DF72" s="5"/>
-      <c r="DG72" s="329" t="s">
+      <c r="DG72" s="336" t="s">
         <v>291</v>
       </c>
-      <c r="DH72" s="329"/>
-      <c r="DI72" s="269"/>
-      <c r="DJ72" s="270"/>
-      <c r="DK72" s="271" t="s">
+      <c r="DH72" s="336"/>
+      <c r="DI72" s="268"/>
+      <c r="DJ72" s="269"/>
+      <c r="DK72" s="270" t="s">
         <v>285</v>
       </c>
       <c r="DL72" s="65"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.0 _8:00AM
Boat Enabled -
InCapacity - [17,8,5,3,1,Cnt] ,
NodeW - [-3] ,
BirdW - [7][CityW-MundiaSahi] ,
FuelW_Day - ['22],
OnHost - [8+1]
VillageW=[0],
CityW=[] ,
[X-MarketShieldMatrix-X] = [6,2,8,2] = [Lx -3 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.1.0.xlsx
+++ b/Usage_S_1.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7AA833-3E81-463C-9BC2-3B088F5294CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B851EA3-D2E0-4ED2-89FF-C57FCB54D70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2718" uniqueCount="318">
   <si>
     <t>UnSettled</t>
   </si>
@@ -952,9 +952,6 @@
     <t>X-MWL(5)  - X</t>
   </si>
   <si>
-    <t>ScootyT</t>
-  </si>
-  <si>
     <t>Cement</t>
   </si>
   <si>
@@ -989,6 +986,12 @@
   </si>
   <si>
     <t>MarketXRecovery</t>
+  </si>
+  <si>
+    <t>X-FuelW(22)_Morning - X</t>
+  </si>
+  <si>
+    <t>ScootyT_WL</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1979,11 +1982,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="360">
+  <cellXfs count="364">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2670,6 +2684,29 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2754,72 +2791,72 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2830,6 +2867,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2876,26 +2919,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3185,8 +3209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="P9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ25" sqref="AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,7 +3250,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AA1" s="308" t="s">
+      <c r="AA1" s="317" t="s">
         <v>247</v>
       </c>
       <c r="AB1" s="36" t="s">
@@ -3241,12 +3265,12 @@
       <c r="AE1" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="AG1" s="305" t="s">
+      <c r="AG1" s="314" t="s">
         <v>241</v>
       </c>
-      <c r="AH1" s="306"/>
-      <c r="AI1" s="306"/>
-      <c r="AJ1" s="307"/>
+      <c r="AH1" s="315"/>
+      <c r="AI1" s="315"/>
+      <c r="AJ1" s="316"/>
     </row>
     <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -3255,15 +3279,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="287">
+      <c r="C2" s="296">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="291" t="s">
+      <c r="E2" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="292"/>
-      <c r="G2" s="293"/>
+      <c r="F2" s="301"/>
+      <c r="G2" s="302"/>
       <c r="H2" s="281"/>
       <c r="I2" s="26" t="s">
         <v>43</v>
@@ -3309,28 +3333,28 @@
       </c>
       <c r="X2" s="98">
         <f ca="1">TODAY()</f>
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="Y2" s="8"/>
       <c r="Z2" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="AA2" s="309"/>
+      <c r="AA2" s="318"/>
       <c r="AB2" s="36">
         <f>SUM(AB3:AB19)</f>
         <v>6</v>
       </c>
       <c r="AC2" s="15">
         <f>SUM(AC3:AC25)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD2" s="36">
         <f>SUM(AD3:AD25)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AE2" s="36">
         <f>SUM(AE3:AE25)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AG2" s="9" t="s">
         <v>92</v>
@@ -3344,13 +3368,13 @@
       <c r="AJ2" s="8"/>
     </row>
     <row r="3" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="285" t="s">
+      <c r="A3" s="294" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="288"/>
+      <c r="C3" s="297"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
@@ -3365,10 +3389,10 @@
       </c>
       <c r="AC3" s="253"/>
       <c r="AD3" s="109"/>
-      <c r="AF3" s="297"/>
+      <c r="AF3" s="306"/>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="286"/>
+      <c r="A4" s="295"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -3378,13 +3402,9 @@
       <c r="E4" s="244">
         <v>5</v>
       </c>
-      <c r="F4" s="205">
-        <v>10</v>
-      </c>
-      <c r="G4" s="353">
-        <v>10</v>
-      </c>
-      <c r="H4" s="353"/>
+      <c r="F4" s="205"/>
+      <c r="G4" s="283"/>
+      <c r="H4" s="283"/>
       <c r="I4" s="9" t="s">
         <v>199</v>
       </c>
@@ -3395,7 +3415,7 @@
         <v>187</v>
       </c>
       <c r="L4" s="169" t="s">
-        <v>281</v>
+        <v>316</v>
       </c>
       <c r="M4" s="83" t="s">
         <v>213</v>
@@ -3413,16 +3433,16 @@
         <v>30</v>
       </c>
       <c r="R4" s="154">
-        <v>0.83680555555555547</v>
+        <v>0.33680555555555558</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>130</v>
       </c>
       <c r="T4" s="154">
-        <v>0.83680555555555547</v>
+        <v>0.33680555555555558</v>
       </c>
       <c r="V4" s="245">
-        <v>45295</v>
+        <v>45296</v>
       </c>
       <c r="Z4" s="25" t="s">
         <v>244</v>
@@ -3432,7 +3452,7 @@
       </c>
       <c r="AC4" s="20"/>
       <c r="AD4" s="24"/>
-      <c r="AF4" s="298"/>
+      <c r="AF4" s="307"/>
       <c r="AG4" s="25"/>
       <c r="AH4" s="25"/>
       <c r="AI4" s="24" t="s">
@@ -3440,22 +3460,14 @@
       </c>
     </row>
     <row r="5" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
-        <v>275</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="D5" s="156">
         <v>-2</v>
       </c>
-      <c r="E5" s="218">
-        <v>30</v>
-      </c>
-      <c r="F5" s="206">
-        <v>5</v>
-      </c>
+      <c r="E5" s="218"/>
+      <c r="F5" s="206"/>
       <c r="G5" s="127"/>
-      <c r="H5" s="127">
-        <v>50</v>
-      </c>
+      <c r="H5" s="127"/>
       <c r="I5" s="9" t="s">
         <v>1</v>
       </c>
@@ -3465,9 +3477,7 @@
       <c r="K5" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="L5" s="169" t="s">
-        <v>288</v>
-      </c>
+      <c r="L5" s="169"/>
       <c r="M5" s="167" t="s">
         <v>142</v>
       </c>
@@ -3500,7 +3510,7 @@
       </c>
       <c r="AC5" s="20"/>
       <c r="AD5" s="24"/>
-      <c r="AF5" s="298"/>
+      <c r="AF5" s="307"/>
       <c r="AG5" s="25"/>
       <c r="AH5" s="25"/>
       <c r="AI5" s="24" t="s">
@@ -3509,7 +3519,7 @@
     </row>
     <row r="6" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>4368</v>
+        <v>4648</v>
       </c>
       <c r="C6">
         <v>4000</v>
@@ -3517,9 +3527,7 @@
       <c r="E6" s="218"/>
       <c r="F6" s="207"/>
       <c r="G6" s="127"/>
-      <c r="H6" s="127">
-        <v>30</v>
-      </c>
+      <c r="H6" s="127"/>
       <c r="I6" s="9" t="s">
         <v>203</v>
       </c>
@@ -3529,9 +3537,7 @@
       <c r="K6" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="L6" s="169" t="s">
-        <v>288</v>
-      </c>
+      <c r="L6" s="169"/>
       <c r="M6" s="83" t="s">
         <v>123</v>
       </c>
@@ -3570,7 +3576,7 @@
       </c>
       <c r="AC6" s="15"/>
       <c r="AD6" s="24"/>
-      <c r="AF6" s="298"/>
+      <c r="AF6" s="307"/>
       <c r="AG6" s="25"/>
       <c r="AI6" s="24"/>
     </row>
@@ -3585,12 +3591,8 @@
         <v>52</v>
       </c>
       <c r="E7" s="165"/>
-      <c r="F7" s="242">
-        <v>10</v>
-      </c>
-      <c r="G7" s="177">
-        <v>50</v>
-      </c>
+      <c r="F7" s="242"/>
+      <c r="G7" s="177"/>
       <c r="H7" s="177"/>
       <c r="I7" s="9" t="s">
         <v>188</v>
@@ -3601,9 +3603,7 @@
       <c r="K7" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="169" t="s">
-        <v>293</v>
-      </c>
+      <c r="L7" s="169"/>
       <c r="M7" s="83" t="s">
         <v>139</v>
       </c>
@@ -3637,7 +3637,7 @@
       <c r="AB7" s="26"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="24"/>
-      <c r="AF7" s="298"/>
+      <c r="AF7" s="307"/>
       <c r="AG7" s="25"/>
       <c r="AH7" s="25"/>
       <c r="AI7" s="24" t="s">
@@ -3646,16 +3646,12 @@
     </row>
     <row r="8" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E8" s="219"/>
-      <c r="F8" s="242">
-        <v>25</v>
-      </c>
-      <c r="G8" s="352">
-        <v>10</v>
-      </c>
-      <c r="H8" s="352"/>
+      <c r="F8" s="242"/>
+      <c r="G8" s="282"/>
+      <c r="H8" s="282"/>
       <c r="I8" s="9" t="s">
         <v>72</v>
       </c>
@@ -3702,7 +3698,7 @@
       <c r="AB8" s="25"/>
       <c r="AC8" s="15"/>
       <c r="AD8" s="24"/>
-      <c r="AF8" s="298"/>
+      <c r="AF8" s="307"/>
       <c r="AG8" s="25"/>
       <c r="AH8" s="25"/>
       <c r="AI8" s="24" t="s">
@@ -3715,16 +3711,12 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>11643</v>
+        <v>11648</v>
       </c>
       <c r="E9" s="163"/>
-      <c r="F9" s="165">
-        <v>14</v>
-      </c>
-      <c r="G9" s="352">
-        <v>10</v>
-      </c>
-      <c r="H9" s="352"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="282"/>
+      <c r="H9" s="282"/>
       <c r="I9" s="9" t="s">
         <v>71</v>
       </c>
@@ -3734,9 +3726,7 @@
       <c r="K9" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="L9" s="169" t="s">
-        <v>273</v>
-      </c>
+      <c r="L9" s="169"/>
       <c r="M9" s="223" t="s">
         <v>163</v>
       </c>
@@ -3769,13 +3759,8 @@
       </c>
       <c r="AB9" s="25"/>
       <c r="AC9" s="15"/>
-      <c r="AD9" s="24">
-        <v>1</v>
-      </c>
-      <c r="AE9">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="298"/>
+      <c r="AD9" s="24"/>
+      <c r="AF9" s="307"/>
       <c r="AG9" s="25" t="s">
         <v>66</v>
       </c>
@@ -3787,18 +3772,10 @@
       </c>
     </row>
     <row r="10" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="220">
-        <v>8</v>
-      </c>
-      <c r="F10" s="206">
-        <v>8</v>
-      </c>
-      <c r="G10" s="177">
-        <v>10</v>
-      </c>
-      <c r="H10" s="177">
-        <v>70</v>
-      </c>
+      <c r="E10" s="220"/>
+      <c r="F10" s="206"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="177"/>
       <c r="I10" s="9" t="s">
         <v>81</v>
       </c>
@@ -3808,9 +3785,7 @@
       <c r="K10" s="213" t="s">
         <v>294</v>
       </c>
-      <c r="L10" s="194" t="s">
-        <v>242</v>
-      </c>
+      <c r="L10" s="194"/>
       <c r="M10" s="83" t="s">
         <v>143</v>
       </c>
@@ -3845,11 +3820,9 @@
       <c r="AA10" s="169" t="s">
         <v>232</v>
       </c>
-      <c r="AC10" s="15">
-        <v>1</v>
-      </c>
+      <c r="AC10" s="15"/>
       <c r="AD10" s="24"/>
-      <c r="AF10" s="298"/>
+      <c r="AF10" s="307"/>
       <c r="AG10" s="25"/>
       <c r="AH10" s="25"/>
       <c r="AI10" s="24">
@@ -3865,12 +3838,8 @@
         <v>-30</v>
       </c>
       <c r="E11" s="221"/>
-      <c r="F11" s="242">
-        <v>5</v>
-      </c>
-      <c r="G11" s="37">
-        <v>5</v>
-      </c>
+      <c r="F11" s="242"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="9" t="s">
         <v>102</v>
@@ -3881,9 +3850,7 @@
       <c r="K11" s="213" t="s">
         <v>116</v>
       </c>
-      <c r="L11" s="169" t="s">
-        <v>282</v>
-      </c>
+      <c r="L11" s="169"/>
       <c r="M11" s="83" t="s">
         <v>124</v>
       </c>
@@ -3914,16 +3881,9 @@
       <c r="AA11" s="169" t="s">
         <v>233</v>
       </c>
-      <c r="AC11" s="15">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="24">
-        <v>1</v>
-      </c>
-      <c r="AE11">
-        <v>2</v>
-      </c>
-      <c r="AF11" s="298"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="24"/>
+      <c r="AF11" s="307"/>
       <c r="AG11" s="25" t="s">
         <v>181</v>
       </c>
@@ -3935,15 +3895,9 @@
       </c>
     </row>
     <row r="12" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="165">
-        <v>15</v>
-      </c>
-      <c r="F12" s="205">
-        <v>55</v>
-      </c>
-      <c r="G12" s="164">
-        <v>100</v>
-      </c>
+      <c r="E12" s="165"/>
+      <c r="F12" s="205"/>
+      <c r="G12" s="164"/>
       <c r="H12" s="164"/>
       <c r="I12" s="28" t="s">
         <v>128</v>
@@ -3987,19 +3941,11 @@
         <v>234</v>
       </c>
       <c r="AC12" s="15"/>
-      <c r="AD12" s="271">
-        <v>1</v>
-      </c>
-      <c r="AF12" s="298"/>
-      <c r="AG12" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI12" s="24" t="s">
-        <v>246</v>
-      </c>
+      <c r="AD12" s="271"/>
+      <c r="AF12" s="307"/>
+      <c r="AG12" s="25"/>
+      <c r="AH12" s="25"/>
+      <c r="AI12" s="24"/>
     </row>
     <row r="13" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
@@ -4007,20 +3953,12 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>11673</v>
-      </c>
-      <c r="E13" s="36">
-        <v>5</v>
-      </c>
-      <c r="F13" s="206">
-        <v>1</v>
-      </c>
-      <c r="G13" s="246">
-        <v>35</v>
-      </c>
-      <c r="H13" s="246">
-        <v>10</v>
-      </c>
+        <v>11678</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="206"/>
+      <c r="G13" s="246"/>
+      <c r="H13" s="246"/>
       <c r="I13" s="9" t="s">
         <v>189</v>
       </c>
@@ -4028,11 +3966,9 @@
         <v>17</v>
       </c>
       <c r="K13" s="228" t="s">
-        <v>314</v>
-      </c>
-      <c r="L13" s="194" t="s">
-        <v>242</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="L13" s="194"/>
       <c r="M13" s="183" t="s">
         <v>155</v>
       </c>
@@ -4067,12 +4003,25 @@
       <c r="AA13" s="169" t="s">
         <v>235</v>
       </c>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="24"/>
-      <c r="AF13" s="298"/>
-      <c r="AG13" s="25"/>
-      <c r="AH13" s="25"/>
-      <c r="AI13" s="24"/>
+      <c r="AC13" s="15">
+        <v>2</v>
+      </c>
+      <c r="AD13" s="24">
+        <v>4</v>
+      </c>
+      <c r="AE13">
+        <v>1</v>
+      </c>
+      <c r="AF13" s="307"/>
+      <c r="AG13" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI13" s="24" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="14" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
@@ -4129,7 +4078,7 @@
       <c r="AD14" s="241">
         <v>1</v>
       </c>
-      <c r="AF14" s="298"/>
+      <c r="AF14" s="307"/>
       <c r="AG14" s="25"/>
       <c r="AH14" s="25"/>
       <c r="AI14" s="24" t="s">
@@ -4176,16 +4125,9 @@
       <c r="AA15" s="169" t="s">
         <v>238</v>
       </c>
-      <c r="AC15" s="15">
-        <v>1</v>
-      </c>
-      <c r="AD15" s="36">
-        <v>1</v>
-      </c>
-      <c r="AE15">
-        <v>1</v>
-      </c>
-      <c r="AF15" s="298"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="36"/>
+      <c r="AF15" s="307"/>
       <c r="AG15" s="25" t="s">
         <v>66</v>
       </c>
@@ -4213,7 +4155,7 @@
         <v>239</v>
       </c>
       <c r="AD16" s="24"/>
-      <c r="AF16" s="298"/>
+      <c r="AF16" s="307"/>
       <c r="AG16" s="25"/>
       <c r="AI16" s="24"/>
     </row>
@@ -4222,23 +4164,23 @@
       <c r="D17" s="25"/>
       <c r="E17" s="34">
         <f>SUM(E4:E15)</f>
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="F17" s="34">
         <f>SUM(F4:F15)</f>
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="G17" s="34">
         <f>SUM(G4:G15)</f>
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="H17" s="189">
         <f>SUM(H4:H15)</f>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="I17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>426</v>
+        <v>5</v>
       </c>
       <c r="J17" s="26"/>
       <c r="K17" s="262"/>
@@ -4251,12 +4193,12 @@
       </c>
       <c r="P17" s="82"/>
       <c r="Q17" s="280" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R17" s="272" t="s">
         <v>271</v>
       </c>
-      <c r="S17" s="284"/>
+      <c r="S17" s="293"/>
       <c r="T17" s="265" t="s">
         <v>284</v>
       </c>
@@ -4270,16 +4212,10 @@
       <c r="AB17" s="50"/>
       <c r="AC17" s="15"/>
       <c r="AD17" s="115"/>
-      <c r="AE17" s="50">
-        <v>2</v>
-      </c>
-      <c r="AF17" s="298"/>
-      <c r="AG17" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="AH17" s="25" t="s">
-        <v>15</v>
-      </c>
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="307"/>
+      <c r="AG17" s="25"/>
+      <c r="AH17" s="25"/>
       <c r="AI17" s="24" t="s">
         <v>246</v>
       </c>
@@ -4293,10 +4229,10 @@
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="289" t="s">
+      <c r="E18" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="290"/>
+      <c r="F18" s="299"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="J18" s="226"/>
@@ -4305,16 +4241,16 @@
         <v>269</v>
       </c>
       <c r="M18" s="278"/>
-      <c r="N18" s="282" t="s">
-        <v>314</v>
-      </c>
-      <c r="O18" s="303" t="s">
-        <v>306</v>
-      </c>
-      <c r="P18" s="303"/>
-      <c r="Q18" s="304"/>
+      <c r="N18" s="291" t="s">
+        <v>313</v>
+      </c>
+      <c r="O18" s="312" t="s">
+        <v>305</v>
+      </c>
+      <c r="P18" s="312"/>
+      <c r="Q18" s="313"/>
       <c r="R18" s="161"/>
-      <c r="S18" s="284"/>
+      <c r="S18" s="293"/>
       <c r="T18" s="17"/>
       <c r="Y18" s="25" t="s">
         <v>286</v>
@@ -4326,7 +4262,7 @@
         <v>254</v>
       </c>
       <c r="AD18" s="24"/>
-      <c r="AF18" s="298"/>
+      <c r="AF18" s="307"/>
       <c r="AG18" s="25"/>
       <c r="AH18" s="25"/>
       <c r="AI18" s="24" t="s">
@@ -4334,34 +4270,27 @@
       </c>
     </row>
     <row r="19" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="354">
-        <v>35</v>
-      </c>
-      <c r="F19" s="59">
-        <v>40</v>
-      </c>
-      <c r="G19" s="355">
-        <v>100</v>
-      </c>
-      <c r="H19" s="357"/>
+      <c r="E19" s="284"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="285"/>
       <c r="I19" s="1"/>
       <c r="J19" s="226"/>
       <c r="L19" s="169" t="s">
         <v>288</v>
       </c>
       <c r="M19" s="119"/>
-      <c r="N19" s="283"/>
+      <c r="N19" s="292"/>
       <c r="O19" s="279" t="s">
-        <v>312</v>
-      </c>
-      <c r="P19" s="294" t="s">
+        <v>311</v>
+      </c>
+      <c r="P19" s="303" t="s">
         <v>290</v>
       </c>
-      <c r="Q19" s="294"/>
-      <c r="R19" s="295" t="s">
+      <c r="Q19" s="303"/>
+      <c r="R19" s="304" t="s">
         <v>277</v>
       </c>
-      <c r="S19" s="295"/>
+      <c r="S19" s="304"/>
       <c r="T19" s="17"/>
       <c r="Z19" s="25" t="s">
         <v>244</v>
@@ -4373,7 +4302,7 @@
       <c r="AC19" s="79"/>
       <c r="AD19" s="115"/>
       <c r="AE19" s="50"/>
-      <c r="AF19" s="298"/>
+      <c r="AF19" s="307"/>
       <c r="AG19" s="25"/>
       <c r="AH19" s="25"/>
       <c r="AI19" s="24" t="s">
@@ -4381,30 +4310,25 @@
       </c>
     </row>
     <row r="20" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="359" t="s">
-        <v>316</v>
+      <c r="A20" s="287" t="s">
+        <v>315</v>
       </c>
       <c r="B20" s="29">
         <v>30</v>
       </c>
-      <c r="E20" s="236">
-        <v>30</v>
-      </c>
-      <c r="F20" s="65">
-        <v>70</v>
-      </c>
-      <c r="G20" s="356"/>
-      <c r="H20" s="357"/>
+      <c r="E20" s="236"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="286"/>
       <c r="J20" s="227"/>
       <c r="L20" s="169" t="s">
         <v>272</v>
       </c>
       <c r="M20" s="119"/>
       <c r="N20" s="231" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O20" s="277" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P20" s="18"/>
       <c r="Q20" s="264"/>
@@ -4425,7 +4349,7 @@
       <c r="AC20" s="258"/>
       <c r="AD20" s="257"/>
       <c r="AE20" s="256"/>
-      <c r="AF20" s="298"/>
+      <c r="AF20" s="307"/>
       <c r="AG20" s="25"/>
       <c r="AH20" s="25"/>
       <c r="AI20" s="24" t="s">
@@ -4433,14 +4357,16 @@
       </c>
     </row>
     <row r="21" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L21" s="169"/>
+      <c r="L21" s="169" t="s">
+        <v>282</v>
+      </c>
       <c r="O21" s="272" t="s">
-        <v>313</v>
-      </c>
-      <c r="P21" s="296" t="s">
+        <v>312</v>
+      </c>
+      <c r="P21" s="305" t="s">
         <v>291</v>
       </c>
-      <c r="Q21" s="296"/>
+      <c r="Q21" s="305"/>
       <c r="R21" s="266"/>
       <c r="S21" s="17"/>
       <c r="T21" s="265" t="s">
@@ -4457,19 +4383,11 @@
       </c>
       <c r="AB21" s="42"/>
       <c r="AC21" s="15"/>
-      <c r="AD21" s="109">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="43">
-        <v>1</v>
-      </c>
-      <c r="AF21" s="298"/>
-      <c r="AG21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH21" s="25" t="s">
-        <v>15</v>
-      </c>
+      <c r="AD21" s="109"/>
+      <c r="AE21" s="43"/>
+      <c r="AF21" s="307"/>
+      <c r="AG21" s="25"/>
+      <c r="AH21" s="25"/>
       <c r="AI21" s="24" t="s">
         <v>246</v>
       </c>
@@ -4492,8 +4410,13 @@
       </c>
       <c r="AB22" s="48"/>
       <c r="AC22" s="15"/>
-      <c r="AD22" s="24"/>
-      <c r="AF22" s="298"/>
+      <c r="AD22" s="24">
+        <v>3</v>
+      </c>
+      <c r="AE22">
+        <v>1</v>
+      </c>
+      <c r="AF22" s="307"/>
       <c r="AG22" s="25" t="s">
         <v>298</v>
       </c>
@@ -4506,7 +4429,7 @@
     </row>
     <row r="23" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L23" s="169" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Z23" s="25" t="s">
         <v>244</v>
@@ -4518,7 +4441,7 @@
       <c r="AC23" s="116"/>
       <c r="AD23" s="115"/>
       <c r="AE23" s="50"/>
-      <c r="AF23" s="298"/>
+      <c r="AF23" s="307"/>
       <c r="AG23" s="25"/>
       <c r="AH23" s="25"/>
       <c r="AI23" s="24" t="s">
@@ -4526,14 +4449,17 @@
       </c>
     </row>
     <row r="24" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R24" s="300" t="s">
+      <c r="L24" s="169" t="s">
+        <v>222</v>
+      </c>
+      <c r="R24" s="309" t="s">
         <v>302</v>
       </c>
       <c r="S24" s="265">
         <v>3</v>
       </c>
       <c r="T24" s="275" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Z24" s="25" t="s">
         <v>244</v>
@@ -4545,7 +4471,7 @@
       <c r="AC24" s="258"/>
       <c r="AD24" s="257"/>
       <c r="AE24" s="256"/>
-      <c r="AF24" s="298"/>
+      <c r="AF24" s="307"/>
       <c r="AG24" s="25"/>
       <c r="AH24" s="25"/>
       <c r="AI24" s="24" t="s">
@@ -4557,17 +4483,17 @@
         <v>2</v>
       </c>
       <c r="K25" s="231" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M25" s="231" t="s">
-        <v>308</v>
-      </c>
-      <c r="R25" s="301"/>
+        <v>307</v>
+      </c>
+      <c r="R25" s="310"/>
       <c r="S25" s="265">
         <v>1</v>
       </c>
       <c r="T25" s="275" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="Y25" s="25" t="s">
         <v>271</v>
@@ -4582,7 +4508,7 @@
       <c r="AC25" s="258"/>
       <c r="AD25" s="257"/>
       <c r="AE25" s="256"/>
-      <c r="AF25" s="298"/>
+      <c r="AF25" s="307"/>
       <c r="AG25" s="25"/>
       <c r="AH25" s="25"/>
       <c r="AI25" s="24" t="s">
@@ -4593,7 +4519,7 @@
       <c r="L26" s="169" t="s">
         <v>289</v>
       </c>
-      <c r="R26" s="302"/>
+      <c r="R26" s="311"/>
       <c r="S26" s="265">
         <v>1</v>
       </c>
@@ -4606,14 +4532,14 @@
       <c r="AA26" s="169" t="s">
         <v>260</v>
       </c>
-      <c r="AF26" s="298"/>
+      <c r="AF26" s="307"/>
     </row>
     <row r="27" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J27" s="25">
         <v>1</v>
       </c>
       <c r="K27" s="231" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M27" s="233"/>
       <c r="Y27" s="25" t="s">
@@ -4625,24 +4551,26 @@
       <c r="AA27" s="169" t="s">
         <v>295</v>
       </c>
-      <c r="AF27" s="298"/>
+      <c r="AF27" s="307"/>
     </row>
     <row r="28" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AA28" s="169" t="s">
         <v>297</v>
       </c>
+      <c r="AB28" s="255"/>
       <c r="AC28" s="15">
         <v>2</v>
       </c>
-      <c r="AE28">
+      <c r="AD28" s="288"/>
+      <c r="AE28" s="363">
         <v>1</v>
       </c>
-      <c r="AF28" s="299"/>
+      <c r="AF28" s="308"/>
       <c r="AG28" s="25" t="s">
         <v>30</v>
       </c>
       <c r="AH28" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AI28" s="1">
         <v>1</v>
@@ -4760,10 +4688,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:T67"/>
+  <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4787,18 +4715,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="326" t="s">
+      <c r="E1" s="323" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="328"/>
+      <c r="F1" s="325"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="326" t="s">
+      <c r="H1" s="323" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="327"/>
-      <c r="J1" s="328"/>
+      <c r="I1" s="324"/>
+      <c r="J1" s="325"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4816,7 +4744,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="329">
+      <c r="B2" s="326">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4843,26 +4771,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="332">
+      <c r="K2" s="341">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="321">
+      <c r="L2" s="339">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="313">
+      <c r="M2" s="329">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J67)</f>
-        <v>11633</v>
+        <f>SUM(E2:J68)</f>
+        <v>11638</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="330"/>
+      <c r="B3" s="327"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4877,13 +4805,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="333"/>
-      <c r="L3" s="284"/>
-      <c r="M3" s="314"/>
+      <c r="K3" s="342"/>
+      <c r="L3" s="293"/>
+      <c r="M3" s="330"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="331"/>
+      <c r="B4" s="328"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4898,9 +4826,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="333"/>
-      <c r="L4" s="284"/>
-      <c r="M4" s="314"/>
+      <c r="K4" s="342"/>
+      <c r="L4" s="293"/>
+      <c r="M4" s="330"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4982,7 +4910,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="310">
+      <c r="B7" s="331">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4999,22 +4927,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="315">
+      <c r="K7" s="333">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="317">
+      <c r="L7" s="335">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="319">
+      <c r="M7" s="337">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="312"/>
+      <c r="B8" s="332"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -5035,9 +4963,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="316"/>
-      <c r="L8" s="318"/>
-      <c r="M8" s="320"/>
+      <c r="K8" s="334"/>
+      <c r="L8" s="336"/>
+      <c r="M8" s="338"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -5117,7 +5045,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="310">
+      <c r="B11" s="331">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -5144,7 +5072,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="312"/>
+      <c r="B12" s="332"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -5201,7 +5129,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="310">
+      <c r="B14" s="331">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -5224,7 +5152,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="312"/>
+      <c r="B15" s="332"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -5248,7 +5176,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="329">
+      <c r="B16" s="326">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -5279,7 +5207,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="330"/>
+      <c r="B17" s="327"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -5297,7 +5225,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="329">
+      <c r="B18" s="326">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -5326,7 +5254,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="331"/>
+      <c r="B19" s="328"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -5386,7 +5314,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="334">
+      <c r="B21" s="343">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -5414,7 +5342,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="335"/>
+      <c r="B22" s="344"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -5466,7 +5394,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="287">
+      <c r="B24" s="296">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -5495,7 +5423,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="288"/>
+      <c r="B25" s="297"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -5523,7 +5451,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="287">
+      <c r="B26" s="296">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -5554,7 +5482,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="325"/>
+      <c r="B27" s="322"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5585,7 +5513,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="287">
+      <c r="B28" s="296">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -5607,7 +5535,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="288"/>
+      <c r="B29" s="297"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -5633,7 +5561,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="287">
+      <c r="B30" s="296">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -5656,7 +5584,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="288"/>
+      <c r="B31" s="297"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -5683,7 +5611,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="287">
+      <c r="B32" s="296">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -5705,7 +5633,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="288"/>
+      <c r="B33" s="297"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -5758,7 +5686,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="287">
+      <c r="B35" s="296">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -5785,7 +5713,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="288"/>
+      <c r="B36" s="297"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -5807,7 +5735,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="287">
+      <c r="B37" s="296">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -5840,7 +5768,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="288"/>
+      <c r="B38" s="297"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -5858,7 +5786,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="287">
+      <c r="B39" s="296">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -5885,7 +5813,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="325"/>
+      <c r="B40" s="322"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5913,7 +5841,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="287">
+      <c r="B41" s="296">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -5940,7 +5868,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="325"/>
+      <c r="B42" s="322"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5958,7 +5886,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="288"/>
+      <c r="B43" s="297"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -5987,7 +5915,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="287">
+      <c r="B44" s="296">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -6013,7 +5941,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="288"/>
+      <c r="B45" s="297"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -6038,7 +5966,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="287">
+      <c r="B46" s="296">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -6060,7 +5988,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="325"/>
+      <c r="B47" s="322"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -6081,7 +6009,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="287">
+      <c r="B48" s="296">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -6101,7 +6029,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="325"/>
+      <c r="B49" s="322"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -6127,7 +6055,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="325"/>
+      <c r="B50" s="322"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -6154,7 +6082,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="287">
+      <c r="B51" s="296">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -6176,7 +6104,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="288"/>
+      <c r="B52" s="297"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -6209,7 +6137,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="287">
+      <c r="B53" s="296">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -6239,7 +6167,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="325"/>
+      <c r="B54" s="322"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -6266,7 +6194,7 @@
       <c r="A55" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="287">
+      <c r="B55" s="296">
         <v>31</v>
       </c>
       <c r="C55" s="96"/>
@@ -6294,7 +6222,7 @@
       <c r="M55" s="82"/>
     </row>
     <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="288"/>
+      <c r="B56" s="297"/>
       <c r="C56" s="96"/>
       <c r="D56" s="82"/>
       <c r="E56" s="82">
@@ -6320,7 +6248,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="322">
+      <c r="B57" s="319">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -6340,7 +6268,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="323"/>
+      <c r="B58" s="320"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -6369,7 +6297,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="324"/>
+      <c r="B59" s="321"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -6395,7 +6323,7 @@
       <c r="M59" s="18"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="287">
+      <c r="B60" s="296">
         <v>2</v>
       </c>
       <c r="C60" s="142"/>
@@ -6421,7 +6349,7 @@
       <c r="M60" s="18"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="325"/>
+      <c r="B61" s="322"/>
       <c r="C61" s="142"/>
       <c r="D61" s="18">
         <v>240</v>
@@ -6447,7 +6375,7 @@
       <c r="M61" s="18"/>
     </row>
     <row r="62" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="288"/>
+      <c r="B62" s="297"/>
       <c r="C62" s="142"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
@@ -6468,7 +6396,7 @@
       <c r="A63" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="310">
+      <c r="B63" s="331">
         <v>3</v>
       </c>
       <c r="C63" s="142"/>
@@ -6490,7 +6418,7 @@
       <c r="M63" s="18"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="311"/>
+      <c r="B64" s="340"/>
       <c r="C64" s="142"/>
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
@@ -6510,7 +6438,7 @@
       <c r="M64" s="18"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="311"/>
+      <c r="B65" s="340"/>
       <c r="C65" s="142"/>
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
@@ -6532,7 +6460,7 @@
       <c r="M65" s="18"/>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="311"/>
+      <c r="B66" s="340"/>
       <c r="C66" s="142"/>
       <c r="D66" s="18">
         <v>500</v>
@@ -6543,7 +6471,7 @@
       <c r="F66" s="18">
         <v>50</v>
       </c>
-      <c r="G66" s="358">
+      <c r="G66" s="18">
         <v>70</v>
       </c>
       <c r="H66" s="18">
@@ -6552,7 +6480,7 @@
       <c r="I66" s="18">
         <v>30</v>
       </c>
-      <c r="J66" s="358">
+      <c r="J66" s="18">
         <v>60</v>
       </c>
       <c r="K66" s="18"/>
@@ -6560,12 +6488,12 @@
       <c r="M66" s="18"/>
     </row>
     <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="312"/>
+      <c r="B67" s="332"/>
       <c r="C67" s="142"/>
       <c r="D67" s="18"/>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
-      <c r="G67" s="358">
+      <c r="G67" s="18">
         <v>30</v>
       </c>
       <c r="H67" s="18"/>
@@ -6574,6 +6502,24 @@
       <c r="K67" s="18"/>
       <c r="L67" s="18"/>
       <c r="M67" s="18"/>
+    </row>
+    <row r="68" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="130">
+        <v>4</v>
+      </c>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18">
+        <v>5</v>
+      </c>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
+      <c r="M68" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -6592,6 +6538,7 @@
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="E1:F1"/>
@@ -6603,7 +6550,6 @@
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="L2:L4"/>
-    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="B37:B38"/>
@@ -6617,10 +6563,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EF39B9-450C-4C51-9807-7AFD5CC29C14}">
-  <dimension ref="A1:DN73"/>
+  <dimension ref="A1:DN88"/>
   <sheetViews>
-    <sheetView topLeftCell="CT53" workbookViewId="0">
-      <selection activeCell="CU67" sqref="CU67"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="U76" sqref="U76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8170,7 +8116,7 @@
       </c>
       <c r="AC14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="AG14" s="99" t="s">
         <v>44</v>
@@ -8215,7 +8161,7 @@
       <c r="AU14" s="43"/>
       <c r="AV14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="AZ14" s="99" t="s">
         <v>44</v>
@@ -8260,7 +8206,7 @@
       <c r="BN14" s="43"/>
       <c r="BO14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="BR14" s="158" t="s">
         <v>44</v>
@@ -8305,7 +8251,7 @@
       <c r="CF14" s="43"/>
       <c r="CG14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45294</v>
+        <v>45295</v>
       </c>
     </row>
     <row r="15" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9816,10 +9762,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="289" t="s">
+      <c r="AG24" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="290"/>
+      <c r="AH24" s="299"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -9839,10 +9785,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="289" t="s">
+      <c r="AZ24" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="290"/>
+      <c r="BA24" s="299"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -9862,10 +9808,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="289" t="s">
+      <c r="BR24" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="290"/>
+      <c r="BS24" s="299"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -9888,10 +9834,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="291" t="s">
+      <c r="B26" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="293"/>
+      <c r="C26" s="302"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9928,10 +9874,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="291" t="s">
+      <c r="R26" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="293"/>
+      <c r="S26" s="302"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9968,10 +9914,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="291" t="s">
+      <c r="AG26" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="293"/>
+      <c r="AH26" s="302"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -10008,10 +9954,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="291" t="s">
+      <c r="AW26" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="293"/>
+      <c r="AX26" s="302"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -10048,10 +9994,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="291" t="s">
+      <c r="BM26" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="293"/>
+      <c r="BN26" s="302"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -11045,7 +10991,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="341">
+      <c r="AX32" s="352">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -11083,7 +11029,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="341">
+      <c r="BN32" s="352">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -11232,7 +11178,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="342"/>
+      <c r="AX33" s="353"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -11268,7 +11214,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="342"/>
+      <c r="BN33" s="353"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -11419,7 +11365,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="343"/>
+      <c r="AX34" s="354"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11457,7 +11403,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="343"/>
+      <c r="BN34" s="354"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11688,10 +11634,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="289" t="s">
+      <c r="B36" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="290"/>
+      <c r="C36" s="299"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -11709,10 +11655,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="289" t="s">
+      <c r="R36" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="290"/>
+      <c r="S36" s="299"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -11730,10 +11676,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="289" t="s">
+      <c r="AG36" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="290"/>
+      <c r="AH36" s="299"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -11751,10 +11697,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="289" t="s">
+      <c r="AW36" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="290"/>
+      <c r="AX36" s="299"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -11772,10 +11718,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="289" t="s">
+      <c r="BM36" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="290"/>
+      <c r="BN36" s="299"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -11795,10 +11741,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="291" t="s">
+      <c r="B38" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="293"/>
+      <c r="C38" s="302"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11838,10 +11784,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="291" t="s">
+      <c r="S38" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="293"/>
+      <c r="T38" s="302"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11881,11 +11827,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="291" t="s">
+      <c r="AJ38" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="292"/>
-      <c r="AL38" s="293"/>
+      <c r="AK38" s="301"/>
+      <c r="AL38" s="302"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11928,13 +11874,13 @@
       <c r="AZ38" s="44"/>
       <c r="BA38" s="199">
         <f ca="1">TODAY()</f>
-        <v>45294</v>
-      </c>
-      <c r="BD38" s="291" t="s">
+        <v>45295</v>
+      </c>
+      <c r="BD38" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="292"/>
-      <c r="BF38" s="293"/>
+      <c r="BE38" s="301"/>
+      <c r="BF38" s="302"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11974,11 +11920,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="291" t="s">
+      <c r="BW38" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="292"/>
-      <c r="BY38" s="293"/>
+      <c r="BX38" s="301"/>
+      <c r="BY38" s="302"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -12930,7 +12876,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="341">
+      <c r="C44" s="352">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12968,10 +12914,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="350">
+      <c r="S44" s="361">
         <v>25</v>
       </c>
-      <c r="T44" s="341">
+      <c r="T44" s="352">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12980,7 +12926,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="344" t="s">
+      <c r="W44" s="355" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -13009,10 +12955,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="350">
+      <c r="AJ44" s="361">
         <v>50</v>
       </c>
-      <c r="AK44" s="341">
+      <c r="AK44" s="352">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -13022,7 +12968,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="344" t="s">
+      <c r="AO44" s="355" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -13052,7 +12998,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="350">
+      <c r="BD44" s="361">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -13063,7 +13009,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="344" t="s">
+      <c r="BI44" s="355" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -13092,7 +13038,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="350">
+      <c r="BW44" s="361">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -13103,7 +13049,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="344" t="s">
+      <c r="CB44" s="355" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -13135,7 +13081,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="342"/>
+      <c r="C45" s="353"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -13169,15 +13115,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="351"/>
-      <c r="T45" s="343"/>
+      <c r="S45" s="362"/>
+      <c r="T45" s="354"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="345"/>
+      <c r="W45" s="356"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13204,8 +13150,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="351"/>
-      <c r="AK45" s="343"/>
+      <c r="AJ45" s="362"/>
+      <c r="AK45" s="354"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -13213,7 +13159,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="345"/>
+      <c r="AO45" s="356"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13241,7 +13187,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="351"/>
+      <c r="BD45" s="362"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -13252,7 +13198,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="345"/>
+      <c r="BI45" s="356"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13279,7 +13225,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="351"/>
+      <c r="BW45" s="362"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -13288,7 +13234,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="345"/>
+      <c r="CB45" s="356"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13318,7 +13264,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="343"/>
+      <c r="C46" s="354"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13745,10 +13691,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="289" t="s">
+      <c r="B48" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="290"/>
+      <c r="C48" s="299"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -13767,10 +13713,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="289" t="s">
+      <c r="S48" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="290"/>
+      <c r="T48" s="299"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -13923,11 +13869,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="346"/>
+      <c r="AQ49" s="357"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="338"/>
-      <c r="AV49" s="339"/>
+      <c r="AU49" s="349"/>
+      <c r="AV49" s="350"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -13939,11 +13885,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="346"/>
+      <c r="BK49" s="357"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="338"/>
-      <c r="BP49" s="339"/>
+      <c r="BO49" s="349"/>
+      <c r="BP49" s="350"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -13954,20 +13900,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="346"/>
+      <c r="CD49" s="357"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="338"/>
-      <c r="CI49" s="339"/>
+      <c r="CH49" s="349"/>
+      <c r="CI49" s="350"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="289" t="s">
+      <c r="AJ50" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="290"/>
+      <c r="AK50" s="299"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -13978,19 +13924,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="346"/>
+      <c r="AQ50" s="357"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="338"/>
-      <c r="AV50" s="339"/>
+      <c r="AU50" s="349"/>
+      <c r="AV50" s="350"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="289" t="s">
+      <c r="BD50" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="290"/>
+      <c r="BE50" s="299"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -13999,18 +13945,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="346"/>
+      <c r="BK50" s="357"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="338"/>
-      <c r="BP50" s="339"/>
+      <c r="BO50" s="349"/>
+      <c r="BP50" s="350"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="289" t="s">
+      <c r="BW50" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="290"/>
+      <c r="BX50" s="299"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -14019,21 +13965,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="346"/>
+      <c r="CD50" s="357"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="338"/>
-      <c r="CI50" s="339"/>
+      <c r="CH50" s="349"/>
+      <c r="CI50" s="350"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="291" t="s">
+      <c r="B51" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="292"/>
-      <c r="D51" s="293"/>
+      <c r="C51" s="301"/>
+      <c r="D51" s="302"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -14083,14 +14029,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="347"/>
+      <c r="AQ51" s="358"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="348"/>
-      <c r="AV51" s="349"/>
+      <c r="AU51" s="359"/>
+      <c r="AV51" s="360"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -14102,14 +14048,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="347"/>
+      <c r="BK51" s="358"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="348"/>
-      <c r="BP51" s="349"/>
+      <c r="BO51" s="359"/>
+      <c r="BP51" s="360"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -14120,14 +14066,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="347"/>
+      <c r="CD51" s="358"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="348"/>
-      <c r="CI51" s="349"/>
+      <c r="CH51" s="359"/>
+      <c r="CI51" s="360"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -14148,11 +14094,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="291" t="s">
+      <c r="V52" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="292"/>
-      <c r="X52" s="293"/>
+      <c r="W52" s="301"/>
+      <c r="X52" s="302"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -14254,11 +14200,11 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="46"/>
-      <c r="AO53" s="291" t="s">
+      <c r="AO53" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="AP53" s="292"/>
-      <c r="AQ53" s="293"/>
+      <c r="AP53" s="301"/>
+      <c r="AQ53" s="302"/>
       <c r="AR53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14303,13 +14249,13 @@
       </c>
       <c r="BG53" s="98">
         <f ca="1">TODAY()</f>
-        <v>45294</v>
-      </c>
-      <c r="BJ53" s="291" t="s">
+        <v>45295</v>
+      </c>
+      <c r="BJ53" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="BK53" s="292"/>
-      <c r="BL53" s="293"/>
+      <c r="BK53" s="301"/>
+      <c r="BL53" s="302"/>
       <c r="BM53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14352,11 +14298,11 @@
       <c r="BZ53" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="CC53" s="291" t="s">
+      <c r="CC53" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="CD53" s="292"/>
-      <c r="CE53" s="293"/>
+      <c r="CD53" s="301"/>
+      <c r="CE53" s="302"/>
       <c r="CF53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14400,11 +14346,11 @@
         <v>108</v>
       </c>
       <c r="CV53" s="42"/>
-      <c r="CW53" s="291" t="s">
+      <c r="CW53" s="300" t="s">
         <v>145</v>
       </c>
-      <c r="CX53" s="292"/>
-      <c r="CY53" s="293"/>
+      <c r="CX53" s="301"/>
+      <c r="CY53" s="302"/>
       <c r="CZ53" s="26" t="s">
         <v>43</v>
       </c>
@@ -17491,10 +17437,10 @@
       </c>
     </row>
     <row r="66" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="289" t="s">
+      <c r="B66" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="290"/>
+      <c r="C66" s="299"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -17507,8 +17453,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="338"/>
-      <c r="O66" s="339"/>
+      <c r="N66" s="349"/>
+      <c r="O66" s="350"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -17648,18 +17594,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="337"/>
+      <c r="J67" s="348"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="338"/>
-      <c r="O67" s="339"/>
+      <c r="N67" s="349"/>
+      <c r="O67" s="350"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="289" t="s">
+      <c r="V67" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="290"/>
+      <c r="W67" s="299"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -17671,8 +17617,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="338"/>
-      <c r="AI67" s="339"/>
+      <c r="AH67" s="349"/>
+      <c r="AI67" s="350"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -17743,7 +17689,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="340"/>
+      <c r="J68" s="351"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -17759,17 +17705,17 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="337"/>
+      <c r="AD68" s="348"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="338"/>
-      <c r="AI68" s="339"/>
+      <c r="AH68" s="349"/>
+      <c r="AI68" s="350"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
-      <c r="AO68" s="289" t="s">
+      <c r="AO68" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="AP68" s="290"/>
+      <c r="AP68" s="299"/>
       <c r="AQ68" s="189"/>
       <c r="AR68" s="9">
         <f>SUM(AO55:AQ66)</f>
@@ -17781,15 +17727,15 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="338"/>
-      <c r="BB68" s="339"/>
+      <c r="BA68" s="349"/>
+      <c r="BB68" s="350"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
-      <c r="BJ68" s="289" t="s">
+      <c r="BJ68" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="BK68" s="290"/>
+      <c r="BK68" s="299"/>
       <c r="BL68" s="189"/>
       <c r="BM68" s="9">
         <f>SUM(BJ55:BL66)</f>
@@ -17801,15 +17747,15 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="338"/>
-      <c r="BW68" s="339"/>
+      <c r="BV68" s="349"/>
+      <c r="BW68" s="350"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
       <c r="BZ68" s="46"/>
-      <c r="CC68" s="289" t="s">
+      <c r="CC68" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="CD68" s="290"/>
+      <c r="CD68" s="299"/>
       <c r="CE68" s="189"/>
       <c r="CF68" s="9">
         <f>SUM(CC55:CE66)</f>
@@ -17821,16 +17767,16 @@
       <c r="CJ68" s="119"/>
       <c r="CK68" s="117"/>
       <c r="CN68" s="2"/>
-      <c r="CO68" s="338"/>
-      <c r="CP68" s="339"/>
+      <c r="CO68" s="349"/>
+      <c r="CP68" s="350"/>
       <c r="CQ68" s="1"/>
       <c r="CR68" s="1"/>
       <c r="CS68" s="46"/>
       <c r="CV68" s="110"/>
-      <c r="CW68" s="289" t="s">
+      <c r="CW68" s="298" t="s">
         <v>4</v>
       </c>
-      <c r="CX68" s="290"/>
+      <c r="CX68" s="299"/>
       <c r="CY68" s="189"/>
       <c r="CZ68" s="9">
         <f>SUM(CW55:CY66)</f>
@@ -17849,7 +17795,7 @@
       <c r="DI68" s="159" t="s">
         <v>271</v>
       </c>
-      <c r="DJ68" s="284"/>
+      <c r="DJ68" s="293"/>
       <c r="DK68" s="265" t="s">
         <v>284</v>
       </c>
@@ -17868,7 +17814,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="340"/>
+      <c r="AD69" s="351"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -17884,10 +17830,10 @@
       <c r="AT69" s="119"/>
       <c r="AU69" s="192"/>
       <c r="AV69" s="119"/>
-      <c r="AW69" s="337"/>
+      <c r="AW69" s="348"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="338"/>
-      <c r="BB69" s="339"/>
+      <c r="BA69" s="349"/>
+      <c r="BB69" s="350"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
@@ -17898,10 +17844,10 @@
       <c r="BO69" s="119"/>
       <c r="BP69" s="192"/>
       <c r="BQ69" s="119"/>
-      <c r="BR69" s="337"/>
+      <c r="BR69" s="348"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="338"/>
-      <c r="BW69" s="339"/>
+      <c r="BV69" s="349"/>
+      <c r="BW69" s="350"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
       <c r="BZ69" s="46"/>
@@ -17912,10 +17858,10 @@
       <c r="CH69" s="119"/>
       <c r="CI69" s="192"/>
       <c r="CJ69" s="119"/>
-      <c r="CK69" s="337"/>
+      <c r="CK69" s="348"/>
       <c r="CN69" s="2"/>
-      <c r="CO69" s="338"/>
-      <c r="CP69" s="339"/>
+      <c r="CO69" s="349"/>
+      <c r="CP69" s="350"/>
       <c r="CQ69" s="1"/>
       <c r="CR69" s="1"/>
       <c r="CS69" s="46"/>
@@ -17927,14 +17873,14 @@
       <c r="DB69" s="262"/>
       <c r="DC69" s="169"/>
       <c r="DD69" s="169"/>
-      <c r="DE69" s="337"/>
+      <c r="DE69" s="348"/>
       <c r="DF69" s="159" t="s">
         <v>280</v>
       </c>
       <c r="DG69" s="18"/>
       <c r="DH69" s="264"/>
       <c r="DI69" s="159"/>
-      <c r="DJ69" s="284"/>
+      <c r="DJ69" s="293"/>
       <c r="DK69" s="17"/>
       <c r="DL69" s="1"/>
       <c r="DM69" s="46"/>
@@ -17947,7 +17893,7 @@
       <c r="AT70" s="117"/>
       <c r="AU70" s="192"/>
       <c r="AV70" s="119"/>
-      <c r="AW70" s="337"/>
+      <c r="AW70" s="348"/>
       <c r="AZ70" s="2"/>
       <c r="BA70" s="152"/>
       <c r="BB70" s="1"/>
@@ -17961,7 +17907,7 @@
       <c r="BO70" s="117"/>
       <c r="BP70" s="192"/>
       <c r="BQ70" s="119"/>
-      <c r="BR70" s="337"/>
+      <c r="BR70" s="348"/>
       <c r="BU70" s="2"/>
       <c r="BV70" s="152"/>
       <c r="BW70" s="1"/>
@@ -17976,7 +17922,7 @@
       <c r="CH70" s="137"/>
       <c r="CI70" s="203"/>
       <c r="CJ70" s="201"/>
-      <c r="CK70" s="340"/>
+      <c r="CK70" s="351"/>
       <c r="CL70" s="50"/>
       <c r="CM70" s="50"/>
       <c r="CN70" s="79"/>
@@ -17993,23 +17939,71 @@
       <c r="DB70" s="117"/>
       <c r="DC70" s="194"/>
       <c r="DD70" s="119"/>
-      <c r="DE70" s="337"/>
+      <c r="DE70" s="348"/>
       <c r="DF70" s="159" t="s">
         <v>275</v>
       </c>
-      <c r="DG70" s="296" t="s">
+      <c r="DG70" s="305" t="s">
         <v>290</v>
       </c>
-      <c r="DH70" s="296"/>
-      <c r="DI70" s="295" t="s">
+      <c r="DH70" s="305"/>
+      <c r="DI70" s="304" t="s">
         <v>277</v>
       </c>
-      <c r="DJ70" s="295"/>
+      <c r="DJ70" s="304"/>
       <c r="DK70" s="17"/>
       <c r="DL70" s="1"/>
       <c r="DM70" s="46"/>
     </row>
     <row r="71" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="300" t="s">
+        <v>145</v>
+      </c>
+      <c r="C71" s="301"/>
+      <c r="D71" s="302"/>
+      <c r="E71" s="281"/>
+      <c r="F71" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G71" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H71" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="I71" s="214" t="s">
+        <v>195</v>
+      </c>
+      <c r="J71" s="83" t="s">
+        <v>153</v>
+      </c>
+      <c r="K71" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="L71" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M71" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="N71" s="171" t="s">
+        <v>92</v>
+      </c>
+      <c r="O71" s="153" t="s">
+        <v>267</v>
+      </c>
+      <c r="P71" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q71" s="156" t="s">
+        <v>268</v>
+      </c>
+      <c r="R71" s="214" t="s">
+        <v>224</v>
+      </c>
+      <c r="S71" s="36" t="s">
+        <v>108</v>
+      </c>
       <c r="AO71" s="236"/>
       <c r="AP71" s="65"/>
       <c r="AQ71" s="79"/>
@@ -18073,6 +18067,21 @@
       <c r="DM71" s="46"/>
     </row>
     <row r="72" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="136"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="G72" s="25"/>
+      <c r="H72" s="117"/>
+      <c r="I72" s="192"/>
+      <c r="J72" s="117"/>
+      <c r="K72" s="117"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="152"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="46"/>
       <c r="CV72" s="63"/>
       <c r="CW72" s="65"/>
       <c r="CX72" s="65"/>
@@ -18084,10 +18093,10 @@
       <c r="DD72" s="137"/>
       <c r="DE72" s="137"/>
       <c r="DF72" s="5"/>
-      <c r="DG72" s="336" t="s">
+      <c r="DG72" s="347" t="s">
         <v>291</v>
       </c>
-      <c r="DH72" s="336"/>
+      <c r="DH72" s="347"/>
       <c r="DI72" s="268"/>
       <c r="DJ72" s="269"/>
       <c r="DK72" s="270" t="s">
@@ -18096,7 +18105,57 @@
       <c r="DL72" s="65"/>
       <c r="DM72" s="168"/>
     </row>
-    <row r="73" spans="2:118" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="244">
+        <v>5</v>
+      </c>
+      <c r="C73" s="205">
+        <v>10</v>
+      </c>
+      <c r="D73" s="283">
+        <v>10</v>
+      </c>
+      <c r="E73" s="283"/>
+      <c r="F73" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G73" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" s="213" t="s">
+        <v>187</v>
+      </c>
+      <c r="I73" s="169" t="s">
+        <v>281</v>
+      </c>
+      <c r="J73" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="K73" s="224" t="s">
+        <v>156</v>
+      </c>
+      <c r="L73" s="143" t="s">
+        <v>193</v>
+      </c>
+      <c r="M73" s="169" t="s">
+        <v>156</v>
+      </c>
+      <c r="N73" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O73" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q73" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="R73" s="1"/>
+      <c r="S73" s="248">
+        <v>45295</v>
+      </c>
       <c r="CW73" s="1"/>
       <c r="CX73" s="1"/>
       <c r="CY73" s="2"/>
@@ -18114,8 +18173,640 @@
       <c r="DL73" s="1"/>
       <c r="DM73" s="24"/>
     </row>
+    <row r="74" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="218">
+        <v>30</v>
+      </c>
+      <c r="C74" s="206">
+        <v>5</v>
+      </c>
+      <c r="D74" s="127"/>
+      <c r="E74" s="127">
+        <v>50</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G74" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="I74" s="169" t="s">
+        <v>288</v>
+      </c>
+      <c r="J74" s="167" t="s">
+        <v>142</v>
+      </c>
+      <c r="K74" s="224" t="s">
+        <v>85</v>
+      </c>
+      <c r="L74" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="M74" s="237" t="s">
+        <v>137</v>
+      </c>
+      <c r="N74" s="197" t="s">
+        <v>86</v>
+      </c>
+      <c r="O74" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="R74" s="1"/>
+      <c r="S74" s="248">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="75" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="218"/>
+      <c r="C75" s="207"/>
+      <c r="D75" s="127"/>
+      <c r="E75" s="127">
+        <v>30</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G75" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="I75" s="169" t="s">
+        <v>288</v>
+      </c>
+      <c r="J75" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="K75" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="L75" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="M75" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="N75" s="176" t="s">
+        <v>69</v>
+      </c>
+      <c r="O75" s="154">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="154">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="R75" s="1"/>
+      <c r="S75" s="248">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="76" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="165"/>
+      <c r="C76" s="242">
+        <v>10</v>
+      </c>
+      <c r="D76" s="177">
+        <v>50</v>
+      </c>
+      <c r="E76" s="177"/>
+      <c r="F76" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G76" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="I76" s="169" t="s">
+        <v>293</v>
+      </c>
+      <c r="J76" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="K76" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="L76" s="143" t="s">
+        <v>192</v>
+      </c>
+      <c r="M76" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N76" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="O76" s="154">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="154">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="R76" s="1"/>
+      <c r="S76" s="248">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="77" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="219"/>
+      <c r="C77" s="242">
+        <v>25</v>
+      </c>
+      <c r="D77" s="282">
+        <v>10</v>
+      </c>
+      <c r="E77" s="282"/>
+      <c r="F77" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G77" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" s="213"/>
+      <c r="I77" s="274" t="s">
+        <v>300</v>
+      </c>
+      <c r="J77" s="83" t="s">
+        <v>214</v>
+      </c>
+      <c r="K77" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="L77" s="187" t="s">
+        <v>196</v>
+      </c>
+      <c r="M77" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="N77" s="188" t="s">
+        <v>65</v>
+      </c>
+      <c r="O77" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="R77" s="273">
+        <v>1</v>
+      </c>
+      <c r="S77" s="248">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="78" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="163"/>
+      <c r="C78" s="165">
+        <v>14</v>
+      </c>
+      <c r="D78" s="282">
+        <v>10</v>
+      </c>
+      <c r="E78" s="282"/>
+      <c r="F78" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G78" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="I78" s="169" t="s">
+        <v>273</v>
+      </c>
+      <c r="J78" s="223" t="s">
+        <v>163</v>
+      </c>
+      <c r="K78" s="224" t="s">
+        <v>170</v>
+      </c>
+      <c r="L78" s="143" t="s">
+        <v>191</v>
+      </c>
+      <c r="M78" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N78" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O78" s="154">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="154">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="R78" s="1"/>
+      <c r="S78" s="248">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="79" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="220">
+        <v>8</v>
+      </c>
+      <c r="C79" s="206">
+        <v>8</v>
+      </c>
+      <c r="D79" s="177">
+        <v>10</v>
+      </c>
+      <c r="E79" s="177">
+        <v>70</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G79" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H79" s="213" t="s">
+        <v>294</v>
+      </c>
+      <c r="I79" s="194" t="s">
+        <v>242</v>
+      </c>
+      <c r="J79" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="K79" s="225" t="s">
+        <v>62</v>
+      </c>
+      <c r="L79" s="144" t="s">
+        <v>122</v>
+      </c>
+      <c r="M79" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="N79" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="O79" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q79" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="R79" s="1"/>
+      <c r="S79" s="248">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="80" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="221"/>
+      <c r="C80" s="242">
+        <v>5</v>
+      </c>
+      <c r="D80" s="37">
+        <v>5</v>
+      </c>
+      <c r="E80" s="37"/>
+      <c r="F80" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G80" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H80" s="213" t="s">
+        <v>116</v>
+      </c>
+      <c r="I80" s="169" t="s">
+        <v>282</v>
+      </c>
+      <c r="J80" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="K80" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="L80" s="186" t="s">
+        <v>110</v>
+      </c>
+      <c r="M80" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="N80" s="198" t="s">
+        <v>161</v>
+      </c>
+      <c r="O80" s="154">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="154">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="R80" s="1"/>
+      <c r="S80" s="248">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="81" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="165">
+        <v>15</v>
+      </c>
+      <c r="C81" s="205">
+        <v>55</v>
+      </c>
+      <c r="D81" s="164">
+        <v>100</v>
+      </c>
+      <c r="E81" s="164"/>
+      <c r="F81" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="G81" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H81" s="213"/>
+      <c r="I81" s="169" t="s">
+        <v>222</v>
+      </c>
+      <c r="J81" s="224" t="s">
+        <v>123</v>
+      </c>
+      <c r="K81" s="225" t="s">
+        <v>62</v>
+      </c>
+      <c r="L81" s="143" t="s">
+        <v>197</v>
+      </c>
+      <c r="M81" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N81" s="188" t="s">
+        <v>181</v>
+      </c>
+      <c r="O81" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="P81" s="24"/>
+      <c r="Q81" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="R81" s="1"/>
+      <c r="S81" s="248">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="82" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="36">
+        <v>5</v>
+      </c>
+      <c r="C82" s="206">
+        <v>1</v>
+      </c>
+      <c r="D82" s="246">
+        <v>35</v>
+      </c>
+      <c r="E82" s="246">
+        <v>10</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G82" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H82" s="228" t="s">
+        <v>313</v>
+      </c>
+      <c r="I82" s="194" t="s">
+        <v>242</v>
+      </c>
+      <c r="J82" s="183" t="s">
+        <v>155</v>
+      </c>
+      <c r="K82" s="183" t="s">
+        <v>85</v>
+      </c>
+      <c r="L82" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="M82" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="N82" s="229" t="s">
+        <v>90</v>
+      </c>
+      <c r="O82" s="154">
+        <v>0.53125</v>
+      </c>
+      <c r="Q82" s="154">
+        <v>0.53125</v>
+      </c>
+      <c r="R82" s="261">
+        <v>1</v>
+      </c>
+      <c r="S82" s="248">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="83" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="165"/>
+      <c r="C83" s="205"/>
+      <c r="D83" s="127"/>
+      <c r="E83" s="127"/>
+      <c r="F83" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" s="213"/>
+      <c r="I83" s="169"/>
+      <c r="J83" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="K83" s="224" t="s">
+        <v>62</v>
+      </c>
+      <c r="L83" s="143" t="s">
+        <v>200</v>
+      </c>
+      <c r="M83" s="169" t="s">
+        <v>47</v>
+      </c>
+      <c r="N83" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="O83" s="154">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="Q83" s="154">
+        <v>0.94097222222222221</v>
+      </c>
+      <c r="R83" s="1"/>
+      <c r="S83" s="248">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="84" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="165"/>
+      <c r="C84" s="34"/>
+      <c r="D84" s="177"/>
+      <c r="E84" s="177"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H84" s="231"/>
+      <c r="I84" s="169"/>
+      <c r="J84" s="83"/>
+      <c r="K84" s="233"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="37"/>
+      <c r="O84" s="154">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="Q84" s="154">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="R84" s="1"/>
+      <c r="S84" s="248">
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="85" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="136"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="G85" s="234"/>
+      <c r="H85" s="119"/>
+      <c r="I85" s="216"/>
+      <c r="J85" s="119"/>
+      <c r="K85" s="117"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="152"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+      <c r="S85" s="46"/>
+    </row>
+    <row r="86" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="34">
+        <f>SUM(B73:B84)</f>
+        <v>63</v>
+      </c>
+      <c r="C86" s="34">
+        <f>SUM(C73:C84)</f>
+        <v>133</v>
+      </c>
+      <c r="D86" s="34">
+        <f>SUM(D73:D84)</f>
+        <v>230</v>
+      </c>
+      <c r="E86" s="189">
+        <f>SUM(E73:E84)</f>
+        <v>160</v>
+      </c>
+      <c r="F86" s="9">
+        <f>SUM(B73:D84)</f>
+        <v>426</v>
+      </c>
+      <c r="G86" s="26"/>
+      <c r="H86" s="262"/>
+      <c r="I86" s="169" t="s">
+        <v>273</v>
+      </c>
+      <c r="J86" s="254"/>
+      <c r="K86" s="117"/>
+      <c r="L86" s="276" t="s">
+        <v>276</v>
+      </c>
+      <c r="M86" s="82"/>
+      <c r="N86" s="280" t="s">
+        <v>314</v>
+      </c>
+      <c r="O86" s="272" t="s">
+        <v>271</v>
+      </c>
+      <c r="P86" s="293"/>
+      <c r="Q86" s="265" t="s">
+        <v>284</v>
+      </c>
+      <c r="R86" s="1"/>
+      <c r="S86" s="46"/>
+    </row>
+    <row r="87" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="298" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="299"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="20"/>
+      <c r="G87" s="226"/>
+      <c r="H87" s="262"/>
+      <c r="I87" s="194" t="s">
+        <v>269</v>
+      </c>
+      <c r="J87" s="278"/>
+      <c r="K87" s="291" t="s">
+        <v>313</v>
+      </c>
+      <c r="L87" s="312" t="s">
+        <v>305</v>
+      </c>
+      <c r="M87" s="312"/>
+      <c r="N87" s="313"/>
+      <c r="O87" s="161"/>
+      <c r="P87" s="293"/>
+      <c r="Q87" s="17"/>
+      <c r="R87" s="1"/>
+      <c r="S87" s="46"/>
+    </row>
+    <row r="88" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="130">
+        <v>35</v>
+      </c>
+      <c r="C88" s="288">
+        <v>40</v>
+      </c>
+      <c r="D88" s="289">
+        <v>100</v>
+      </c>
+      <c r="E88" s="79"/>
+      <c r="F88" s="65"/>
+      <c r="G88" s="227"/>
+      <c r="H88" s="137"/>
+      <c r="I88" s="169" t="s">
+        <v>288</v>
+      </c>
+      <c r="J88" s="201"/>
+      <c r="K88" s="292"/>
+      <c r="L88" s="290" t="s">
+        <v>311</v>
+      </c>
+      <c r="M88" s="345" t="s">
+        <v>290</v>
+      </c>
+      <c r="N88" s="345"/>
+      <c r="O88" s="346" t="s">
+        <v>277</v>
+      </c>
+      <c r="P88" s="346"/>
+      <c r="Q88" s="269"/>
+      <c r="R88" s="65"/>
+      <c r="S88" s="168"/>
+    </row>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="84">
     <mergeCell ref="BJ53:BL53"/>
     <mergeCell ref="BJ68:BK68"/>
     <mergeCell ref="BV68:BV69"/>
@@ -18193,6 +18884,13 @@
     <mergeCell ref="DE69:DE70"/>
     <mergeCell ref="DG70:DH70"/>
     <mergeCell ref="DI70:DJ70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="P86:P87"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="K87:K88"/>
+    <mergeCell ref="L87:N87"/>
+    <mergeCell ref="M88:N88"/>
+    <mergeCell ref="O88:P88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.1.0 _12:20PM
Boat Enabled -
InCapacity - [17,8,5,3,1,Cnt] ,
NodeW - [-3] ,
BirdW - [7] ,
FuelW_Day - ['22],
OnHost - [8+1]
VillageW=[0],
CityW=[] ,
[X-MarketShieldMatrix-X] = [6,2,8,2] = [Lx -3 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.1.0.xlsx
+++ b/Usage_S_1.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B851EA3-D2E0-4ED2-89FF-C57FCB54D70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2E0525-55A7-4133-A6C5-0875D22D3FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2718" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2720" uniqueCount="319">
   <si>
     <t>UnSettled</t>
   </si>
@@ -992,6 +992,9 @@
   </si>
   <si>
     <t>ScootyT_WL</t>
+  </si>
+  <si>
+    <t>X-FuelW(22)_Day - X</t>
   </si>
 </sst>
 </file>
@@ -2707,6 +2710,49 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2749,47 +2795,74 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2800,103 +2873,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2910,16 +2905,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3209,8 +3212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ25" sqref="AJ25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3250,7 +3253,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AA1" s="317" t="s">
+      <c r="AA1" s="304" t="s">
         <v>247</v>
       </c>
       <c r="AB1" s="36" t="s">
@@ -3265,12 +3268,12 @@
       <c r="AE1" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="AG1" s="314" t="s">
+      <c r="AG1" s="301" t="s">
         <v>241</v>
       </c>
-      <c r="AH1" s="315"/>
-      <c r="AI1" s="315"/>
-      <c r="AJ1" s="316"/>
+      <c r="AH1" s="302"/>
+      <c r="AI1" s="302"/>
+      <c r="AJ1" s="303"/>
     </row>
     <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -3279,15 +3282,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="296">
+      <c r="C2" s="311">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="300" t="s">
+      <c r="E2" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="301"/>
-      <c r="G2" s="302"/>
+      <c r="F2" s="316"/>
+      <c r="G2" s="317"/>
       <c r="H2" s="281"/>
       <c r="I2" s="26" t="s">
         <v>43</v>
@@ -3339,7 +3342,7 @@
       <c r="Z2" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="AA2" s="318"/>
+      <c r="AA2" s="305"/>
       <c r="AB2" s="36">
         <f>SUM(AB3:AB19)</f>
         <v>6</v>
@@ -3368,13 +3371,13 @@
       <c r="AJ2" s="8"/>
     </row>
     <row r="3" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="294" t="s">
+      <c r="A3" s="309" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="297"/>
+      <c r="C3" s="312"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
@@ -3389,10 +3392,10 @@
       </c>
       <c r="AC3" s="253"/>
       <c r="AD3" s="109"/>
-      <c r="AF3" s="306"/>
+      <c r="AF3" s="293"/>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="295"/>
+      <c r="A4" s="310"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -3400,7 +3403,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="244">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F4" s="205"/>
       <c r="G4" s="283"/>
@@ -3415,7 +3418,7 @@
         <v>187</v>
       </c>
       <c r="L4" s="169" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="M4" s="83" t="s">
         <v>213</v>
@@ -3433,13 +3436,13 @@
         <v>30</v>
       </c>
       <c r="R4" s="154">
-        <v>0.33680555555555558</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>130</v>
       </c>
       <c r="T4" s="154">
-        <v>0.33680555555555558</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="V4" s="245">
         <v>45296</v>
@@ -3452,7 +3455,7 @@
       </c>
       <c r="AC4" s="20"/>
       <c r="AD4" s="24"/>
-      <c r="AF4" s="307"/>
+      <c r="AF4" s="294"/>
       <c r="AG4" s="25"/>
       <c r="AH4" s="25"/>
       <c r="AI4" s="24" t="s">
@@ -3460,7 +3463,9 @@
       </c>
     </row>
     <row r="5" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>55</v>
+      </c>
       <c r="D5" s="156">
         <v>-2</v>
       </c>
@@ -3510,7 +3515,7 @@
       </c>
       <c r="AC5" s="20"/>
       <c r="AD5" s="24"/>
-      <c r="AF5" s="307"/>
+      <c r="AF5" s="294"/>
       <c r="AG5" s="25"/>
       <c r="AH5" s="25"/>
       <c r="AI5" s="24" t="s">
@@ -3576,7 +3581,7 @@
       </c>
       <c r="AC6" s="15"/>
       <c r="AD6" s="24"/>
-      <c r="AF6" s="307"/>
+      <c r="AF6" s="294"/>
       <c r="AG6" s="25"/>
       <c r="AI6" s="24"/>
     </row>
@@ -3637,7 +3642,7 @@
       <c r="AB7" s="26"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="24"/>
-      <c r="AF7" s="307"/>
+      <c r="AF7" s="294"/>
       <c r="AG7" s="25"/>
       <c r="AH7" s="25"/>
       <c r="AI7" s="24" t="s">
@@ -3646,7 +3651,7 @@
     </row>
     <row r="8" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8">
-        <v>190</v>
+        <v>125</v>
       </c>
       <c r="E8" s="219"/>
       <c r="F8" s="242"/>
@@ -3698,7 +3703,7 @@
       <c r="AB8" s="25"/>
       <c r="AC8" s="15"/>
       <c r="AD8" s="24"/>
-      <c r="AF8" s="307"/>
+      <c r="AF8" s="294"/>
       <c r="AG8" s="25"/>
       <c r="AH8" s="25"/>
       <c r="AI8" s="24" t="s">
@@ -3711,7 +3716,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>11648</v>
+        <v>11703</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="165"/>
@@ -3760,7 +3765,7 @@
       <c r="AB9" s="25"/>
       <c r="AC9" s="15"/>
       <c r="AD9" s="24"/>
-      <c r="AF9" s="307"/>
+      <c r="AF9" s="294"/>
       <c r="AG9" s="25" t="s">
         <v>66</v>
       </c>
@@ -3772,7 +3777,9 @@
       </c>
     </row>
     <row r="10" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="220"/>
+      <c r="E10" s="220">
+        <v>10</v>
+      </c>
       <c r="F10" s="206"/>
       <c r="G10" s="177"/>
       <c r="H10" s="177"/>
@@ -3785,7 +3792,9 @@
       <c r="K10" s="213" t="s">
         <v>294</v>
       </c>
-      <c r="L10" s="194"/>
+      <c r="L10" s="169" t="s">
+        <v>316</v>
+      </c>
       <c r="M10" s="83" t="s">
         <v>143</v>
       </c>
@@ -3822,7 +3831,7 @@
       </c>
       <c r="AC10" s="15"/>
       <c r="AD10" s="24"/>
-      <c r="AF10" s="307"/>
+      <c r="AF10" s="294"/>
       <c r="AG10" s="25"/>
       <c r="AH10" s="25"/>
       <c r="AI10" s="24">
@@ -3867,13 +3876,13 @@
         <v>161</v>
       </c>
       <c r="R11" s="154">
-        <v>0.83333333333333337</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="T11" s="154">
-        <v>0.83333333333333337</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="V11" s="245">
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="Z11" s="25" t="s">
         <v>256</v>
@@ -3883,7 +3892,7 @@
       </c>
       <c r="AC11" s="15"/>
       <c r="AD11" s="24"/>
-      <c r="AF11" s="307"/>
+      <c r="AF11" s="294"/>
       <c r="AG11" s="25" t="s">
         <v>181</v>
       </c>
@@ -3942,7 +3951,7 @@
       </c>
       <c r="AC12" s="15"/>
       <c r="AD12" s="271"/>
-      <c r="AF12" s="307"/>
+      <c r="AF12" s="294"/>
       <c r="AG12" s="25"/>
       <c r="AH12" s="25"/>
       <c r="AI12" s="24"/>
@@ -3953,7 +3962,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>11678</v>
+        <v>11733</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="206"/>
@@ -4012,7 +4021,7 @@
       <c r="AE13">
         <v>1</v>
       </c>
-      <c r="AF13" s="307"/>
+      <c r="AF13" s="294"/>
       <c r="AG13" s="25" t="s">
         <v>65</v>
       </c>
@@ -4026,7 +4035,9 @@
     <row r="14" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="165"/>
+      <c r="E14" s="165">
+        <v>40</v>
+      </c>
       <c r="F14" s="205"/>
       <c r="G14" s="127"/>
       <c r="H14" s="127"/>
@@ -4037,7 +4048,9 @@
         <v>17</v>
       </c>
       <c r="K14" s="213"/>
-      <c r="L14" s="169"/>
+      <c r="L14" s="169" t="s">
+        <v>318</v>
+      </c>
       <c r="M14" s="83" t="s">
         <v>124</v>
       </c>
@@ -4078,7 +4091,7 @@
       <c r="AD14" s="241">
         <v>1</v>
       </c>
-      <c r="AF14" s="307"/>
+      <c r="AF14" s="294"/>
       <c r="AG14" s="25"/>
       <c r="AH14" s="25"/>
       <c r="AI14" s="24" t="s">
@@ -4127,7 +4140,7 @@
       </c>
       <c r="AC15" s="15"/>
       <c r="AD15" s="36"/>
-      <c r="AF15" s="307"/>
+      <c r="AF15" s="294"/>
       <c r="AG15" s="25" t="s">
         <v>66</v>
       </c>
@@ -4155,7 +4168,7 @@
         <v>239</v>
       </c>
       <c r="AD16" s="24"/>
-      <c r="AF16" s="307"/>
+      <c r="AF16" s="294"/>
       <c r="AG16" s="25"/>
       <c r="AI16" s="24"/>
     </row>
@@ -4164,7 +4177,7 @@
       <c r="D17" s="25"/>
       <c r="E17" s="34">
         <f>SUM(E4:E15)</f>
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="F17" s="34">
         <f>SUM(F4:F15)</f>
@@ -4180,7 +4193,7 @@
       </c>
       <c r="I17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="J17" s="26"/>
       <c r="K17" s="262"/>
@@ -4198,7 +4211,7 @@
       <c r="R17" s="272" t="s">
         <v>271</v>
       </c>
-      <c r="S17" s="293"/>
+      <c r="S17" s="308"/>
       <c r="T17" s="265" t="s">
         <v>284</v>
       </c>
@@ -4213,7 +4226,7 @@
       <c r="AC17" s="15"/>
       <c r="AD17" s="115"/>
       <c r="AE17" s="50"/>
-      <c r="AF17" s="307"/>
+      <c r="AF17" s="294"/>
       <c r="AG17" s="25"/>
       <c r="AH17" s="25"/>
       <c r="AI17" s="24" t="s">
@@ -4229,10 +4242,10 @@
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="298" t="s">
+      <c r="E18" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="299"/>
+      <c r="F18" s="314"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="J18" s="226"/>
@@ -4241,16 +4254,16 @@
         <v>269</v>
       </c>
       <c r="M18" s="278"/>
-      <c r="N18" s="291" t="s">
+      <c r="N18" s="306" t="s">
         <v>313</v>
       </c>
-      <c r="O18" s="312" t="s">
+      <c r="O18" s="299" t="s">
         <v>305</v>
       </c>
-      <c r="P18" s="312"/>
-      <c r="Q18" s="313"/>
+      <c r="P18" s="299"/>
+      <c r="Q18" s="300"/>
       <c r="R18" s="161"/>
-      <c r="S18" s="293"/>
+      <c r="S18" s="308"/>
       <c r="T18" s="17"/>
       <c r="Y18" s="25" t="s">
         <v>286</v>
@@ -4262,7 +4275,7 @@
         <v>254</v>
       </c>
       <c r="AD18" s="24"/>
-      <c r="AF18" s="307"/>
+      <c r="AF18" s="294"/>
       <c r="AG18" s="25"/>
       <c r="AH18" s="25"/>
       <c r="AI18" s="24" t="s">
@@ -4279,18 +4292,18 @@
         <v>288</v>
       </c>
       <c r="M19" s="119"/>
-      <c r="N19" s="292"/>
+      <c r="N19" s="307"/>
       <c r="O19" s="279" t="s">
         <v>311</v>
       </c>
-      <c r="P19" s="303" t="s">
+      <c r="P19" s="318" t="s">
         <v>290</v>
       </c>
-      <c r="Q19" s="303"/>
-      <c r="R19" s="304" t="s">
+      <c r="Q19" s="318"/>
+      <c r="R19" s="319" t="s">
         <v>277</v>
       </c>
-      <c r="S19" s="304"/>
+      <c r="S19" s="319"/>
       <c r="T19" s="17"/>
       <c r="Z19" s="25" t="s">
         <v>244</v>
@@ -4302,7 +4315,7 @@
       <c r="AC19" s="79"/>
       <c r="AD19" s="115"/>
       <c r="AE19" s="50"/>
-      <c r="AF19" s="307"/>
+      <c r="AF19" s="294"/>
       <c r="AG19" s="25"/>
       <c r="AH19" s="25"/>
       <c r="AI19" s="24" t="s">
@@ -4320,9 +4333,7 @@
       <c r="F20" s="65"/>
       <c r="G20" s="286"/>
       <c r="J20" s="227"/>
-      <c r="L20" s="169" t="s">
-        <v>272</v>
-      </c>
+      <c r="L20" s="169"/>
       <c r="M20" s="119"/>
       <c r="N20" s="231" t="s">
         <v>313</v>
@@ -4349,7 +4360,7 @@
       <c r="AC20" s="258"/>
       <c r="AD20" s="257"/>
       <c r="AE20" s="256"/>
-      <c r="AF20" s="307"/>
+      <c r="AF20" s="294"/>
       <c r="AG20" s="25"/>
       <c r="AH20" s="25"/>
       <c r="AI20" s="24" t="s">
@@ -4363,10 +4374,10 @@
       <c r="O21" s="272" t="s">
         <v>312</v>
       </c>
-      <c r="P21" s="305" t="s">
+      <c r="P21" s="292" t="s">
         <v>291</v>
       </c>
-      <c r="Q21" s="305"/>
+      <c r="Q21" s="292"/>
       <c r="R21" s="266"/>
       <c r="S21" s="17"/>
       <c r="T21" s="265" t="s">
@@ -4385,7 +4396,7 @@
       <c r="AC21" s="15"/>
       <c r="AD21" s="109"/>
       <c r="AE21" s="43"/>
-      <c r="AF21" s="307"/>
+      <c r="AF21" s="294"/>
       <c r="AG21" s="25"/>
       <c r="AH21" s="25"/>
       <c r="AI21" s="24" t="s">
@@ -4416,7 +4427,7 @@
       <c r="AE22">
         <v>1</v>
       </c>
-      <c r="AF22" s="307"/>
+      <c r="AF22" s="294"/>
       <c r="AG22" s="25" t="s">
         <v>298</v>
       </c>
@@ -4441,7 +4452,7 @@
       <c r="AC23" s="116"/>
       <c r="AD23" s="115"/>
       <c r="AE23" s="50"/>
-      <c r="AF23" s="307"/>
+      <c r="AF23" s="294"/>
       <c r="AG23" s="25"/>
       <c r="AH23" s="25"/>
       <c r="AI23" s="24" t="s">
@@ -4452,7 +4463,7 @@
       <c r="L24" s="169" t="s">
         <v>222</v>
       </c>
-      <c r="R24" s="309" t="s">
+      <c r="R24" s="296" t="s">
         <v>302</v>
       </c>
       <c r="S24" s="265">
@@ -4471,7 +4482,7 @@
       <c r="AC24" s="258"/>
       <c r="AD24" s="257"/>
       <c r="AE24" s="256"/>
-      <c r="AF24" s="307"/>
+      <c r="AF24" s="294"/>
       <c r="AG24" s="25"/>
       <c r="AH24" s="25"/>
       <c r="AI24" s="24" t="s">
@@ -4485,10 +4496,13 @@
       <c r="K25" s="231" t="s">
         <v>308</v>
       </c>
+      <c r="L25" s="169" t="s">
+        <v>316</v>
+      </c>
       <c r="M25" s="231" t="s">
         <v>307</v>
       </c>
-      <c r="R25" s="310"/>
+      <c r="R25" s="297"/>
       <c r="S25" s="265">
         <v>1</v>
       </c>
@@ -4508,7 +4522,7 @@
       <c r="AC25" s="258"/>
       <c r="AD25" s="257"/>
       <c r="AE25" s="256"/>
-      <c r="AF25" s="307"/>
+      <c r="AF25" s="294"/>
       <c r="AG25" s="25"/>
       <c r="AH25" s="25"/>
       <c r="AI25" s="24" t="s">
@@ -4519,7 +4533,7 @@
       <c r="L26" s="169" t="s">
         <v>289</v>
       </c>
-      <c r="R26" s="311"/>
+      <c r="R26" s="298"/>
       <c r="S26" s="265">
         <v>1</v>
       </c>
@@ -4532,7 +4546,7 @@
       <c r="AA26" s="169" t="s">
         <v>260</v>
       </c>
-      <c r="AF26" s="307"/>
+      <c r="AF26" s="294"/>
     </row>
     <row r="27" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J27" s="25">
@@ -4551,7 +4565,7 @@
       <c r="AA27" s="169" t="s">
         <v>295</v>
       </c>
-      <c r="AF27" s="307"/>
+      <c r="AF27" s="294"/>
     </row>
     <row r="28" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AA28" s="169" t="s">
@@ -4562,10 +4576,10 @@
         <v>2</v>
       </c>
       <c r="AD28" s="288"/>
-      <c r="AE28" s="363">
+      <c r="AE28" s="291">
         <v>1</v>
       </c>
-      <c r="AF28" s="308"/>
+      <c r="AF28" s="295"/>
       <c r="AG28" s="25" t="s">
         <v>30</v>
       </c>
@@ -4578,12 +4592,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="AF3:AF28"/>
-    <mergeCell ref="R24:R26"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="N18:N19"/>
     <mergeCell ref="S17:S18"/>
     <mergeCell ref="A3:A4"/>
@@ -4592,6 +4600,12 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="P19:Q19"/>
     <mergeCell ref="R19:S19"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="AF3:AF28"/>
+    <mergeCell ref="R24:R26"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4690,8 +4704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4715,18 +4729,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="323" t="s">
+      <c r="E1" s="331" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="325"/>
+      <c r="F1" s="333"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="323" t="s">
+      <c r="H1" s="331" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="324"/>
-      <c r="J1" s="325"/>
+      <c r="I1" s="332"/>
+      <c r="J1" s="333"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4744,7 +4758,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="326">
+      <c r="B2" s="328">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4771,26 +4785,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="341">
+      <c r="K2" s="323">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="339">
+      <c r="L2" s="342">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="329">
+      <c r="M2" s="334">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
         <f>SUM(E2:J68)</f>
-        <v>11638</v>
+        <v>11693</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="327"/>
+      <c r="B3" s="330"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4805,13 +4819,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="342"/>
-      <c r="L3" s="293"/>
-      <c r="M3" s="330"/>
+      <c r="K3" s="324"/>
+      <c r="L3" s="308"/>
+      <c r="M3" s="335"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="328"/>
+      <c r="B4" s="329"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -4826,9 +4840,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="342"/>
-      <c r="L4" s="293"/>
-      <c r="M4" s="330"/>
+      <c r="K4" s="324"/>
+      <c r="L4" s="308"/>
+      <c r="M4" s="335"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4910,7 +4924,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="331">
+      <c r="B7" s="320">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4927,22 +4941,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="333">
+      <c r="K7" s="336">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="335">
+      <c r="L7" s="338">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="337">
+      <c r="M7" s="340">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="332"/>
+      <c r="B8" s="322"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4963,9 +4977,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="334"/>
-      <c r="L8" s="336"/>
-      <c r="M8" s="338"/>
+      <c r="K8" s="337"/>
+      <c r="L8" s="339"/>
+      <c r="M8" s="341"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -5045,7 +5059,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="331">
+      <c r="B11" s="320">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -5072,7 +5086,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="332"/>
+      <c r="B12" s="322"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -5129,7 +5143,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="331">
+      <c r="B14" s="320">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -5152,7 +5166,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="332"/>
+      <c r="B15" s="322"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -5176,7 +5190,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="326">
+      <c r="B16" s="328">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -5207,7 +5221,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="327"/>
+      <c r="B17" s="330"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -5225,7 +5239,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="326">
+      <c r="B18" s="328">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -5254,7 +5268,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="328"/>
+      <c r="B19" s="329"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -5314,7 +5328,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="343">
+      <c r="B21" s="326">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -5342,7 +5356,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="344"/>
+      <c r="B22" s="327"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -5394,7 +5408,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="296">
+      <c r="B24" s="311">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -5423,7 +5437,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="297"/>
+      <c r="B25" s="312"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -5451,7 +5465,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="296">
+      <c r="B26" s="311">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -5482,7 +5496,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="322"/>
+      <c r="B27" s="325"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5513,7 +5527,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="296">
+      <c r="B28" s="311">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -5535,7 +5549,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="297"/>
+      <c r="B29" s="312"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -5561,7 +5575,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="296">
+      <c r="B30" s="311">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -5584,7 +5598,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="297"/>
+      <c r="B31" s="312"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -5611,7 +5625,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="296">
+      <c r="B32" s="311">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -5633,7 +5647,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="297"/>
+      <c r="B33" s="312"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -5686,7 +5700,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="296">
+      <c r="B35" s="311">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -5713,7 +5727,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="297"/>
+      <c r="B36" s="312"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -5735,7 +5749,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="296">
+      <c r="B37" s="311">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -5768,7 +5782,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="297"/>
+      <c r="B38" s="312"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -5786,7 +5800,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="296">
+      <c r="B39" s="311">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -5813,7 +5827,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="322"/>
+      <c r="B40" s="325"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5841,7 +5855,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="296">
+      <c r="B41" s="311">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -5868,7 +5882,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="322"/>
+      <c r="B42" s="325"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5886,7 +5900,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="297"/>
+      <c r="B43" s="312"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -5915,7 +5929,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="296">
+      <c r="B44" s="311">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -5941,7 +5955,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="297"/>
+      <c r="B45" s="312"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -5966,7 +5980,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="296">
+      <c r="B46" s="311">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -5988,7 +6002,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="322"/>
+      <c r="B47" s="325"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -6009,7 +6023,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="296">
+      <c r="B48" s="311">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -6029,7 +6043,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="322"/>
+      <c r="B49" s="325"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -6055,7 +6069,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="322"/>
+      <c r="B50" s="325"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -6082,7 +6096,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="296">
+      <c r="B51" s="311">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -6104,7 +6118,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="297"/>
+      <c r="B52" s="312"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -6137,7 +6151,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="296">
+      <c r="B53" s="311">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -6167,7 +6181,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="322"/>
+      <c r="B54" s="325"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -6194,7 +6208,7 @@
       <c r="A55" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="296">
+      <c r="B55" s="311">
         <v>31</v>
       </c>
       <c r="C55" s="96"/>
@@ -6222,7 +6236,7 @@
       <c r="M55" s="82"/>
     </row>
     <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="297"/>
+      <c r="B56" s="312"/>
       <c r="C56" s="96"/>
       <c r="D56" s="82"/>
       <c r="E56" s="82">
@@ -6248,7 +6262,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="319">
+      <c r="B57" s="343">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -6268,7 +6282,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="320"/>
+      <c r="B58" s="344"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -6297,7 +6311,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="321"/>
+      <c r="B59" s="345"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -6323,7 +6337,7 @@
       <c r="M59" s="18"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="296">
+      <c r="B60" s="311">
         <v>2</v>
       </c>
       <c r="C60" s="142"/>
@@ -6349,7 +6363,7 @@
       <c r="M60" s="18"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="322"/>
+      <c r="B61" s="325"/>
       <c r="C61" s="142"/>
       <c r="D61" s="18">
         <v>240</v>
@@ -6375,7 +6389,7 @@
       <c r="M61" s="18"/>
     </row>
     <row r="62" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="297"/>
+      <c r="B62" s="312"/>
       <c r="C62" s="142"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
@@ -6396,7 +6410,7 @@
       <c r="A63" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="331">
+      <c r="B63" s="320">
         <v>3</v>
       </c>
       <c r="C63" s="142"/>
@@ -6418,7 +6432,7 @@
       <c r="M63" s="18"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="340"/>
+      <c r="B64" s="321"/>
       <c r="C64" s="142"/>
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
@@ -6438,7 +6452,7 @@
       <c r="M64" s="18"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="340"/>
+      <c r="B65" s="321"/>
       <c r="C65" s="142"/>
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
@@ -6460,7 +6474,7 @@
       <c r="M65" s="18"/>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="340"/>
+      <c r="B66" s="321"/>
       <c r="C66" s="142"/>
       <c r="D66" s="18">
         <v>500</v>
@@ -6488,7 +6502,7 @@
       <c r="M66" s="18"/>
     </row>
     <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="332"/>
+      <c r="B67" s="322"/>
       <c r="C67" s="142"/>
       <c r="D67" s="18"/>
       <c r="E67" s="18"/>
@@ -6511,9 +6525,13 @@
       <c r="D68" s="18"/>
       <c r="E68" s="18"/>
       <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
+      <c r="G68" s="18">
+        <v>40</v>
+      </c>
       <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
+      <c r="I68" s="18">
+        <v>15</v>
+      </c>
       <c r="J68" s="18">
         <v>5</v>
       </c>
@@ -6523,6 +6541,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L2:L4"/>
     <mergeCell ref="B63:B67"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="B32:B33"/>
@@ -6539,23 +6574,6 @@
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="B60:B62"/>
     <mergeCell ref="B35:B36"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B46:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9762,10 +9780,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="298" t="s">
+      <c r="AG24" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="299"/>
+      <c r="AH24" s="314"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -9785,10 +9803,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="298" t="s">
+      <c r="AZ24" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="299"/>
+      <c r="BA24" s="314"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -9808,10 +9826,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="298" t="s">
+      <c r="BR24" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="299"/>
+      <c r="BS24" s="314"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -9834,10 +9852,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="300" t="s">
+      <c r="B26" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="302"/>
+      <c r="C26" s="317"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9874,10 +9892,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="300" t="s">
+      <c r="R26" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="302"/>
+      <c r="S26" s="317"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9914,10 +9932,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="300" t="s">
+      <c r="AG26" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="302"/>
+      <c r="AH26" s="317"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9954,10 +9972,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="300" t="s">
+      <c r="AW26" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="302"/>
+      <c r="AX26" s="317"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9994,10 +10012,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="300" t="s">
+      <c r="BM26" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="302"/>
+      <c r="BN26" s="317"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -10991,7 +11009,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="352">
+      <c r="AX32" s="358">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -11029,7 +11047,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="352">
+      <c r="BN32" s="358">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -11178,7 +11196,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="353"/>
+      <c r="AX33" s="359"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -11214,7 +11232,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="353"/>
+      <c r="BN33" s="359"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -11365,7 +11383,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="354"/>
+      <c r="AX34" s="360"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11403,7 +11421,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="354"/>
+      <c r="BN34" s="360"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11634,10 +11652,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="298" t="s">
+      <c r="B36" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="299"/>
+      <c r="C36" s="314"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -11655,10 +11673,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="298" t="s">
+      <c r="R36" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="299"/>
+      <c r="S36" s="314"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -11676,10 +11694,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="298" t="s">
+      <c r="AG36" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="299"/>
+      <c r="AH36" s="314"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -11697,10 +11715,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="298" t="s">
+      <c r="AW36" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="299"/>
+      <c r="AX36" s="314"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -11718,10 +11736,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="298" t="s">
+      <c r="BM36" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="299"/>
+      <c r="BN36" s="314"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -11741,10 +11759,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="300" t="s">
+      <c r="B38" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="302"/>
+      <c r="C38" s="317"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11784,10 +11802,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="300" t="s">
+      <c r="S38" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="302"/>
+      <c r="T38" s="317"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11827,11 +11845,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="300" t="s">
+      <c r="AJ38" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="301"/>
-      <c r="AL38" s="302"/>
+      <c r="AK38" s="316"/>
+      <c r="AL38" s="317"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11876,11 +11894,11 @@
         <f ca="1">TODAY()</f>
         <v>45295</v>
       </c>
-      <c r="BD38" s="300" t="s">
+      <c r="BD38" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="301"/>
-      <c r="BF38" s="302"/>
+      <c r="BE38" s="316"/>
+      <c r="BF38" s="317"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11920,11 +11938,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="300" t="s">
+      <c r="BW38" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="301"/>
-      <c r="BY38" s="302"/>
+      <c r="BX38" s="316"/>
+      <c r="BY38" s="317"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -12876,7 +12894,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="352">
+      <c r="C44" s="358">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12914,10 +12932,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="361">
+      <c r="S44" s="351">
         <v>25</v>
       </c>
-      <c r="T44" s="352">
+      <c r="T44" s="358">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12926,7 +12944,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="355" t="s">
+      <c r="W44" s="353" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12955,10 +12973,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="361">
+      <c r="AJ44" s="351">
         <v>50</v>
       </c>
-      <c r="AK44" s="352">
+      <c r="AK44" s="358">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12968,7 +12986,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="355" t="s">
+      <c r="AO44" s="353" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -12998,7 +13016,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="361">
+      <c r="BD44" s="351">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -13009,7 +13027,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="355" t="s">
+      <c r="BI44" s="353" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -13038,7 +13056,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="361">
+      <c r="BW44" s="351">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -13049,7 +13067,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="355" t="s">
+      <c r="CB44" s="353" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -13081,7 +13099,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="353"/>
+      <c r="C45" s="359"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -13115,15 +13133,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="362"/>
-      <c r="T45" s="354"/>
+      <c r="S45" s="352"/>
+      <c r="T45" s="360"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="356"/>
+      <c r="W45" s="354"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13150,8 +13168,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="362"/>
-      <c r="AK45" s="354"/>
+      <c r="AJ45" s="352"/>
+      <c r="AK45" s="360"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -13159,7 +13177,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="356"/>
+      <c r="AO45" s="354"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13187,7 +13205,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="362"/>
+      <c r="BD45" s="352"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -13198,7 +13216,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="356"/>
+      <c r="BI45" s="354"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13225,7 +13243,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="362"/>
+      <c r="BW45" s="352"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -13234,7 +13252,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="356"/>
+      <c r="CB45" s="354"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13264,7 +13282,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="354"/>
+      <c r="C46" s="360"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13691,10 +13709,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="298" t="s">
+      <c r="B48" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="299"/>
+      <c r="C48" s="314"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -13713,10 +13731,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="298" t="s">
+      <c r="S48" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="299"/>
+      <c r="T48" s="314"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -13869,11 +13887,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="357"/>
+      <c r="AQ49" s="355"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="349"/>
-      <c r="AV49" s="350"/>
+      <c r="AU49" s="346"/>
+      <c r="AV49" s="347"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -13885,11 +13903,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="357"/>
+      <c r="BK49" s="355"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="349"/>
-      <c r="BP49" s="350"/>
+      <c r="BO49" s="346"/>
+      <c r="BP49" s="347"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -13900,20 +13918,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="357"/>
+      <c r="CD49" s="355"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="349"/>
-      <c r="CI49" s="350"/>
+      <c r="CH49" s="346"/>
+      <c r="CI49" s="347"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="298" t="s">
+      <c r="AJ50" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="299"/>
+      <c r="AK50" s="314"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -13924,19 +13942,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="357"/>
+      <c r="AQ50" s="355"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="349"/>
-      <c r="AV50" s="350"/>
+      <c r="AU50" s="346"/>
+      <c r="AV50" s="347"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="298" t="s">
+      <c r="BD50" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="299"/>
+      <c r="BE50" s="314"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -13945,18 +13963,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="357"/>
+      <c r="BK50" s="355"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="349"/>
-      <c r="BP50" s="350"/>
+      <c r="BO50" s="346"/>
+      <c r="BP50" s="347"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="298" t="s">
+      <c r="BW50" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="299"/>
+      <c r="BX50" s="314"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -13965,21 +13983,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="357"/>
+      <c r="CD50" s="355"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="349"/>
-      <c r="CI50" s="350"/>
+      <c r="CH50" s="346"/>
+      <c r="CI50" s="347"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="300" t="s">
+      <c r="B51" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="301"/>
-      <c r="D51" s="302"/>
+      <c r="C51" s="316"/>
+      <c r="D51" s="317"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -14029,14 +14047,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="358"/>
+      <c r="AQ51" s="356"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="359"/>
-      <c r="AV51" s="360"/>
+      <c r="AU51" s="357"/>
+      <c r="AV51" s="350"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -14048,14 +14066,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="358"/>
+      <c r="BK51" s="356"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="359"/>
-      <c r="BP51" s="360"/>
+      <c r="BO51" s="357"/>
+      <c r="BP51" s="350"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -14066,14 +14084,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="358"/>
+      <c r="CD51" s="356"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="359"/>
-      <c r="CI51" s="360"/>
+      <c r="CH51" s="357"/>
+      <c r="CI51" s="350"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -14094,11 +14112,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="300" t="s">
+      <c r="V52" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="301"/>
-      <c r="X52" s="302"/>
+      <c r="W52" s="316"/>
+      <c r="X52" s="317"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -14200,11 +14218,11 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="46"/>
-      <c r="AO53" s="300" t="s">
+      <c r="AO53" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="AP53" s="301"/>
-      <c r="AQ53" s="302"/>
+      <c r="AP53" s="316"/>
+      <c r="AQ53" s="317"/>
       <c r="AR53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14251,11 +14269,11 @@
         <f ca="1">TODAY()</f>
         <v>45295</v>
       </c>
-      <c r="BJ53" s="300" t="s">
+      <c r="BJ53" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="BK53" s="301"/>
-      <c r="BL53" s="302"/>
+      <c r="BK53" s="316"/>
+      <c r="BL53" s="317"/>
       <c r="BM53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14298,11 +14316,11 @@
       <c r="BZ53" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="CC53" s="300" t="s">
+      <c r="CC53" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="CD53" s="301"/>
-      <c r="CE53" s="302"/>
+      <c r="CD53" s="316"/>
+      <c r="CE53" s="317"/>
       <c r="CF53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14346,11 +14364,11 @@
         <v>108</v>
       </c>
       <c r="CV53" s="42"/>
-      <c r="CW53" s="300" t="s">
+      <c r="CW53" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="CX53" s="301"/>
-      <c r="CY53" s="302"/>
+      <c r="CX53" s="316"/>
+      <c r="CY53" s="317"/>
       <c r="CZ53" s="26" t="s">
         <v>43</v>
       </c>
@@ -17437,10 +17455,10 @@
       </c>
     </row>
     <row r="66" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="298" t="s">
+      <c r="B66" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="299"/>
+      <c r="C66" s="314"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -17453,8 +17471,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="349"/>
-      <c r="O66" s="350"/>
+      <c r="N66" s="346"/>
+      <c r="O66" s="347"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -17597,15 +17615,15 @@
       <c r="J67" s="348"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="349"/>
-      <c r="O67" s="350"/>
+      <c r="N67" s="346"/>
+      <c r="O67" s="347"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="298" t="s">
+      <c r="V67" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="299"/>
+      <c r="W67" s="314"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -17617,8 +17635,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="349"/>
-      <c r="AI67" s="350"/>
+      <c r="AH67" s="346"/>
+      <c r="AI67" s="347"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -17689,7 +17707,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="351"/>
+      <c r="J68" s="349"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -17707,15 +17725,15 @@
       <c r="AC68" s="119"/>
       <c r="AD68" s="348"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="349"/>
-      <c r="AI68" s="350"/>
+      <c r="AH68" s="346"/>
+      <c r="AI68" s="347"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
-      <c r="AO68" s="298" t="s">
+      <c r="AO68" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="AP68" s="299"/>
+      <c r="AP68" s="314"/>
       <c r="AQ68" s="189"/>
       <c r="AR68" s="9">
         <f>SUM(AO55:AQ66)</f>
@@ -17727,15 +17745,15 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="349"/>
-      <c r="BB68" s="350"/>
+      <c r="BA68" s="346"/>
+      <c r="BB68" s="347"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
-      <c r="BJ68" s="298" t="s">
+      <c r="BJ68" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="BK68" s="299"/>
+      <c r="BK68" s="314"/>
       <c r="BL68" s="189"/>
       <c r="BM68" s="9">
         <f>SUM(BJ55:BL66)</f>
@@ -17747,15 +17765,15 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="349"/>
-      <c r="BW68" s="350"/>
+      <c r="BV68" s="346"/>
+      <c r="BW68" s="347"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
       <c r="BZ68" s="46"/>
-      <c r="CC68" s="298" t="s">
+      <c r="CC68" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="CD68" s="299"/>
+      <c r="CD68" s="314"/>
       <c r="CE68" s="189"/>
       <c r="CF68" s="9">
         <f>SUM(CC55:CE66)</f>
@@ -17767,16 +17785,16 @@
       <c r="CJ68" s="119"/>
       <c r="CK68" s="117"/>
       <c r="CN68" s="2"/>
-      <c r="CO68" s="349"/>
-      <c r="CP68" s="350"/>
+      <c r="CO68" s="346"/>
+      <c r="CP68" s="347"/>
       <c r="CQ68" s="1"/>
       <c r="CR68" s="1"/>
       <c r="CS68" s="46"/>
       <c r="CV68" s="110"/>
-      <c r="CW68" s="298" t="s">
+      <c r="CW68" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="CX68" s="299"/>
+      <c r="CX68" s="314"/>
       <c r="CY68" s="189"/>
       <c r="CZ68" s="9">
         <f>SUM(CW55:CY66)</f>
@@ -17795,7 +17813,7 @@
       <c r="DI68" s="159" t="s">
         <v>271</v>
       </c>
-      <c r="DJ68" s="293"/>
+      <c r="DJ68" s="308"/>
       <c r="DK68" s="265" t="s">
         <v>284</v>
       </c>
@@ -17814,7 +17832,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="351"/>
+      <c r="AD69" s="349"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -17832,8 +17850,8 @@
       <c r="AV69" s="119"/>
       <c r="AW69" s="348"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="349"/>
-      <c r="BB69" s="350"/>
+      <c r="BA69" s="346"/>
+      <c r="BB69" s="347"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
@@ -17846,8 +17864,8 @@
       <c r="BQ69" s="119"/>
       <c r="BR69" s="348"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="349"/>
-      <c r="BW69" s="350"/>
+      <c r="BV69" s="346"/>
+      <c r="BW69" s="347"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
       <c r="BZ69" s="46"/>
@@ -17860,8 +17878,8 @@
       <c r="CJ69" s="119"/>
       <c r="CK69" s="348"/>
       <c r="CN69" s="2"/>
-      <c r="CO69" s="349"/>
-      <c r="CP69" s="350"/>
+      <c r="CO69" s="346"/>
+      <c r="CP69" s="347"/>
       <c r="CQ69" s="1"/>
       <c r="CR69" s="1"/>
       <c r="CS69" s="46"/>
@@ -17880,7 +17898,7 @@
       <c r="DG69" s="18"/>
       <c r="DH69" s="264"/>
       <c r="DI69" s="159"/>
-      <c r="DJ69" s="293"/>
+      <c r="DJ69" s="308"/>
       <c r="DK69" s="17"/>
       <c r="DL69" s="1"/>
       <c r="DM69" s="46"/>
@@ -17922,7 +17940,7 @@
       <c r="CH70" s="137"/>
       <c r="CI70" s="203"/>
       <c r="CJ70" s="201"/>
-      <c r="CK70" s="351"/>
+      <c r="CK70" s="349"/>
       <c r="CL70" s="50"/>
       <c r="CM70" s="50"/>
       <c r="CN70" s="79"/>
@@ -17943,24 +17961,24 @@
       <c r="DF70" s="159" t="s">
         <v>275</v>
       </c>
-      <c r="DG70" s="305" t="s">
+      <c r="DG70" s="292" t="s">
         <v>290</v>
       </c>
-      <c r="DH70" s="305"/>
-      <c r="DI70" s="304" t="s">
+      <c r="DH70" s="292"/>
+      <c r="DI70" s="319" t="s">
         <v>277</v>
       </c>
-      <c r="DJ70" s="304"/>
+      <c r="DJ70" s="319"/>
       <c r="DK70" s="17"/>
       <c r="DL70" s="1"/>
       <c r="DM70" s="46"/>
     </row>
     <row r="71" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="300" t="s">
+      <c r="B71" s="315" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="301"/>
-      <c r="D71" s="302"/>
+      <c r="C71" s="316"/>
+      <c r="D71" s="317"/>
       <c r="E71" s="281"/>
       <c r="F71" s="26" t="s">
         <v>43</v>
@@ -18093,10 +18111,10 @@
       <c r="DD72" s="137"/>
       <c r="DE72" s="137"/>
       <c r="DF72" s="5"/>
-      <c r="DG72" s="347" t="s">
+      <c r="DG72" s="361" t="s">
         <v>291</v>
       </c>
-      <c r="DH72" s="347"/>
+      <c r="DH72" s="361"/>
       <c r="DI72" s="268"/>
       <c r="DJ72" s="269"/>
       <c r="DK72" s="270" t="s">
@@ -18737,7 +18755,7 @@
       <c r="O86" s="272" t="s">
         <v>271</v>
       </c>
-      <c r="P86" s="293"/>
+      <c r="P86" s="308"/>
       <c r="Q86" s="265" t="s">
         <v>284</v>
       </c>
@@ -18745,10 +18763,10 @@
       <c r="S86" s="46"/>
     </row>
     <row r="87" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="298" t="s">
+      <c r="B87" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="299"/>
+      <c r="C87" s="314"/>
       <c r="D87" s="20"/>
       <c r="E87" s="20"/>
       <c r="G87" s="226"/>
@@ -18757,16 +18775,16 @@
         <v>269</v>
       </c>
       <c r="J87" s="278"/>
-      <c r="K87" s="291" t="s">
+      <c r="K87" s="306" t="s">
         <v>313</v>
       </c>
-      <c r="L87" s="312" t="s">
+      <c r="L87" s="299" t="s">
         <v>305</v>
       </c>
-      <c r="M87" s="312"/>
-      <c r="N87" s="313"/>
+      <c r="M87" s="299"/>
+      <c r="N87" s="300"/>
       <c r="O87" s="161"/>
-      <c r="P87" s="293"/>
+      <c r="P87" s="308"/>
       <c r="Q87" s="17"/>
       <c r="R87" s="1"/>
       <c r="S87" s="46"/>
@@ -18789,58 +18807,59 @@
         <v>288</v>
       </c>
       <c r="J88" s="201"/>
-      <c r="K88" s="292"/>
+      <c r="K88" s="307"/>
       <c r="L88" s="290" t="s">
         <v>311</v>
       </c>
-      <c r="M88" s="345" t="s">
+      <c r="M88" s="362" t="s">
         <v>290</v>
       </c>
-      <c r="N88" s="345"/>
-      <c r="O88" s="346" t="s">
+      <c r="N88" s="362"/>
+      <c r="O88" s="363" t="s">
         <v>277</v>
       </c>
-      <c r="P88" s="346"/>
+      <c r="P88" s="363"/>
       <c r="Q88" s="269"/>
       <c r="R88" s="65"/>
       <c r="S88" s="168"/>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="P86:P87"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="K87:K88"/>
+    <mergeCell ref="L87:N87"/>
+    <mergeCell ref="M88:N88"/>
+    <mergeCell ref="O88:P88"/>
+    <mergeCell ref="DG72:DH72"/>
+    <mergeCell ref="CW53:CY53"/>
+    <mergeCell ref="CW68:CX68"/>
+    <mergeCell ref="DJ68:DJ69"/>
+    <mergeCell ref="DE69:DE70"/>
+    <mergeCell ref="DG70:DH70"/>
+    <mergeCell ref="DI70:DJ70"/>
+    <mergeCell ref="CC53:CE53"/>
+    <mergeCell ref="CC68:CD68"/>
+    <mergeCell ref="CO68:CO69"/>
+    <mergeCell ref="CP68:CP69"/>
+    <mergeCell ref="CK69:CK70"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -18856,41 +18875,40 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="CC53:CE53"/>
-    <mergeCell ref="CC68:CD68"/>
-    <mergeCell ref="CO68:CO69"/>
-    <mergeCell ref="CP68:CP69"/>
-    <mergeCell ref="CK69:CK70"/>
-    <mergeCell ref="DG72:DH72"/>
-    <mergeCell ref="CW53:CY53"/>
-    <mergeCell ref="CW68:CX68"/>
-    <mergeCell ref="DJ68:DJ69"/>
-    <mergeCell ref="DE69:DE70"/>
-    <mergeCell ref="DG70:DH70"/>
-    <mergeCell ref="DI70:DJ70"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="P86:P87"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="K87:K88"/>
-    <mergeCell ref="L87:N87"/>
-    <mergeCell ref="M88:N88"/>
-    <mergeCell ref="O88:P88"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Updates_Afternoon_ S.1.0.1.1 _6:40PM
Boat Enabled -
InCapacity - [17,8,5,3,1,Cnt] ,
NodeW - [-3] ,
BirdW - [7][CityW-MundiaSahi] ,
FuelW_Day - ['22],
OnHost - [8+1]
VillageW=[0],
CityW=[] ,
[X-MarketShieldMatrix-X] = [6,2,8,2] = [Lx -3 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.1.0.xlsx
+++ b/Usage_S_1.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2E0525-55A7-4133-A6C5-0875D22D3FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F21F8D-35FE-4220-A055-6C391D3A38D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3213,7 +3213,7 @@
   <dimension ref="A1:AJ28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3469,7 +3469,9 @@
       <c r="D5" s="156">
         <v>-2</v>
       </c>
-      <c r="E5" s="218"/>
+      <c r="E5" s="218">
+        <v>10</v>
+      </c>
       <c r="F5" s="206"/>
       <c r="G5" s="127"/>
       <c r="H5" s="127"/>
@@ -3499,10 +3501,10 @@
         <v>86</v>
       </c>
       <c r="R5" s="154">
-        <v>0.83680555555555547</v>
+        <v>0.75</v>
       </c>
       <c r="T5" s="154">
-        <v>0.83680555555555547</v>
+        <v>0.75</v>
       </c>
       <c r="V5" s="245">
         <v>45295</v>
@@ -3529,7 +3531,9 @@
       <c r="C6">
         <v>4000</v>
       </c>
-      <c r="E6" s="218"/>
+      <c r="E6" s="218">
+        <v>20</v>
+      </c>
       <c r="F6" s="207"/>
       <c r="G6" s="127"/>
       <c r="H6" s="127"/>
@@ -3559,13 +3563,13 @@
         <v>69</v>
       </c>
       <c r="R6" s="154">
-        <v>0.98263888888888884</v>
+        <v>0.75</v>
       </c>
       <c r="T6" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.75</v>
       </c>
       <c r="V6" s="245">
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="Y6" s="25" t="s">
         <v>279</v>
@@ -3591,9 +3595,6 @@
       </c>
       <c r="B7" s="29">
         <v>0</v>
-      </c>
-      <c r="C7">
-        <v>52</v>
       </c>
       <c r="E7" s="165"/>
       <c r="F7" s="242"/>
@@ -3631,7 +3632,7 @@
         <v>0.73263888888888884</v>
       </c>
       <c r="V7" s="245">
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="Z7" s="25" t="s">
         <v>244</v>
@@ -3650,9 +3651,6 @@
       </c>
     </row>
     <row r="8" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8">
-        <v>125</v>
-      </c>
       <c r="E8" s="219"/>
       <c r="F8" s="242"/>
       <c r="G8" s="282"/>
@@ -3718,6 +3716,9 @@
         <f>7000+B6+B5-C2</f>
         <v>11703</v>
       </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
       <c r="E9" s="163"/>
       <c r="F9" s="165"/>
       <c r="G9" s="282"/>
@@ -3754,7 +3755,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="V9" s="245">
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="Z9" s="25" t="s">
         <v>257</v>
@@ -3844,7 +3845,10 @@
       </c>
       <c r="B11" s="8">
         <f>B9-B13</f>
-        <v>-30</v>
+        <v>-180</v>
+      </c>
+      <c r="C11">
+        <v>22</v>
       </c>
       <c r="E11" s="221"/>
       <c r="F11" s="242"/>
@@ -3904,7 +3908,9 @@
       </c>
     </row>
     <row r="12" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="165"/>
+      <c r="E12" s="165">
+        <v>120</v>
+      </c>
       <c r="F12" s="205"/>
       <c r="G12" s="164"/>
       <c r="H12" s="164"/>
@@ -3941,7 +3947,7 @@
         <v>0.83680555555555547</v>
       </c>
       <c r="V12" s="245">
-        <v>45294</v>
+        <v>45295</v>
       </c>
       <c r="Z12" s="25" t="s">
         <v>244</v>
@@ -3962,7 +3968,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>11733</v>
+        <v>11883</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="206"/>
@@ -4049,7 +4055,7 @@
       </c>
       <c r="K14" s="213"/>
       <c r="L14" s="169" t="s">
-        <v>318</v>
+        <v>273</v>
       </c>
       <c r="M14" s="83" t="s">
         <v>124</v>
@@ -4177,7 +4183,7 @@
       <c r="D17" s="25"/>
       <c r="E17" s="34">
         <f>SUM(E4:E15)</f>
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="F17" s="34">
         <f>SUM(F4:F15)</f>
@@ -4193,7 +4199,7 @@
       </c>
       <c r="I17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="J17" s="26"/>
       <c r="K17" s="262"/>
@@ -4705,7 +4711,7 @@
   <dimension ref="A1:T68"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="O67" sqref="O67"/>
+      <selection activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4799,7 +4805,7 @@
       </c>
       <c r="O2">
         <f>SUM(E2:J68)</f>
-        <v>11693</v>
+        <v>11843</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -6523,12 +6529,18 @@
       </c>
       <c r="C68" s="18"/>
       <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
+      <c r="E68" s="18">
+        <v>20</v>
+      </c>
+      <c r="F68" s="18">
+        <v>120</v>
+      </c>
       <c r="G68" s="18">
         <v>40</v>
       </c>
-      <c r="H68" s="18"/>
+      <c r="H68" s="18">
+        <v>10</v>
+      </c>
       <c r="I68" s="18">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Rw Updates_Afternoon_ S.1.0.1.2 _2:10PM
Boat Enabled -
InCapacity - [17,8,5,3,1,Cnt] ,
NodeW - [-3] ,
BirdW - [7][CityW-MundiaSahi] ,
FuelW_Day - ['22],
OnHost - [8+1]
VillageW=[0],
CityW=[] ,
[X-MarketShieldMatrix-X] = [6,2,8,2] = [Lx -3 , Bx - 4 ]

Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.1.0.xlsx
+++ b/Usage_S_1.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F21F8D-35FE-4220-A055-6C391D3A38D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8BF9F4-9937-4A3B-9273-8B530656D941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2720" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2850" uniqueCount="319">
   <si>
     <t>UnSettled</t>
   </si>
@@ -2000,7 +2000,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="364">
+  <cellXfs count="365">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2711,6 +2711,48 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2754,124 +2796,94 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2879,19 +2891,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2905,24 +2914,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3213,7 +3214,7 @@
   <dimension ref="A1:AJ28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3227,7 +3228,7 @@
     <col min="8" max="8" width="10.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="117" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="117" customWidth="1"/>
     <col min="12" max="12" width="22.28515625" style="192" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="117" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="117" bestFit="1" customWidth="1"/>
@@ -3253,7 +3254,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AA1" s="304" t="s">
+      <c r="AA1" s="318" t="s">
         <v>247</v>
       </c>
       <c r="AB1" s="36" t="s">
@@ -3268,12 +3269,12 @@
       <c r="AE1" s="249" t="s">
         <v>224</v>
       </c>
-      <c r="AG1" s="301" t="s">
+      <c r="AG1" s="315" t="s">
         <v>241</v>
       </c>
-      <c r="AH1" s="302"/>
-      <c r="AI1" s="302"/>
-      <c r="AJ1" s="303"/>
+      <c r="AH1" s="316"/>
+      <c r="AI1" s="316"/>
+      <c r="AJ1" s="317"/>
     </row>
     <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -3282,15 +3283,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="311">
+      <c r="C2" s="297">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="315" t="s">
+      <c r="E2" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="316"/>
-      <c r="G2" s="317"/>
+      <c r="F2" s="302"/>
+      <c r="G2" s="303"/>
       <c r="H2" s="281"/>
       <c r="I2" s="26" t="s">
         <v>43</v>
@@ -3336,13 +3337,13 @@
       </c>
       <c r="X2" s="98">
         <f ca="1">TODAY()</f>
-        <v>45295</v>
+        <v>45296</v>
       </c>
       <c r="Y2" s="8"/>
       <c r="Z2" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="AA2" s="305"/>
+      <c r="AA2" s="319"/>
       <c r="AB2" s="36">
         <f>SUM(AB3:AB19)</f>
         <v>6</v>
@@ -3371,13 +3372,13 @@
       <c r="AJ2" s="8"/>
     </row>
     <row r="3" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="309" t="s">
+      <c r="A3" s="295" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="312"/>
+      <c r="C3" s="298"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
@@ -3392,19 +3393,17 @@
       </c>
       <c r="AC3" s="253"/>
       <c r="AD3" s="109"/>
-      <c r="AF3" s="293"/>
+      <c r="AF3" s="307"/>
     </row>
     <row r="4" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="310"/>
+      <c r="A4" s="296"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="244">
-        <v>10</v>
-      </c>
+      <c r="E4" s="244"/>
       <c r="F4" s="205"/>
       <c r="G4" s="283"/>
       <c r="H4" s="283"/>
@@ -3417,9 +3416,7 @@
       <c r="K4" s="213" t="s">
         <v>187</v>
       </c>
-      <c r="L4" s="169" t="s">
-        <v>318</v>
-      </c>
+      <c r="L4" s="169"/>
       <c r="M4" s="83" t="s">
         <v>213</v>
       </c>
@@ -3436,7 +3433,7 @@
         <v>30</v>
       </c>
       <c r="R4" s="154">
-        <v>0.50347222222222221</v>
+        <v>0.75</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>130</v>
@@ -3455,7 +3452,7 @@
       </c>
       <c r="AC4" s="20"/>
       <c r="AD4" s="24"/>
-      <c r="AF4" s="294"/>
+      <c r="AF4" s="308"/>
       <c r="AG4" s="25"/>
       <c r="AH4" s="25"/>
       <c r="AI4" s="24" t="s">
@@ -3470,7 +3467,7 @@
         <v>-2</v>
       </c>
       <c r="E5" s="218">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F5" s="206"/>
       <c r="G5" s="127"/>
@@ -3484,7 +3481,9 @@
       <c r="K5" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="L5" s="169"/>
+      <c r="L5" s="169" t="s">
+        <v>318</v>
+      </c>
       <c r="M5" s="167" t="s">
         <v>142</v>
       </c>
@@ -3501,13 +3500,13 @@
         <v>86</v>
       </c>
       <c r="R5" s="154">
-        <v>0.75</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="T5" s="154">
-        <v>0.75</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="V5" s="245">
-        <v>45295</v>
+        <v>45296</v>
       </c>
       <c r="Z5" s="25" t="s">
         <v>244</v>
@@ -3517,7 +3516,7 @@
       </c>
       <c r="AC5" s="20"/>
       <c r="AD5" s="24"/>
-      <c r="AF5" s="294"/>
+      <c r="AF5" s="308"/>
       <c r="AG5" s="25"/>
       <c r="AH5" s="25"/>
       <c r="AI5" s="24" t="s">
@@ -3529,11 +3528,9 @@
         <v>4648</v>
       </c>
       <c r="C6">
-        <v>4000</v>
-      </c>
-      <c r="E6" s="218">
-        <v>20</v>
-      </c>
+        <v>3500</v>
+      </c>
+      <c r="E6" s="218"/>
       <c r="F6" s="207"/>
       <c r="G6" s="127"/>
       <c r="H6" s="127"/>
@@ -3585,7 +3582,7 @@
       </c>
       <c r="AC6" s="15"/>
       <c r="AD6" s="24"/>
-      <c r="AF6" s="294"/>
+      <c r="AF6" s="308"/>
       <c r="AG6" s="25"/>
       <c r="AI6" s="24"/>
     </row>
@@ -3596,7 +3593,12 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="165"/>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="E7" s="165">
+        <v>10</v>
+      </c>
       <c r="F7" s="242"/>
       <c r="G7" s="177"/>
       <c r="H7" s="177"/>
@@ -3609,7 +3611,9 @@
       <c r="K7" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="169"/>
+      <c r="L7" s="169" t="s">
+        <v>288</v>
+      </c>
       <c r="M7" s="83" t="s">
         <v>139</v>
       </c>
@@ -3643,7 +3647,7 @@
       <c r="AB7" s="26"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="24"/>
-      <c r="AF7" s="294"/>
+      <c r="AF7" s="308"/>
       <c r="AG7" s="25"/>
       <c r="AH7" s="25"/>
       <c r="AI7" s="24" t="s">
@@ -3701,7 +3705,7 @@
       <c r="AB8" s="25"/>
       <c r="AC8" s="15"/>
       <c r="AD8" s="24"/>
-      <c r="AF8" s="294"/>
+      <c r="AF8" s="308"/>
       <c r="AG8" s="25"/>
       <c r="AH8" s="25"/>
       <c r="AI8" s="24" t="s">
@@ -3715,9 +3719,6 @@
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
         <v>11703</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
       </c>
       <c r="E9" s="163"/>
       <c r="F9" s="165"/>
@@ -3766,7 +3767,7 @@
       <c r="AB9" s="25"/>
       <c r="AC9" s="15"/>
       <c r="AD9" s="24"/>
-      <c r="AF9" s="294"/>
+      <c r="AF9" s="308"/>
       <c r="AG9" s="25" t="s">
         <v>66</v>
       </c>
@@ -3778,9 +3779,10 @@
       </c>
     </row>
     <row r="10" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="220">
-        <v>10</v>
-      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="220"/>
       <c r="F10" s="206"/>
       <c r="G10" s="177"/>
       <c r="H10" s="177"/>
@@ -3832,7 +3834,7 @@
       </c>
       <c r="AC10" s="15"/>
       <c r="AD10" s="24"/>
-      <c r="AF10" s="294"/>
+      <c r="AF10" s="308"/>
       <c r="AG10" s="25"/>
       <c r="AH10" s="25"/>
       <c r="AI10" s="24">
@@ -3850,7 +3852,9 @@
       <c r="C11">
         <v>22</v>
       </c>
-      <c r="E11" s="221"/>
+      <c r="E11" s="221">
+        <v>10</v>
+      </c>
       <c r="F11" s="242"/>
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
@@ -3863,7 +3867,9 @@
       <c r="K11" s="213" t="s">
         <v>116</v>
       </c>
-      <c r="L11" s="169"/>
+      <c r="L11" s="194" t="s">
+        <v>300</v>
+      </c>
       <c r="M11" s="83" t="s">
         <v>124</v>
       </c>
@@ -3886,7 +3892,7 @@
         <v>0.50347222222222221</v>
       </c>
       <c r="V11" s="245">
-        <v>45295</v>
+        <v>45296</v>
       </c>
       <c r="Z11" s="25" t="s">
         <v>256</v>
@@ -3896,7 +3902,7 @@
       </c>
       <c r="AC11" s="15"/>
       <c r="AD11" s="24"/>
-      <c r="AF11" s="294"/>
+      <c r="AF11" s="308"/>
       <c r="AG11" s="25" t="s">
         <v>181</v>
       </c>
@@ -3909,7 +3915,7 @@
     </row>
     <row r="12" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="165">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="F12" s="205"/>
       <c r="G12" s="164"/>
@@ -3947,7 +3953,7 @@
         <v>0.83680555555555547</v>
       </c>
       <c r="V12" s="245">
-        <v>45295</v>
+        <v>45296</v>
       </c>
       <c r="Z12" s="25" t="s">
         <v>244</v>
@@ -3957,7 +3963,7 @@
       </c>
       <c r="AC12" s="15"/>
       <c r="AD12" s="271"/>
-      <c r="AF12" s="294"/>
+      <c r="AF12" s="308"/>
       <c r="AG12" s="25"/>
       <c r="AH12" s="25"/>
       <c r="AI12" s="24"/>
@@ -3970,7 +3976,9 @@
         <f>B18+Purchase!O2</f>
         <v>11883</v>
       </c>
-      <c r="E13" s="36"/>
+      <c r="E13" s="36">
+        <v>10</v>
+      </c>
       <c r="F13" s="206"/>
       <c r="G13" s="246"/>
       <c r="H13" s="246"/>
@@ -3983,7 +3991,9 @@
       <c r="K13" s="228" t="s">
         <v>313</v>
       </c>
-      <c r="L13" s="194"/>
+      <c r="L13" s="169" t="s">
+        <v>289</v>
+      </c>
       <c r="M13" s="183" t="s">
         <v>155</v>
       </c>
@@ -4000,17 +4010,17 @@
         <v>90</v>
       </c>
       <c r="R13" s="154">
-        <v>0.53125</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="S13"/>
       <c r="T13" s="154">
-        <v>0.53125</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="U13" s="261">
         <v>1</v>
       </c>
       <c r="V13" s="245">
-        <v>45294</v>
+        <v>45296</v>
       </c>
       <c r="Z13" s="25" t="s">
         <v>244</v>
@@ -4027,7 +4037,7 @@
       <c r="AE13">
         <v>1</v>
       </c>
-      <c r="AF13" s="294"/>
+      <c r="AF13" s="308"/>
       <c r="AG13" s="25" t="s">
         <v>65</v>
       </c>
@@ -4041,9 +4051,7 @@
     <row r="14" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="165">
-        <v>40</v>
-      </c>
+      <c r="E14" s="165"/>
       <c r="F14" s="205"/>
       <c r="G14" s="127"/>
       <c r="H14" s="127"/>
@@ -4097,7 +4105,7 @@
       <c r="AD14" s="241">
         <v>1</v>
       </c>
-      <c r="AF14" s="294"/>
+      <c r="AF14" s="308"/>
       <c r="AG14" s="25"/>
       <c r="AH14" s="25"/>
       <c r="AI14" s="24" t="s">
@@ -4146,7 +4154,7 @@
       </c>
       <c r="AC15" s="15"/>
       <c r="AD15" s="36"/>
-      <c r="AF15" s="294"/>
+      <c r="AF15" s="308"/>
       <c r="AG15" s="25" t="s">
         <v>66</v>
       </c>
@@ -4174,7 +4182,7 @@
         <v>239</v>
       </c>
       <c r="AD16" s="24"/>
-      <c r="AF16" s="294"/>
+      <c r="AF16" s="308"/>
       <c r="AG16" s="25"/>
       <c r="AI16" s="24"/>
     </row>
@@ -4183,7 +4191,7 @@
       <c r="D17" s="25"/>
       <c r="E17" s="34">
         <f>SUM(E4:E15)</f>
-        <v>210</v>
+        <v>70</v>
       </c>
       <c r="F17" s="34">
         <f>SUM(F4:F15)</f>
@@ -4193,13 +4201,10 @@
         <f>SUM(G4:G15)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="189">
-        <f>SUM(H4:H15)</f>
-        <v>0</v>
-      </c>
+      <c r="H17" s="189"/>
       <c r="I17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>210</v>
+        <v>70</v>
       </c>
       <c r="J17" s="26"/>
       <c r="K17" s="262"/>
@@ -4217,7 +4222,7 @@
       <c r="R17" s="272" t="s">
         <v>271</v>
       </c>
-      <c r="S17" s="308"/>
+      <c r="S17" s="294"/>
       <c r="T17" s="265" t="s">
         <v>284</v>
       </c>
@@ -4232,7 +4237,7 @@
       <c r="AC17" s="15"/>
       <c r="AD17" s="115"/>
       <c r="AE17" s="50"/>
-      <c r="AF17" s="294"/>
+      <c r="AF17" s="308"/>
       <c r="AG17" s="25"/>
       <c r="AH17" s="25"/>
       <c r="AI17" s="24" t="s">
@@ -4248,10 +4253,10 @@
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="313" t="s">
+      <c r="E18" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="314"/>
+      <c r="F18" s="300"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="J18" s="226"/>
@@ -4260,16 +4265,16 @@
         <v>269</v>
       </c>
       <c r="M18" s="278"/>
-      <c r="N18" s="306" t="s">
+      <c r="N18" s="292" t="s">
         <v>313</v>
       </c>
-      <c r="O18" s="299" t="s">
+      <c r="O18" s="313" t="s">
         <v>305</v>
       </c>
-      <c r="P18" s="299"/>
-      <c r="Q18" s="300"/>
+      <c r="P18" s="313"/>
+      <c r="Q18" s="314"/>
       <c r="R18" s="161"/>
-      <c r="S18" s="308"/>
+      <c r="S18" s="294"/>
       <c r="T18" s="17"/>
       <c r="Y18" s="25" t="s">
         <v>286</v>
@@ -4281,7 +4286,7 @@
         <v>254</v>
       </c>
       <c r="AD18" s="24"/>
-      <c r="AF18" s="294"/>
+      <c r="AF18" s="308"/>
       <c r="AG18" s="25"/>
       <c r="AH18" s="25"/>
       <c r="AI18" s="24" t="s">
@@ -4292,24 +4297,29 @@
       <c r="E19" s="284"/>
       <c r="F19" s="59"/>
       <c r="G19" s="285"/>
-      <c r="I19" s="1"/>
+      <c r="H19" s="2">
+        <v>220</v>
+      </c>
+      <c r="I19" s="1">
+        <v>280</v>
+      </c>
       <c r="J19" s="226"/>
       <c r="L19" s="169" t="s">
         <v>288</v>
       </c>
       <c r="M19" s="119"/>
-      <c r="N19" s="307"/>
+      <c r="N19" s="293"/>
       <c r="O19" s="279" t="s">
         <v>311</v>
       </c>
-      <c r="P19" s="318" t="s">
+      <c r="P19" s="304" t="s">
         <v>290</v>
       </c>
-      <c r="Q19" s="318"/>
-      <c r="R19" s="319" t="s">
+      <c r="Q19" s="304"/>
+      <c r="R19" s="305" t="s">
         <v>277</v>
       </c>
-      <c r="S19" s="319"/>
+      <c r="S19" s="305"/>
       <c r="T19" s="17"/>
       <c r="Z19" s="25" t="s">
         <v>244</v>
@@ -4321,7 +4331,7 @@
       <c r="AC19" s="79"/>
       <c r="AD19" s="115"/>
       <c r="AE19" s="50"/>
-      <c r="AF19" s="294"/>
+      <c r="AF19" s="308"/>
       <c r="AG19" s="25"/>
       <c r="AH19" s="25"/>
       <c r="AI19" s="24" t="s">
@@ -4366,7 +4376,7 @@
       <c r="AC20" s="258"/>
       <c r="AD20" s="257"/>
       <c r="AE20" s="256"/>
-      <c r="AF20" s="294"/>
+      <c r="AF20" s="308"/>
       <c r="AG20" s="25"/>
       <c r="AH20" s="25"/>
       <c r="AI20" s="24" t="s">
@@ -4380,10 +4390,10 @@
       <c r="O21" s="272" t="s">
         <v>312</v>
       </c>
-      <c r="P21" s="292" t="s">
+      <c r="P21" s="306" t="s">
         <v>291</v>
       </c>
-      <c r="Q21" s="292"/>
+      <c r="Q21" s="306"/>
       <c r="R21" s="266"/>
       <c r="S21" s="17"/>
       <c r="T21" s="265" t="s">
@@ -4402,7 +4412,7 @@
       <c r="AC21" s="15"/>
       <c r="AD21" s="109"/>
       <c r="AE21" s="43"/>
-      <c r="AF21" s="294"/>
+      <c r="AF21" s="308"/>
       <c r="AG21" s="25"/>
       <c r="AH21" s="25"/>
       <c r="AI21" s="24" t="s">
@@ -4433,7 +4443,7 @@
       <c r="AE22">
         <v>1</v>
       </c>
-      <c r="AF22" s="294"/>
+      <c r="AF22" s="308"/>
       <c r="AG22" s="25" t="s">
         <v>298</v>
       </c>
@@ -4458,7 +4468,7 @@
       <c r="AC23" s="116"/>
       <c r="AD23" s="115"/>
       <c r="AE23" s="50"/>
-      <c r="AF23" s="294"/>
+      <c r="AF23" s="308"/>
       <c r="AG23" s="25"/>
       <c r="AH23" s="25"/>
       <c r="AI23" s="24" t="s">
@@ -4469,7 +4479,7 @@
       <c r="L24" s="169" t="s">
         <v>222</v>
       </c>
-      <c r="R24" s="296" t="s">
+      <c r="R24" s="310" t="s">
         <v>302</v>
       </c>
       <c r="S24" s="265">
@@ -4488,7 +4498,7 @@
       <c r="AC24" s="258"/>
       <c r="AD24" s="257"/>
       <c r="AE24" s="256"/>
-      <c r="AF24" s="294"/>
+      <c r="AF24" s="308"/>
       <c r="AG24" s="25"/>
       <c r="AH24" s="25"/>
       <c r="AI24" s="24" t="s">
@@ -4508,7 +4518,7 @@
       <c r="M25" s="231" t="s">
         <v>307</v>
       </c>
-      <c r="R25" s="297"/>
+      <c r="R25" s="311"/>
       <c r="S25" s="265">
         <v>1</v>
       </c>
@@ -4528,7 +4538,7 @@
       <c r="AC25" s="258"/>
       <c r="AD25" s="257"/>
       <c r="AE25" s="256"/>
-      <c r="AF25" s="294"/>
+      <c r="AF25" s="308"/>
       <c r="AG25" s="25"/>
       <c r="AH25" s="25"/>
       <c r="AI25" s="24" t="s">
@@ -4539,7 +4549,7 @@
       <c r="L26" s="169" t="s">
         <v>289</v>
       </c>
-      <c r="R26" s="298"/>
+      <c r="R26" s="312"/>
       <c r="S26" s="265">
         <v>1</v>
       </c>
@@ -4552,7 +4562,7 @@
       <c r="AA26" s="169" t="s">
         <v>260</v>
       </c>
-      <c r="AF26" s="294"/>
+      <c r="AF26" s="308"/>
     </row>
     <row r="27" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J27" s="25">
@@ -4571,7 +4581,7 @@
       <c r="AA27" s="169" t="s">
         <v>295</v>
       </c>
-      <c r="AF27" s="294"/>
+      <c r="AF27" s="308"/>
     </row>
     <row r="28" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AA28" s="169" t="s">
@@ -4585,7 +4595,7 @@
       <c r="AE28" s="291">
         <v>1</v>
       </c>
-      <c r="AF28" s="295"/>
+      <c r="AF28" s="309"/>
       <c r="AG28" s="25" t="s">
         <v>30</v>
       </c>
@@ -4598,6 +4608,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="AF3:AF28"/>
+    <mergeCell ref="R24:R26"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="N18:N19"/>
     <mergeCell ref="S17:S18"/>
     <mergeCell ref="A3:A4"/>
@@ -4606,12 +4622,6 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="P19:Q19"/>
     <mergeCell ref="R19:S19"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="AF3:AF28"/>
-    <mergeCell ref="R24:R26"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AA1:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4708,10 +4718,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:T68"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="M65" sqref="M65"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="R65" sqref="R65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4735,18 +4745,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="331" t="s">
+      <c r="E1" s="324" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="333"/>
+      <c r="F1" s="326"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="331" t="s">
+      <c r="H1" s="324" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="332"/>
-      <c r="J1" s="333"/>
+      <c r="I1" s="325"/>
+      <c r="J1" s="326"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -4764,7 +4774,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="328">
+      <c r="B2" s="327">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -4791,15 +4801,15 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="323">
+      <c r="K2" s="342">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="342">
+      <c r="L2" s="340">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="334">
+      <c r="M2" s="330">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
@@ -4810,7 +4820,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="330"/>
+      <c r="B3" s="328"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -4825,9 +4835,9 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="324"/>
-      <c r="L3" s="308"/>
-      <c r="M3" s="335"/>
+      <c r="K3" s="343"/>
+      <c r="L3" s="294"/>
+      <c r="M3" s="331"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
@@ -4846,9 +4856,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="324"/>
-      <c r="L4" s="308"/>
-      <c r="M4" s="335"/>
+      <c r="K4" s="343"/>
+      <c r="L4" s="294"/>
+      <c r="M4" s="331"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -4930,7 +4940,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="320">
+      <c r="B7" s="332">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -4947,22 +4957,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="336">
+      <c r="K7" s="334">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="338">
+      <c r="L7" s="336">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="340">
+      <c r="M7" s="338">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="322"/>
+      <c r="B8" s="333"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -4983,9 +4993,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="337"/>
-      <c r="L8" s="339"/>
-      <c r="M8" s="341"/>
+      <c r="K8" s="335"/>
+      <c r="L8" s="337"/>
+      <c r="M8" s="339"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -5065,7 +5075,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="320">
+      <c r="B11" s="332">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -5092,7 +5102,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="322"/>
+      <c r="B12" s="333"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -5149,7 +5159,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="320">
+      <c r="B14" s="332">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -5172,7 +5182,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="322"/>
+      <c r="B15" s="333"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -5196,7 +5206,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="328">
+      <c r="B16" s="327">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -5227,7 +5237,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="330"/>
+      <c r="B17" s="328"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -5245,7 +5255,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="328">
+      <c r="B18" s="327">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -5334,7 +5344,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="326">
+      <c r="B21" s="344">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -5362,7 +5372,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="327"/>
+      <c r="B22" s="345"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -5414,7 +5424,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="311">
+      <c r="B24" s="297">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -5443,7 +5453,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="312"/>
+      <c r="B25" s="298"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -5471,7 +5481,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="311">
+      <c r="B26" s="297">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -5502,7 +5512,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="325"/>
+      <c r="B27" s="323"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -5533,7 +5543,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="311">
+      <c r="B28" s="297">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -5555,7 +5565,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="312"/>
+      <c r="B29" s="298"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -5581,7 +5591,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="311">
+      <c r="B30" s="297">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -5604,7 +5614,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="312"/>
+      <c r="B31" s="298"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -5631,7 +5641,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="311">
+      <c r="B32" s="297">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -5653,7 +5663,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="312"/>
+      <c r="B33" s="298"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -5706,7 +5716,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="311">
+      <c r="B35" s="297">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -5733,7 +5743,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="312"/>
+      <c r="B36" s="298"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -5755,7 +5765,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="311">
+      <c r="B37" s="297">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -5788,7 +5798,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="312"/>
+      <c r="B38" s="298"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -5806,7 +5816,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="311">
+      <c r="B39" s="297">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -5833,7 +5843,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="325"/>
+      <c r="B40" s="323"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -5861,7 +5871,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="311">
+      <c r="B41" s="297">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -5888,7 +5898,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="325"/>
+      <c r="B42" s="323"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -5906,7 +5916,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="312"/>
+      <c r="B43" s="298"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -5935,7 +5945,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="311">
+      <c r="B44" s="297">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -5961,7 +5971,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="312"/>
+      <c r="B45" s="298"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -5986,7 +5996,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="311">
+      <c r="B46" s="297">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -6008,7 +6018,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="325"/>
+      <c r="B47" s="323"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -6029,7 +6039,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="311">
+      <c r="B48" s="297">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -6049,7 +6059,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="325"/>
+      <c r="B49" s="323"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -6075,7 +6085,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="325"/>
+      <c r="B50" s="323"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -6102,7 +6112,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="311">
+      <c r="B51" s="297">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -6124,7 +6134,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="312"/>
+      <c r="B52" s="298"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -6157,7 +6167,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="311">
+      <c r="B53" s="297">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -6187,7 +6197,7 @@
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="325"/>
+      <c r="B54" s="323"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -6214,7 +6224,7 @@
       <c r="A55" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="311">
+      <c r="B55" s="297">
         <v>31</v>
       </c>
       <c r="C55" s="96"/>
@@ -6242,7 +6252,7 @@
       <c r="M55" s="82"/>
     </row>
     <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="312"/>
+      <c r="B56" s="298"/>
       <c r="C56" s="96"/>
       <c r="D56" s="82"/>
       <c r="E56" s="82">
@@ -6268,7 +6278,7 @@
       <c r="M56" s="82"/>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="343">
+      <c r="B57" s="320">
         <v>1</v>
       </c>
       <c r="C57" s="142"/>
@@ -6288,7 +6298,7 @@
       <c r="M57" s="18"/>
     </row>
     <row r="58" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="344"/>
+      <c r="B58" s="321"/>
       <c r="C58" s="142"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18">
@@ -6317,7 +6327,7 @@
       <c r="A59" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="345"/>
+      <c r="B59" s="322"/>
       <c r="C59" s="142"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18">
@@ -6343,7 +6353,7 @@
       <c r="M59" s="18"/>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="311">
+      <c r="B60" s="297">
         <v>2</v>
       </c>
       <c r="C60" s="142"/>
@@ -6369,7 +6379,7 @@
       <c r="M60" s="18"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="325"/>
+      <c r="B61" s="323"/>
       <c r="C61" s="142"/>
       <c r="D61" s="18">
         <v>240</v>
@@ -6395,7 +6405,7 @@
       <c r="M61" s="18"/>
     </row>
     <row r="62" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="312"/>
+      <c r="B62" s="298"/>
       <c r="C62" s="142"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
@@ -6416,7 +6426,7 @@
       <c r="A63" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="320">
+      <c r="B63" s="332">
         <v>3</v>
       </c>
       <c r="C63" s="142"/>
@@ -6438,7 +6448,7 @@
       <c r="M63" s="18"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="321"/>
+      <c r="B64" s="341"/>
       <c r="C64" s="142"/>
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
@@ -6458,7 +6468,7 @@
       <c r="M64" s="18"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="321"/>
+      <c r="B65" s="341"/>
       <c r="C65" s="142"/>
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
@@ -6480,7 +6490,7 @@
       <c r="M65" s="18"/>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="321"/>
+      <c r="B66" s="341"/>
       <c r="C66" s="142"/>
       <c r="D66" s="18">
         <v>500</v>
@@ -6508,7 +6518,7 @@
       <c r="M66" s="18"/>
     </row>
     <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="322"/>
+      <c r="B67" s="333"/>
       <c r="C67" s="142"/>
       <c r="D67" s="18"/>
       <c r="E67" s="18"/>
@@ -6524,10 +6534,10 @@
       <c r="M67" s="18"/>
     </row>
     <row r="68" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="130">
+      <c r="B68" s="34">
         <v>4</v>
       </c>
-      <c r="C68" s="18"/>
+      <c r="C68" s="142"/>
       <c r="D68" s="18"/>
       <c r="E68" s="18">
         <v>20</v>
@@ -6551,25 +6561,28 @@
       <c r="L68" s="18"/>
       <c r="M68" s="18"/>
     </row>
+    <row r="69" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="130">
+        <v>5</v>
+      </c>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="364">
+        <v>30</v>
+      </c>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="364">
+        <v>30</v>
+      </c>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
+      <c r="M69" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L2:L4"/>
     <mergeCell ref="B63:B67"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="B32:B33"/>
@@ -6586,6 +6599,23 @@
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="B60:B62"/>
     <mergeCell ref="B35:B36"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B46:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6593,10 +6623,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EF39B9-450C-4C51-9807-7AFD5CC29C14}">
-  <dimension ref="A1:DN88"/>
+  <dimension ref="A1:DN108"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="U76" sqref="U76"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90:S108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8146,7 +8176,7 @@
       </c>
       <c r="AC14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45295</v>
+        <v>45296</v>
       </c>
       <c r="AG14" s="99" t="s">
         <v>44</v>
@@ -8191,7 +8221,7 @@
       <c r="AU14" s="43"/>
       <c r="AV14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45295</v>
+        <v>45296</v>
       </c>
       <c r="AZ14" s="99" t="s">
         <v>44</v>
@@ -8236,7 +8266,7 @@
       <c r="BN14" s="43"/>
       <c r="BO14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45295</v>
+        <v>45296</v>
       </c>
       <c r="BR14" s="158" t="s">
         <v>44</v>
@@ -8281,7 +8311,7 @@
       <c r="CF14" s="43"/>
       <c r="CG14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45295</v>
+        <v>45296</v>
       </c>
     </row>
     <row r="15" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9792,10 +9822,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="313" t="s">
+      <c r="AG24" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="314"/>
+      <c r="AH24" s="300"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -9815,10 +9845,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="313" t="s">
+      <c r="AZ24" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="314"/>
+      <c r="BA24" s="300"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -9838,10 +9868,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="313" t="s">
+      <c r="BR24" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="314"/>
+      <c r="BS24" s="300"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -9864,10 +9894,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="315" t="s">
+      <c r="B26" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="317"/>
+      <c r="C26" s="303"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9904,10 +9934,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="315" t="s">
+      <c r="R26" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="317"/>
+      <c r="S26" s="303"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9944,10 +9974,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="315" t="s">
+      <c r="AG26" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="317"/>
+      <c r="AH26" s="303"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9984,10 +10014,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="315" t="s">
+      <c r="AW26" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="317"/>
+      <c r="AX26" s="303"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -10024,10 +10054,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="315" t="s">
+      <c r="BM26" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="317"/>
+      <c r="BN26" s="303"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -11021,7 +11051,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="358">
+      <c r="AX32" s="353">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -11059,7 +11089,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="358">
+      <c r="BN32" s="353">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -11208,7 +11238,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="359"/>
+      <c r="AX33" s="354"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -11244,7 +11274,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="359"/>
+      <c r="BN33" s="354"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -11395,7 +11425,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="360"/>
+      <c r="AX34" s="355"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11433,7 +11463,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="360"/>
+      <c r="BN34" s="355"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -11664,10 +11694,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="313" t="s">
+      <c r="B36" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="314"/>
+      <c r="C36" s="300"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -11685,10 +11715,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="313" t="s">
+      <c r="R36" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="314"/>
+      <c r="S36" s="300"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -11706,10 +11736,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="313" t="s">
+      <c r="AG36" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="314"/>
+      <c r="AH36" s="300"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -11727,10 +11757,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="313" t="s">
+      <c r="AW36" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="314"/>
+      <c r="AX36" s="300"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -11748,10 +11778,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="313" t="s">
+      <c r="BM36" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="314"/>
+      <c r="BN36" s="300"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -11771,10 +11801,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="315" t="s">
+      <c r="B38" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="317"/>
+      <c r="C38" s="303"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11814,10 +11844,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="315" t="s">
+      <c r="S38" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="317"/>
+      <c r="T38" s="303"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11857,11 +11887,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="315" t="s">
+      <c r="AJ38" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="316"/>
-      <c r="AL38" s="317"/>
+      <c r="AK38" s="302"/>
+      <c r="AL38" s="303"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11904,13 +11934,13 @@
       <c r="AZ38" s="44"/>
       <c r="BA38" s="199">
         <f ca="1">TODAY()</f>
-        <v>45295</v>
-      </c>
-      <c r="BD38" s="315" t="s">
+        <v>45296</v>
+      </c>
+      <c r="BD38" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="316"/>
-      <c r="BF38" s="317"/>
+      <c r="BE38" s="302"/>
+      <c r="BF38" s="303"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11950,11 +11980,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="315" t="s">
+      <c r="BW38" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="316"/>
-      <c r="BY38" s="317"/>
+      <c r="BX38" s="302"/>
+      <c r="BY38" s="303"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -12906,7 +12936,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="358">
+      <c r="C44" s="353">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -12944,10 +12974,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="351">
+      <c r="S44" s="362">
         <v>25</v>
       </c>
-      <c r="T44" s="358">
+      <c r="T44" s="353">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -12956,7 +12986,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="353" t="s">
+      <c r="W44" s="356" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -12985,10 +13015,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="351">
+      <c r="AJ44" s="362">
         <v>50</v>
       </c>
-      <c r="AK44" s="358">
+      <c r="AK44" s="353">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -12998,7 +13028,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="353" t="s">
+      <c r="AO44" s="356" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -13028,7 +13058,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="351">
+      <c r="BD44" s="362">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -13039,7 +13069,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="353" t="s">
+      <c r="BI44" s="356" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -13068,7 +13098,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="351">
+      <c r="BW44" s="362">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -13079,7 +13109,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="353" t="s">
+      <c r="CB44" s="356" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -13111,7 +13141,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="359"/>
+      <c r="C45" s="354"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -13145,15 +13175,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="352"/>
-      <c r="T45" s="360"/>
+      <c r="S45" s="363"/>
+      <c r="T45" s="355"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="354"/>
+      <c r="W45" s="357"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13180,8 +13210,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="352"/>
-      <c r="AK45" s="360"/>
+      <c r="AJ45" s="363"/>
+      <c r="AK45" s="355"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -13189,7 +13219,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="354"/>
+      <c r="AO45" s="357"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13217,7 +13247,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="352"/>
+      <c r="BD45" s="363"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -13228,7 +13258,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="354"/>
+      <c r="BI45" s="357"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13255,7 +13285,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="352"/>
+      <c r="BW45" s="363"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -13264,7 +13294,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="354"/>
+      <c r="CB45" s="357"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -13294,7 +13324,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="360"/>
+      <c r="C46" s="355"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -13721,10 +13751,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="313" t="s">
+      <c r="B48" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="314"/>
+      <c r="C48" s="300"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -13743,10 +13773,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="313" t="s">
+      <c r="S48" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="314"/>
+      <c r="T48" s="300"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -13899,11 +13929,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="355"/>
+      <c r="AQ49" s="358"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="346"/>
-      <c r="AV49" s="347"/>
+      <c r="AU49" s="350"/>
+      <c r="AV49" s="351"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -13915,11 +13945,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="355"/>
+      <c r="BK49" s="358"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="346"/>
-      <c r="BP49" s="347"/>
+      <c r="BO49" s="350"/>
+      <c r="BP49" s="351"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -13930,20 +13960,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="355"/>
+      <c r="CD49" s="358"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="346"/>
-      <c r="CI49" s="347"/>
+      <c r="CH49" s="350"/>
+      <c r="CI49" s="351"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="313" t="s">
+      <c r="AJ50" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="314"/>
+      <c r="AK50" s="300"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -13954,19 +13984,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="355"/>
+      <c r="AQ50" s="358"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="346"/>
-      <c r="AV50" s="347"/>
+      <c r="AU50" s="350"/>
+      <c r="AV50" s="351"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="313" t="s">
+      <c r="BD50" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="314"/>
+      <c r="BE50" s="300"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -13975,18 +14005,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="355"/>
+      <c r="BK50" s="358"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="346"/>
-      <c r="BP50" s="347"/>
+      <c r="BO50" s="350"/>
+      <c r="BP50" s="351"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="313" t="s">
+      <c r="BW50" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="314"/>
+      <c r="BX50" s="300"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -13995,21 +14025,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="355"/>
+      <c r="CD50" s="358"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="346"/>
-      <c r="CI50" s="347"/>
+      <c r="CH50" s="350"/>
+      <c r="CI50" s="351"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:117" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="315" t="s">
+      <c r="B51" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="316"/>
-      <c r="D51" s="317"/>
+      <c r="C51" s="302"/>
+      <c r="D51" s="303"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -14059,14 +14089,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="356"/>
+      <c r="AQ51" s="359"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="357"/>
-      <c r="AV51" s="350"/>
+      <c r="AU51" s="360"/>
+      <c r="AV51" s="361"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -14078,14 +14108,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="356"/>
+      <c r="BK51" s="359"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="357"/>
-      <c r="BP51" s="350"/>
+      <c r="BO51" s="360"/>
+      <c r="BP51" s="361"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -14096,14 +14126,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="356"/>
+      <c r="CD51" s="359"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="357"/>
-      <c r="CI51" s="350"/>
+      <c r="CH51" s="360"/>
+      <c r="CI51" s="361"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -14124,11 +14154,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="315" t="s">
+      <c r="V52" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="316"/>
-      <c r="X52" s="317"/>
+      <c r="W52" s="302"/>
+      <c r="X52" s="303"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -14230,11 +14260,11 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="46"/>
-      <c r="AO53" s="315" t="s">
+      <c r="AO53" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="AP53" s="316"/>
-      <c r="AQ53" s="317"/>
+      <c r="AP53" s="302"/>
+      <c r="AQ53" s="303"/>
       <c r="AR53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14279,13 +14309,13 @@
       </c>
       <c r="BG53" s="98">
         <f ca="1">TODAY()</f>
-        <v>45295</v>
-      </c>
-      <c r="BJ53" s="315" t="s">
+        <v>45296</v>
+      </c>
+      <c r="BJ53" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="BK53" s="316"/>
-      <c r="BL53" s="317"/>
+      <c r="BK53" s="302"/>
+      <c r="BL53" s="303"/>
       <c r="BM53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14328,11 +14358,11 @@
       <c r="BZ53" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="CC53" s="315" t="s">
+      <c r="CC53" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="CD53" s="316"/>
-      <c r="CE53" s="317"/>
+      <c r="CD53" s="302"/>
+      <c r="CE53" s="303"/>
       <c r="CF53" s="26" t="s">
         <v>43</v>
       </c>
@@ -14376,11 +14406,11 @@
         <v>108</v>
       </c>
       <c r="CV53" s="42"/>
-      <c r="CW53" s="315" t="s">
+      <c r="CW53" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="CX53" s="316"/>
-      <c r="CY53" s="317"/>
+      <c r="CX53" s="302"/>
+      <c r="CY53" s="303"/>
       <c r="CZ53" s="26" t="s">
         <v>43</v>
       </c>
@@ -17467,10 +17497,10 @@
       </c>
     </row>
     <row r="66" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="313" t="s">
+      <c r="B66" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="314"/>
+      <c r="C66" s="300"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -17483,8 +17513,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="346"/>
-      <c r="O66" s="347"/>
+      <c r="N66" s="350"/>
+      <c r="O66" s="351"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -17624,18 +17654,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="348"/>
+      <c r="J67" s="349"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="346"/>
-      <c r="O67" s="347"/>
+      <c r="N67" s="350"/>
+      <c r="O67" s="351"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="313" t="s">
+      <c r="V67" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="314"/>
+      <c r="W67" s="300"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -17647,8 +17677,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="346"/>
-      <c r="AI67" s="347"/>
+      <c r="AH67" s="350"/>
+      <c r="AI67" s="351"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -17719,7 +17749,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="349"/>
+      <c r="J68" s="352"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -17735,17 +17765,17 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="348"/>
+      <c r="AD68" s="349"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="346"/>
-      <c r="AI68" s="347"/>
+      <c r="AH68" s="350"/>
+      <c r="AI68" s="351"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
-      <c r="AO68" s="313" t="s">
+      <c r="AO68" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="AP68" s="314"/>
+      <c r="AP68" s="300"/>
       <c r="AQ68" s="189"/>
       <c r="AR68" s="9">
         <f>SUM(AO55:AQ66)</f>
@@ -17757,15 +17787,15 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="346"/>
-      <c r="BB68" s="347"/>
+      <c r="BA68" s="350"/>
+      <c r="BB68" s="351"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
-      <c r="BJ68" s="313" t="s">
+      <c r="BJ68" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="BK68" s="314"/>
+      <c r="BK68" s="300"/>
       <c r="BL68" s="189"/>
       <c r="BM68" s="9">
         <f>SUM(BJ55:BL66)</f>
@@ -17777,15 +17807,15 @@
       <c r="BQ68" s="119"/>
       <c r="BR68" s="117"/>
       <c r="BU68" s="2"/>
-      <c r="BV68" s="346"/>
-      <c r="BW68" s="347"/>
+      <c r="BV68" s="350"/>
+      <c r="BW68" s="351"/>
       <c r="BX68" s="1"/>
       <c r="BY68" s="1"/>
       <c r="BZ68" s="46"/>
-      <c r="CC68" s="313" t="s">
+      <c r="CC68" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="CD68" s="314"/>
+      <c r="CD68" s="300"/>
       <c r="CE68" s="189"/>
       <c r="CF68" s="9">
         <f>SUM(CC55:CE66)</f>
@@ -17797,16 +17827,16 @@
       <c r="CJ68" s="119"/>
       <c r="CK68" s="117"/>
       <c r="CN68" s="2"/>
-      <c r="CO68" s="346"/>
-      <c r="CP68" s="347"/>
+      <c r="CO68" s="350"/>
+      <c r="CP68" s="351"/>
       <c r="CQ68" s="1"/>
       <c r="CR68" s="1"/>
       <c r="CS68" s="46"/>
       <c r="CV68" s="110"/>
-      <c r="CW68" s="313" t="s">
+      <c r="CW68" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="CX68" s="314"/>
+      <c r="CX68" s="300"/>
       <c r="CY68" s="189"/>
       <c r="CZ68" s="9">
         <f>SUM(CW55:CY66)</f>
@@ -17825,7 +17855,7 @@
       <c r="DI68" s="159" t="s">
         <v>271</v>
       </c>
-      <c r="DJ68" s="308"/>
+      <c r="DJ68" s="294"/>
       <c r="DK68" s="265" t="s">
         <v>284</v>
       </c>
@@ -17844,7 +17874,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="349"/>
+      <c r="AD69" s="352"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -17860,10 +17890,10 @@
       <c r="AT69" s="119"/>
       <c r="AU69" s="192"/>
       <c r="AV69" s="119"/>
-      <c r="AW69" s="348"/>
+      <c r="AW69" s="349"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="346"/>
-      <c r="BB69" s="347"/>
+      <c r="BA69" s="350"/>
+      <c r="BB69" s="351"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
@@ -17874,10 +17904,10 @@
       <c r="BO69" s="119"/>
       <c r="BP69" s="192"/>
       <c r="BQ69" s="119"/>
-      <c r="BR69" s="348"/>
+      <c r="BR69" s="349"/>
       <c r="BU69" s="2"/>
-      <c r="BV69" s="346"/>
-      <c r="BW69" s="347"/>
+      <c r="BV69" s="350"/>
+      <c r="BW69" s="351"/>
       <c r="BX69" s="1"/>
       <c r="BY69" s="1"/>
       <c r="BZ69" s="46"/>
@@ -17888,10 +17918,10 @@
       <c r="CH69" s="119"/>
       <c r="CI69" s="192"/>
       <c r="CJ69" s="119"/>
-      <c r="CK69" s="348"/>
+      <c r="CK69" s="349"/>
       <c r="CN69" s="2"/>
-      <c r="CO69" s="346"/>
-      <c r="CP69" s="347"/>
+      <c r="CO69" s="350"/>
+      <c r="CP69" s="351"/>
       <c r="CQ69" s="1"/>
       <c r="CR69" s="1"/>
       <c r="CS69" s="46"/>
@@ -17903,14 +17933,14 @@
       <c r="DB69" s="262"/>
       <c r="DC69" s="169"/>
       <c r="DD69" s="169"/>
-      <c r="DE69" s="348"/>
+      <c r="DE69" s="349"/>
       <c r="DF69" s="159" t="s">
         <v>280</v>
       </c>
       <c r="DG69" s="18"/>
       <c r="DH69" s="264"/>
       <c r="DI69" s="159"/>
-      <c r="DJ69" s="308"/>
+      <c r="DJ69" s="294"/>
       <c r="DK69" s="17"/>
       <c r="DL69" s="1"/>
       <c r="DM69" s="46"/>
@@ -17923,7 +17953,7 @@
       <c r="AT70" s="117"/>
       <c r="AU70" s="192"/>
       <c r="AV70" s="119"/>
-      <c r="AW70" s="348"/>
+      <c r="AW70" s="349"/>
       <c r="AZ70" s="2"/>
       <c r="BA70" s="152"/>
       <c r="BB70" s="1"/>
@@ -17937,7 +17967,7 @@
       <c r="BO70" s="117"/>
       <c r="BP70" s="192"/>
       <c r="BQ70" s="119"/>
-      <c r="BR70" s="348"/>
+      <c r="BR70" s="349"/>
       <c r="BU70" s="2"/>
       <c r="BV70" s="152"/>
       <c r="BW70" s="1"/>
@@ -17952,7 +17982,7 @@
       <c r="CH70" s="137"/>
       <c r="CI70" s="203"/>
       <c r="CJ70" s="201"/>
-      <c r="CK70" s="349"/>
+      <c r="CK70" s="352"/>
       <c r="CL70" s="50"/>
       <c r="CM70" s="50"/>
       <c r="CN70" s="79"/>
@@ -17969,28 +17999,28 @@
       <c r="DB70" s="117"/>
       <c r="DC70" s="194"/>
       <c r="DD70" s="119"/>
-      <c r="DE70" s="348"/>
+      <c r="DE70" s="349"/>
       <c r="DF70" s="159" t="s">
         <v>275</v>
       </c>
-      <c r="DG70" s="292" t="s">
+      <c r="DG70" s="306" t="s">
         <v>290</v>
       </c>
-      <c r="DH70" s="292"/>
-      <c r="DI70" s="319" t="s">
+      <c r="DH70" s="306"/>
+      <c r="DI70" s="305" t="s">
         <v>277</v>
       </c>
-      <c r="DJ70" s="319"/>
+      <c r="DJ70" s="305"/>
       <c r="DK70" s="17"/>
       <c r="DL70" s="1"/>
       <c r="DM70" s="46"/>
     </row>
     <row r="71" spans="2:118" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="315" t="s">
+      <c r="B71" s="301" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="316"/>
-      <c r="D71" s="317"/>
+      <c r="C71" s="302"/>
+      <c r="D71" s="303"/>
       <c r="E71" s="281"/>
       <c r="F71" s="26" t="s">
         <v>43</v>
@@ -18123,10 +18153,10 @@
       <c r="DD72" s="137"/>
       <c r="DE72" s="137"/>
       <c r="DF72" s="5"/>
-      <c r="DG72" s="361" t="s">
+      <c r="DG72" s="348" t="s">
         <v>291</v>
       </c>
-      <c r="DH72" s="361"/>
+      <c r="DH72" s="348"/>
       <c r="DI72" s="268"/>
       <c r="DJ72" s="269"/>
       <c r="DK72" s="270" t="s">
@@ -18767,7 +18797,7 @@
       <c r="O86" s="272" t="s">
         <v>271</v>
       </c>
-      <c r="P86" s="308"/>
+      <c r="P86" s="294"/>
       <c r="Q86" s="265" t="s">
         <v>284</v>
       </c>
@@ -18775,10 +18805,10 @@
       <c r="S86" s="46"/>
     </row>
     <row r="87" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="313" t="s">
+      <c r="B87" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="314"/>
+      <c r="C87" s="300"/>
       <c r="D87" s="20"/>
       <c r="E87" s="20"/>
       <c r="G87" s="226"/>
@@ -18787,16 +18817,16 @@
         <v>269</v>
       </c>
       <c r="J87" s="278"/>
-      <c r="K87" s="306" t="s">
+      <c r="K87" s="292" t="s">
         <v>313</v>
       </c>
-      <c r="L87" s="299" t="s">
+      <c r="L87" s="313" t="s">
         <v>305</v>
       </c>
-      <c r="M87" s="299"/>
-      <c r="N87" s="300"/>
+      <c r="M87" s="313"/>
+      <c r="N87" s="314"/>
       <c r="O87" s="161"/>
-      <c r="P87" s="308"/>
+      <c r="P87" s="294"/>
       <c r="Q87" s="17"/>
       <c r="R87" s="1"/>
       <c r="S87" s="46"/>
@@ -18819,59 +18849,805 @@
         <v>288</v>
       </c>
       <c r="J88" s="201"/>
-      <c r="K88" s="307"/>
+      <c r="K88" s="293"/>
       <c r="L88" s="290" t="s">
         <v>311</v>
       </c>
-      <c r="M88" s="362" t="s">
+      <c r="M88" s="346" t="s">
         <v>290</v>
       </c>
-      <c r="N88" s="362"/>
-      <c r="O88" s="363" t="s">
+      <c r="N88" s="346"/>
+      <c r="O88" s="347" t="s">
         <v>277</v>
       </c>
-      <c r="P88" s="363"/>
+      <c r="P88" s="347"/>
       <c r="Q88" s="269"/>
       <c r="R88" s="65"/>
       <c r="S88" s="168"/>
     </row>
+    <row r="89" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="301" t="s">
+        <v>145</v>
+      </c>
+      <c r="C90" s="302"/>
+      <c r="D90" s="303"/>
+      <c r="E90" s="281"/>
+      <c r="F90" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G90" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="H90" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="I90" s="214" t="s">
+        <v>195</v>
+      </c>
+      <c r="J90" s="83" t="s">
+        <v>153</v>
+      </c>
+      <c r="K90" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="L90" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M90" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="N90" s="171" t="s">
+        <v>92</v>
+      </c>
+      <c r="O90" s="153" t="s">
+        <v>267</v>
+      </c>
+      <c r="P90" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q90" s="156" t="s">
+        <v>268</v>
+      </c>
+      <c r="R90" s="214" t="s">
+        <v>224</v>
+      </c>
+      <c r="S90" s="36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="G91" s="25"/>
+      <c r="H91" s="117"/>
+      <c r="I91" s="192"/>
+      <c r="J91" s="117"/>
+      <c r="K91" s="117"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="152"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+      <c r="S91" s="24"/>
+    </row>
+    <row r="92" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="244">
+        <v>10</v>
+      </c>
+      <c r="C92" s="205"/>
+      <c r="D92" s="283">
+        <v>10</v>
+      </c>
+      <c r="E92" s="283"/>
+      <c r="F92" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G92" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H92" s="213" t="s">
+        <v>187</v>
+      </c>
+      <c r="I92" s="169" t="s">
+        <v>318</v>
+      </c>
+      <c r="J92" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="K92" s="224" t="s">
+        <v>156</v>
+      </c>
+      <c r="L92" s="143" t="s">
+        <v>193</v>
+      </c>
+      <c r="M92" s="169" t="s">
+        <v>156</v>
+      </c>
+      <c r="N92" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O92" s="154">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="P92" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q92" s="154">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="R92" s="1"/>
+      <c r="S92" s="245">
+        <v>45296</v>
+      </c>
+    </row>
+    <row r="93" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="218">
+        <v>10</v>
+      </c>
+      <c r="C93" s="206"/>
+      <c r="D93" s="127"/>
+      <c r="E93" s="127"/>
+      <c r="F93" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G93" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="I93" s="169"/>
+      <c r="J93" s="167" t="s">
+        <v>142</v>
+      </c>
+      <c r="K93" s="224" t="s">
+        <v>85</v>
+      </c>
+      <c r="L93" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="M93" s="237" t="s">
+        <v>137</v>
+      </c>
+      <c r="N93" s="197" t="s">
+        <v>86</v>
+      </c>
+      <c r="O93" s="154">
+        <v>0.75</v>
+      </c>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="154">
+        <v>0.75</v>
+      </c>
+      <c r="R93" s="1"/>
+      <c r="S93" s="245">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="94" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="218">
+        <v>20</v>
+      </c>
+      <c r="C94" s="207"/>
+      <c r="D94" s="127"/>
+      <c r="E94" s="127"/>
+      <c r="F94" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G94" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="I94" s="169"/>
+      <c r="J94" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="K94" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="L94" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="M94" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="N94" s="176" t="s">
+        <v>69</v>
+      </c>
+      <c r="O94" s="154">
+        <v>0.75</v>
+      </c>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="154">
+        <v>0.75</v>
+      </c>
+      <c r="R94" s="1"/>
+      <c r="S94" s="245">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="95" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="165"/>
+      <c r="C95" s="242"/>
+      <c r="D95" s="177">
+        <v>50</v>
+      </c>
+      <c r="E95" s="177"/>
+      <c r="F95" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G95" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="I95" s="169" t="s">
+        <v>288</v>
+      </c>
+      <c r="J95" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="K95" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="L95" s="143" t="s">
+        <v>192</v>
+      </c>
+      <c r="M95" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N95" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="O95" s="154">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="154">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="R95" s="1"/>
+      <c r="S95" s="245">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="96" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="219"/>
+      <c r="C96" s="242"/>
+      <c r="D96" s="282"/>
+      <c r="E96" s="282"/>
+      <c r="F96" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G96" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H96" s="213"/>
+      <c r="I96" s="274" t="s">
+        <v>300</v>
+      </c>
+      <c r="J96" s="83" t="s">
+        <v>214</v>
+      </c>
+      <c r="K96" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="L96" s="187" t="s">
+        <v>196</v>
+      </c>
+      <c r="M96" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="N96" s="188" t="s">
+        <v>65</v>
+      </c>
+      <c r="O96" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="R96" s="273">
+        <v>1</v>
+      </c>
+      <c r="S96" s="245">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="97" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="163"/>
+      <c r="C97" s="165">
+        <v>14</v>
+      </c>
+      <c r="D97" s="282"/>
+      <c r="E97" s="282"/>
+      <c r="F97" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G97" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="H97" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="I97" s="169"/>
+      <c r="J97" s="223" t="s">
+        <v>163</v>
+      </c>
+      <c r="K97" s="224" t="s">
+        <v>170</v>
+      </c>
+      <c r="L97" s="143" t="s">
+        <v>191</v>
+      </c>
+      <c r="M97" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N97" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O97" s="154">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="154">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="R97" s="1"/>
+      <c r="S97" s="245">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="98" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="220">
+        <v>10</v>
+      </c>
+      <c r="C98" s="206"/>
+      <c r="D98" s="177"/>
+      <c r="E98" s="177"/>
+      <c r="F98" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G98" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H98" s="213" t="s">
+        <v>294</v>
+      </c>
+      <c r="I98" s="169" t="s">
+        <v>316</v>
+      </c>
+      <c r="J98" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="K98" s="225" t="s">
+        <v>62</v>
+      </c>
+      <c r="L98" s="144" t="s">
+        <v>122</v>
+      </c>
+      <c r="M98" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="N98" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="O98" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="P98" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q98" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="R98" s="1"/>
+      <c r="S98" s="245">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="99" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="221"/>
+      <c r="C99" s="242">
+        <v>5</v>
+      </c>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G99" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H99" s="213" t="s">
+        <v>116</v>
+      </c>
+      <c r="I99" s="169" t="s">
+        <v>289</v>
+      </c>
+      <c r="J99" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="K99" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="L99" s="186" t="s">
+        <v>110</v>
+      </c>
+      <c r="M99" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="N99" s="198" t="s">
+        <v>161</v>
+      </c>
+      <c r="O99" s="154">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="154">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="R99" s="1"/>
+      <c r="S99" s="245">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="100" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="165">
+        <v>120</v>
+      </c>
+      <c r="C100" s="205"/>
+      <c r="D100" s="164"/>
+      <c r="E100" s="164"/>
+      <c r="F100" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="G100" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H100" s="213"/>
+      <c r="I100" s="169" t="s">
+        <v>222</v>
+      </c>
+      <c r="J100" s="224" t="s">
+        <v>123</v>
+      </c>
+      <c r="K100" s="225" t="s">
+        <v>62</v>
+      </c>
+      <c r="L100" s="143" t="s">
+        <v>197</v>
+      </c>
+      <c r="M100" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N100" s="188" t="s">
+        <v>181</v>
+      </c>
+      <c r="O100" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="P100" s="24"/>
+      <c r="Q100" s="154">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="R100" s="1"/>
+      <c r="S100" s="245">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="101" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="36"/>
+      <c r="C101" s="206"/>
+      <c r="D101" s="246">
+        <v>10</v>
+      </c>
+      <c r="E101" s="246"/>
+      <c r="F101" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G101" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H101" s="228" t="s">
+        <v>313</v>
+      </c>
+      <c r="I101" s="194"/>
+      <c r="J101" s="183" t="s">
+        <v>155</v>
+      </c>
+      <c r="K101" s="183" t="s">
+        <v>85</v>
+      </c>
+      <c r="L101" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="M101" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="N101" s="229" t="s">
+        <v>90</v>
+      </c>
+      <c r="O101" s="154">
+        <v>0.53125</v>
+      </c>
+      <c r="Q101" s="154">
+        <v>0.53125</v>
+      </c>
+      <c r="R101" s="261">
+        <v>1</v>
+      </c>
+      <c r="S101" s="245">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="102" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="165">
+        <v>40</v>
+      </c>
+      <c r="C102" s="205">
+        <v>1</v>
+      </c>
+      <c r="D102" s="127"/>
+      <c r="E102" s="127"/>
+      <c r="F102" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G102" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H102" s="213"/>
+      <c r="I102" s="169" t="s">
+        <v>273</v>
+      </c>
+      <c r="J102" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="K102" s="224" t="s">
+        <v>62</v>
+      </c>
+      <c r="L102" s="143" t="s">
+        <v>200</v>
+      </c>
+      <c r="M102" s="169" t="s">
+        <v>47</v>
+      </c>
+      <c r="N102" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="O102" s="154">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="Q102" s="154">
+        <v>0.94097222222222221</v>
+      </c>
+      <c r="R102" s="1"/>
+      <c r="S102" s="245">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="103" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="165"/>
+      <c r="C103" s="34"/>
+      <c r="D103" s="177"/>
+      <c r="E103" s="177"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="H103" s="231"/>
+      <c r="I103" s="169"/>
+      <c r="J103" s="83"/>
+      <c r="K103" s="233"/>
+      <c r="L103" s="9"/>
+      <c r="M103" s="8"/>
+      <c r="N103" s="37"/>
+      <c r="O103" s="154">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="Q103" s="154">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="R103" s="1"/>
+      <c r="S103" s="245">
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="104" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="G104" s="234"/>
+      <c r="H104" s="119"/>
+      <c r="I104" s="216"/>
+      <c r="J104" s="119"/>
+      <c r="K104" s="117"/>
+      <c r="N104" s="2"/>
+      <c r="O104" s="152"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+      <c r="R104" s="1"/>
+      <c r="S104" s="24"/>
+    </row>
+    <row r="105" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="34">
+        <f>SUM(B92:B103)</f>
+        <v>210</v>
+      </c>
+      <c r="C105" s="34">
+        <f>SUM(C92:C103)</f>
+        <v>20</v>
+      </c>
+      <c r="D105" s="34">
+        <f>SUM(D92:D103)</f>
+        <v>70</v>
+      </c>
+      <c r="E105" s="189"/>
+      <c r="F105" s="9">
+        <f>SUM(B92:D103)</f>
+        <v>300</v>
+      </c>
+      <c r="G105" s="26"/>
+      <c r="H105" s="262"/>
+      <c r="I105" s="169" t="s">
+        <v>273</v>
+      </c>
+      <c r="J105" s="254"/>
+      <c r="K105" s="117"/>
+      <c r="L105" s="276" t="s">
+        <v>276</v>
+      </c>
+      <c r="M105" s="82"/>
+      <c r="N105" s="280" t="s">
+        <v>314</v>
+      </c>
+      <c r="O105" s="272" t="s">
+        <v>271</v>
+      </c>
+      <c r="P105" s="294"/>
+      <c r="Q105" s="265" t="s">
+        <v>284</v>
+      </c>
+      <c r="R105" s="1"/>
+      <c r="S105" s="24"/>
+    </row>
+    <row r="106" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="299" t="s">
+        <v>4</v>
+      </c>
+      <c r="C106" s="300"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="20"/>
+      <c r="G106" s="226"/>
+      <c r="H106" s="262"/>
+      <c r="I106" s="194" t="s">
+        <v>269</v>
+      </c>
+      <c r="J106" s="278"/>
+      <c r="K106" s="292" t="s">
+        <v>313</v>
+      </c>
+      <c r="L106" s="313" t="s">
+        <v>305</v>
+      </c>
+      <c r="M106" s="313"/>
+      <c r="N106" s="314"/>
+      <c r="O106" s="161"/>
+      <c r="P106" s="294"/>
+      <c r="Q106" s="17"/>
+      <c r="R106" s="1"/>
+      <c r="S106" s="24"/>
+    </row>
+    <row r="107" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="284"/>
+      <c r="C107" s="59"/>
+      <c r="D107" s="285"/>
+      <c r="E107" s="2">
+        <v>220</v>
+      </c>
+      <c r="F107" s="1">
+        <v>280</v>
+      </c>
+      <c r="G107" s="226"/>
+      <c r="H107" s="117"/>
+      <c r="I107" s="169" t="s">
+        <v>288</v>
+      </c>
+      <c r="J107" s="119"/>
+      <c r="K107" s="293"/>
+      <c r="L107" s="279" t="s">
+        <v>311</v>
+      </c>
+      <c r="M107" s="304" t="s">
+        <v>290</v>
+      </c>
+      <c r="N107" s="304"/>
+      <c r="O107" s="305" t="s">
+        <v>277</v>
+      </c>
+      <c r="P107" s="305"/>
+      <c r="Q107" s="17"/>
+      <c r="R107" s="1"/>
+      <c r="S107" s="24"/>
+    </row>
+    <row r="108" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="236"/>
+      <c r="C108" s="65"/>
+      <c r="D108" s="286"/>
+      <c r="E108" s="2"/>
+      <c r="G108" s="227"/>
+      <c r="H108" s="117"/>
+      <c r="I108" s="169"/>
+      <c r="J108" s="119"/>
+      <c r="K108" s="231" t="s">
+        <v>313</v>
+      </c>
+      <c r="L108" s="277" t="s">
+        <v>309</v>
+      </c>
+      <c r="M108" s="18"/>
+      <c r="N108" s="264"/>
+      <c r="O108" s="159" t="s">
+        <v>279</v>
+      </c>
+      <c r="P108" s="17"/>
+      <c r="Q108" s="265" t="s">
+        <v>285</v>
+      </c>
+      <c r="R108" s="1"/>
+      <c r="S108" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="P86:P87"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="K87:K88"/>
-    <mergeCell ref="L87:N87"/>
-    <mergeCell ref="M88:N88"/>
-    <mergeCell ref="O88:P88"/>
-    <mergeCell ref="DG72:DH72"/>
-    <mergeCell ref="CW53:CY53"/>
-    <mergeCell ref="CW68:CX68"/>
-    <mergeCell ref="DJ68:DJ69"/>
-    <mergeCell ref="DE69:DE70"/>
-    <mergeCell ref="DG70:DH70"/>
-    <mergeCell ref="DI70:DJ70"/>
-    <mergeCell ref="CC53:CE53"/>
-    <mergeCell ref="CC68:CD68"/>
-    <mergeCell ref="CO68:CO69"/>
-    <mergeCell ref="CP68:CP69"/>
-    <mergeCell ref="CK69:CK70"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
+  <mergeCells count="91">
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="P105:P106"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="K106:K107"/>
+    <mergeCell ref="L106:N106"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="O107:P107"/>
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -18887,40 +19663,41 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
-    <mergeCell ref="BJ53:BL53"/>
-    <mergeCell ref="BJ68:BK68"/>
-    <mergeCell ref="BV68:BV69"/>
-    <mergeCell ref="BW68:BW69"/>
-    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="CC53:CE53"/>
+    <mergeCell ref="CC68:CD68"/>
+    <mergeCell ref="CO68:CO69"/>
+    <mergeCell ref="CP68:CP69"/>
+    <mergeCell ref="CK69:CK70"/>
+    <mergeCell ref="DG72:DH72"/>
+    <mergeCell ref="CW53:CY53"/>
+    <mergeCell ref="CW68:CX68"/>
+    <mergeCell ref="DJ68:DJ69"/>
+    <mergeCell ref="DE69:DE70"/>
+    <mergeCell ref="DG70:DH70"/>
+    <mergeCell ref="DI70:DJ70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="P86:P87"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="K87:K88"/>
+    <mergeCell ref="L87:N87"/>
+    <mergeCell ref="M88:N88"/>
+    <mergeCell ref="O88:P88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>